<commit_message>
Numeracao nas frases da coluna Resultado Esperado
</commit_message>
<xml_diff>
--- a/maps/contratarPacoteDados/exportedScenarios/scenarios.xlsx
+++ b/maps/contratarPacoteDados/exportedScenarios/scenarios.xlsx
@@ -77,12 +77,12 @@
 Quer algo mais.</t>
   </si>
   <si>
-    <t>Chamada é encaminhada para a URA Cognitiva;
-Ouvir a saudacão da URA Cognitiva conforme descrito na DF.
-A URA Congnitiva informa que entendeu que deseja falar sobre Contratação de Pacotes;
-A URA Cognitiva informa que o cliente já possui um pacote ativado
+    <t>1 - Chamada é encaminhada para a URA Cognitiva;
+2 - Ouvir a saudacão da URA Cognitiva conforme descrito na DF.
+3 - A URA Congnitiva informa que entendeu que deseja falar sobre Contratação de Pacotes;
+4 - A URA Cognitiva informa que o cliente já possui um pacote ativado
 e que precisa consumi-lo antes de contratar um novo pacote;
-A URA Cognitiva transfere para o desambiguador.</t>
+5 - A URA Cognitiva transfere para o desambiguador.</t>
   </si>
   <si>
     <t>2</t>
@@ -95,12 +95,12 @@
 Não quer mais nada.</t>
   </si>
   <si>
-    <t>Chamada é encaminhada para a URA Cognitiva;
-Ouvir a saudacão da URA Cognitiva conforme descrito na DF.
-A URA Congnitiva informa que entendeu que deseja falar sobre Contratação de Pacotes;
-A URA Cognitiva informa que o cliente já possui um pacote ativado
+    <t>1 - Chamada é encaminhada para a URA Cognitiva;
+2 - Ouvir a saudacão da URA Cognitiva conforme descrito na DF.
+3 - A URA Congnitiva informa que entendeu que deseja falar sobre Contratação de Pacotes;
+4 - A URA Cognitiva informa que o cliente já possui um pacote ativado
 e que precisa consumi-lo antes de contratar um novo pacote;
-A URA Cognitiva agradece e encerra a ligação.</t>
+5 - A URA Cognitiva agradece e encerra a ligação.</t>
   </si>
   <si>
     <t>3</t>
@@ -114,12 +114,12 @@
 Quer algo mais.</t>
   </si>
   <si>
-    <t>Chamada é encaminhada para a URA Cognitiva;
-Ouvir a saudacão da URA Cognitiva conforme descrito na DF.
-A URA Congnitiva informa que entendeu que deseja falar sobre Contratação de Pacotes;
-A URA Cognitiva informa que está com um bloqueio financeiro e por isso está impedido
+    <t>1 - Chamada é encaminhada para a URA Cognitiva;
+2 - Ouvir a saudacão da URA Cognitiva conforme descrito na DF.
+3 - A URA Congnitiva informa que entendeu que deseja falar sobre Contratação de Pacotes;
+4 - A URA Cognitiva informa que está com um bloqueio financeiro e por isso está impedido
 de contratar um novo pacote;
-A URA Cognitiva transfere para o desambiguador.</t>
+5 - A URA Cognitiva transfere para o desambiguador.</t>
   </si>
   <si>
     <t>4</t>
@@ -133,12 +133,12 @@
 Não quer mais nada.</t>
   </si>
   <si>
-    <t>Chamada é encaminhada para a URA Cognitiva;
-Ouvir a saudacão da URA Cognitiva conforme descrito na DF.
-A URA Congnitiva informa que entendeu que deseja falar sobre Contratação de Pacotes;
-A URA Cognitiva informa que está com um bloqueio financeiro e por isso está impedido
+    <t>1 - Chamada é encaminhada para a URA Cognitiva;
+2 - Ouvir a saudacão da URA Cognitiva conforme descrito na DF.
+3 - A URA Congnitiva informa que entendeu que deseja falar sobre Contratação de Pacotes;
+4 - A URA Cognitiva informa que está com um bloqueio financeiro e por isso está impedido
 de contratar um novo pacote;
-A URA Cognitiva agradece e encerra a ligação.</t>
+5 - A URA Cognitiva agradece e encerra a ligação.</t>
   </si>
   <si>
     <t>5</t>
@@ -155,13 +155,13 @@
 Quer algo mais.</t>
   </si>
   <si>
-    <t>Chamada é encaminhada para a URA Cognitiva;
-Ouvir a saudacão da URA Cognitiva conforme descrito na DF.
-A URA Congnitiva informa que entendeu que deseja falar sobre Contratação de Pacotes;
-A URA Cognitiva pede para aguardar enquanto verifica a internet;
-A URA Cognitiva informa o pacote de dados foi consumido e, por estar inadimplente,
+    <t>1 - Chamada é encaminhada para a URA Cognitiva;
+2 - Ouvir a saudacão da URA Cognitiva conforme descrito na DF.
+3 - A URA Congnitiva informa que entendeu que deseja falar sobre Contratação de Pacotes;
+4 - A URA Cognitiva pede para aguardar enquanto verifica a internet;
+5 - A URA Cognitiva informa o pacote de dados foi consumido e, por estar inadimplente,
 a velocidade está reduzida e não pode contratar um novo pacote;
-A URA Cognitiva transfere para o desambiguador.</t>
+6 - A URA Cognitiva transfere para o desambiguador.</t>
   </si>
   <si>
     <t>6</t>
@@ -178,13 +178,13 @@
 Não quer mais nada.</t>
   </si>
   <si>
-    <t>Chamada é encaminhada para a URA Cognitiva;
-Ouvir a saudacão da URA Cognitiva conforme descrito na DF.
-A URA Congnitiva informa que entendeu que deseja falar sobre Contratação de Pacotes;
-A URA Cognitiva pede para aguardar enquanto verifica a internet;
-A URA Cognitiva informa o pacote de dados foi consumido e, por estar inadimplente,
+    <t>1 - Chamada é encaminhada para a URA Cognitiva;
+2 - Ouvir a saudacão da URA Cognitiva conforme descrito na DF.
+3 - A URA Congnitiva informa que entendeu que deseja falar sobre Contratação de Pacotes;
+4 - A URA Cognitiva pede para aguardar enquanto verifica a internet;
+5 - A URA Cognitiva informa o pacote de dados foi consumido e, por estar inadimplente,
 a velocidade está reduzida e não pode contratar um novo pacote;
-A URA Cognitiva agradece e encerra a ligação.</t>
+6 - A URA Cognitiva agradece e encerra a ligação.</t>
   </si>
   <si>
     <t>7</t>
@@ -204,14 +204,14 @@
 Quer algo mais.</t>
   </si>
   <si>
-    <t>Chamada é encaminhada para a URA Cognitiva;
-Ouvir a saudacão da URA Cognitiva conforme descrito na DF.
-A URA Congnitiva informa que entendeu que deseja falar sobre Contratação de Pacotes;
-A URA Cognitiva pede para aguardar enquanto verifica a internet;
-A URA Cognitiva informa que está com velocidade reduzida porque já consumiu o pacote,
+    <t>1 - Chamada é encaminhada para a URA Cognitiva;
+2 - Ouvir a saudacão da URA Cognitiva conforme descrito na DF.
+3 - A URA Congnitiva informa que entendeu que deseja falar sobre Contratação de Pacotes;
+4 - A URA Cognitiva pede para aguardar enquanto verifica a internet;
+5 - A URA Cognitiva informa que está com velocidade reduzida porque já consumiu o pacote,
 mas pode contratar um pacote adicional e verifica se existem pacotes disponiveis;
-A URA Cognitiva informa que não existem pacotes disponiveis no momento;
-A URA Cognitiva transfere para o desambiguador.</t>
+6 - A URA Cognitiva informa que não existem pacotes disponiveis no momento;
+7 - A URA Cognitiva transfere para o desambiguador.</t>
   </si>
   <si>
     <t>8</t>
@@ -231,14 +231,14 @@
 Não quer mais nada.</t>
   </si>
   <si>
-    <t>Chamada é encaminhada para a URA Cognitiva;
-Ouvir a saudacão da URA Cognitiva conforme descrito na DF.
-A URA Congnitiva informa que entendeu que deseja falar sobre Contratação de Pacotes;
-A URA Cognitiva pede para aguardar enquanto verifica a internet;
-A URA Cognitiva informa que está com velocidade reduzida porque já consumiu o pacote,
+    <t>1 - Chamada é encaminhada para a URA Cognitiva;
+2 - Ouvir a saudacão da URA Cognitiva conforme descrito na DF.
+3 - A URA Congnitiva informa que entendeu que deseja falar sobre Contratação de Pacotes;
+4 - A URA Cognitiva pede para aguardar enquanto verifica a internet;
+5 - A URA Cognitiva informa que está com velocidade reduzida porque já consumiu o pacote,
 mas pode contratar um pacote adicional e verifica se existem pacotes disponiveis;
-A URA Cognitiva informa que não existem pacotes disponiveis no momento;
-A URA Cognitiva agradece e encerra a ligação.</t>
+6 - A URA Cognitiva informa que não existem pacotes disponiveis no momento;
+7 - A URA Cognitiva agradece e encerra a ligação.</t>
   </si>
   <si>
     <t>9</t>
@@ -262,15 +262,15 @@
 Quer algo mais.</t>
   </si>
   <si>
-    <t>Chamada é encaminhada para a URA Cognitiva;
-Ouvir a saudacão da URA Cognitiva conforme descrito na DF.
-A URA Congnitiva informa que entendeu que deseja falar sobre Contratação de Pacotes;
-A URA Cognitiva pede para aguardar enquanto verifica a internet;
-A URA Cognitiva informa que está com velocidade reduzida porque já consumiu o pacote,
+    <t>1 - Chamada é encaminhada para a URA Cognitiva;
+2 - Ouvir a saudacão da URA Cognitiva conforme descrito na DF.
+3 - A URA Congnitiva informa que entendeu que deseja falar sobre Contratação de Pacotes;
+4 - A URA Cognitiva pede para aguardar enquanto verifica a internet;
+5 - A URA Cognitiva informa que está com velocidade reduzida porque já consumiu o pacote,
 mas pode contratar um pacote adicional e verifica se existem pacotes disponiveis;
-A URA Cognitiva lista e oferece os pacotes disponíveis ao cliente;
-URA informa o pacote foi contratado;
-A URA Cognitiva transfere para o desambiguador.</t>
+6 - A URA Cognitiva lista e oferece os pacotes disponíveis ao cliente;
+7 - URA informa o pacote foi contratado;
+8 - A URA Cognitiva transfere para o desambiguador.</t>
   </si>
   <si>
     <t>10</t>
@@ -294,15 +294,15 @@
 Não quer mais nada.</t>
   </si>
   <si>
-    <t>Chamada é encaminhada para a URA Cognitiva;
-Ouvir a saudacão da URA Cognitiva conforme descrito na DF.
-A URA Congnitiva informa que entendeu que deseja falar sobre Contratação de Pacotes;
-A URA Cognitiva pede para aguardar enquanto verifica a internet;
-A URA Cognitiva informa que está com velocidade reduzida porque já consumiu o pacote,
+    <t>1 - Chamada é encaminhada para a URA Cognitiva;
+2 - Ouvir a saudacão da URA Cognitiva conforme descrito na DF.
+3 - A URA Congnitiva informa que entendeu que deseja falar sobre Contratação de Pacotes;
+4 - A URA Cognitiva pede para aguardar enquanto verifica a internet;
+5 - A URA Cognitiva informa que está com velocidade reduzida porque já consumiu o pacote,
 mas pode contratar um pacote adicional e verifica se existem pacotes disponiveis;
-A URA Cognitiva lista e oferece os pacotes disponíveis ao cliente;
-URA informa o pacote foi contratado;
-A URA Cognitiva agradece e encerra a ligação.</t>
+6 - A URA Cognitiva lista e oferece os pacotes disponíveis ao cliente;
+7 - URA informa o pacote foi contratado;
+8 - A URA Cognitiva agradece e encerra a ligação.</t>
   </si>
   <si>
     <t>11</t>
@@ -326,15 +326,15 @@
 Quer algo mais.</t>
   </si>
   <si>
-    <t>Chamada é encaminhada para a URA Cognitiva;
-Ouvir a saudacão da URA Cognitiva conforme descrito na DF.
-A URA Congnitiva informa que entendeu que deseja falar sobre Contratação de Pacotes;
-A URA Cognitiva pede para aguardar enquanto verifica a internet;
-A URA Cognitiva informa que está com velocidade reduzida porque já consumiu o pacote,
+    <t>1 - Chamada é encaminhada para a URA Cognitiva;
+2 - Ouvir a saudacão da URA Cognitiva conforme descrito na DF.
+3 - A URA Congnitiva informa que entendeu que deseja falar sobre Contratação de Pacotes;
+4 - A URA Cognitiva pede para aguardar enquanto verifica a internet;
+5 - A URA Cognitiva informa que está com velocidade reduzida porque já consumiu o pacote,
 mas pode contratar um pacote adicional e verifica se existem pacotes disponiveis;
-A URA Cognitiva lista e oferece os pacotes disponíveis ao cliente;
-URA informa o pacote não foi contratado;
-A URA Cognitiva transfere para o desambiguador.</t>
+6 - A URA Cognitiva lista e oferece os pacotes disponíveis ao cliente;
+7 - URA informa o pacote não foi contratado;
+8 - A URA Cognitiva transfere para o desambiguador.</t>
   </si>
   <si>
     <t>12</t>
@@ -358,15 +358,15 @@
 Não quer mais nada.</t>
   </si>
   <si>
-    <t>Chamada é encaminhada para a URA Cognitiva;
-Ouvir a saudacão da URA Cognitiva conforme descrito na DF.
-A URA Congnitiva informa que entendeu que deseja falar sobre Contratação de Pacotes;
-A URA Cognitiva pede para aguardar enquanto verifica a internet;
-A URA Cognitiva informa que está com velocidade reduzida porque já consumiu o pacote,
+    <t>1 - Chamada é encaminhada para a URA Cognitiva;
+2 - Ouvir a saudacão da URA Cognitiva conforme descrito na DF.
+3 - A URA Congnitiva informa que entendeu que deseja falar sobre Contratação de Pacotes;
+4 - A URA Cognitiva pede para aguardar enquanto verifica a internet;
+5 - A URA Cognitiva informa que está com velocidade reduzida porque já consumiu o pacote,
 mas pode contratar um pacote adicional e verifica se existem pacotes disponiveis;
-A URA Cognitiva lista e oferece os pacotes disponíveis ao cliente;
-URA informa o pacote não foi contratado;
-A URA Cognitiva agradece e encerra a ligação.</t>
+6 - A URA Cognitiva lista e oferece os pacotes disponíveis ao cliente;
+7 - URA informa o pacote não foi contratado;
+8 - A URA Cognitiva agradece e encerra a ligação.</t>
   </si>
   <si>
     <t>13</t>
@@ -391,16 +391,16 @@
 Quer algo mais.</t>
   </si>
   <si>
-    <t>Chamada é encaminhada para a URA Cognitiva;
-Ouvir a saudacão da URA Cognitiva conforme descrito na DF.
-A URA Congnitiva informa que entendeu que deseja falar sobre Contratação de Pacotes;
-A URA Cognitiva pede para aguardar enquanto verifica a internet;
-A URA Cognitiva informa que está com velocidade reduzida porque já consumiu o pacote,
+    <t>1 - Chamada é encaminhada para a URA Cognitiva;
+2 - Ouvir a saudacão da URA Cognitiva conforme descrito na DF.
+3 - A URA Congnitiva informa que entendeu que deseja falar sobre Contratação de Pacotes;
+4 - A URA Cognitiva pede para aguardar enquanto verifica a internet;
+5 - A URA Cognitiva informa que está com velocidade reduzida porque já consumiu o pacote,
 mas pode contratar um pacote adicional e verifica se existem pacotes disponiveis;
-A URA Cognitiva lista e oferece os pacotes disponíveis ao cliente;
-URA informa que precisa da senha única;
-URA informa o pacote foi contratado;
-A URA Cognitiva transfere para o desambiguador.</t>
+6 - A URA Cognitiva lista e oferece os pacotes disponíveis ao cliente;
+7 - URA informa que precisa da senha única;
+8 - URA informa o pacote foi contratado;
+9 - A URA Cognitiva transfere para o desambiguador.</t>
   </si>
   <si>
     <t>14</t>
@@ -425,16 +425,16 @@
 Não quer mais nada.</t>
   </si>
   <si>
-    <t>Chamada é encaminhada para a URA Cognitiva;
-Ouvir a saudacão da URA Cognitiva conforme descrito na DF.
-A URA Congnitiva informa que entendeu que deseja falar sobre Contratação de Pacotes;
-A URA Cognitiva pede para aguardar enquanto verifica a internet;
-A URA Cognitiva informa que está com velocidade reduzida porque já consumiu o pacote,
+    <t>1 - Chamada é encaminhada para a URA Cognitiva;
+2 - Ouvir a saudacão da URA Cognitiva conforme descrito na DF.
+3 - A URA Congnitiva informa que entendeu que deseja falar sobre Contratação de Pacotes;
+4 - A URA Cognitiva pede para aguardar enquanto verifica a internet;
+5 - A URA Cognitiva informa que está com velocidade reduzida porque já consumiu o pacote,
 mas pode contratar um pacote adicional e verifica se existem pacotes disponiveis;
-A URA Cognitiva lista e oferece os pacotes disponíveis ao cliente;
-URA informa que precisa da senha única;
-URA informa o pacote foi contratado;
-A URA Cognitiva agradece e encerra a ligação.</t>
+6 - A URA Cognitiva lista e oferece os pacotes disponíveis ao cliente;
+7 - URA informa que precisa da senha única;
+8 - URA informa o pacote foi contratado;
+9 - A URA Cognitiva agradece e encerra a ligação.</t>
   </si>
   <si>
     <t>15</t>
@@ -459,16 +459,16 @@
 Quer algo mais.</t>
   </si>
   <si>
-    <t>Chamada é encaminhada para a URA Cognitiva;
-Ouvir a saudacão da URA Cognitiva conforme descrito na DF.
-A URA Congnitiva informa que entendeu que deseja falar sobre Contratação de Pacotes;
-A URA Cognitiva pede para aguardar enquanto verifica a internet;
-A URA Cognitiva informa que está com velocidade reduzida porque já consumiu o pacote,
+    <t>1 - Chamada é encaminhada para a URA Cognitiva;
+2 - Ouvir a saudacão da URA Cognitiva conforme descrito na DF.
+3 - A URA Congnitiva informa que entendeu que deseja falar sobre Contratação de Pacotes;
+4 - A URA Cognitiva pede para aguardar enquanto verifica a internet;
+5 - A URA Cognitiva informa que está com velocidade reduzida porque já consumiu o pacote,
 mas pode contratar um pacote adicional e verifica se existem pacotes disponiveis;
-A URA Cognitiva lista e oferece os pacotes disponíveis ao cliente;
-URA informa que precisa da senha única;
-URA informa o pacote não foi contratado;
-A URA Cognitiva transfere para o desambiguador.</t>
+6 - A URA Cognitiva lista e oferece os pacotes disponíveis ao cliente;
+7 - URA informa que precisa da senha única;
+8 - URA informa o pacote não foi contratado;
+9 - A URA Cognitiva transfere para o desambiguador.</t>
   </si>
   <si>
     <t>16</t>
@@ -493,16 +493,16 @@
 Não quer mais nada.</t>
   </si>
   <si>
-    <t>Chamada é encaminhada para a URA Cognitiva;
-Ouvir a saudacão da URA Cognitiva conforme descrito na DF.
-A URA Congnitiva informa que entendeu que deseja falar sobre Contratação de Pacotes;
-A URA Cognitiva pede para aguardar enquanto verifica a internet;
-A URA Cognitiva informa que está com velocidade reduzida porque já consumiu o pacote,
+    <t>1 - Chamada é encaminhada para a URA Cognitiva;
+2 - Ouvir a saudacão da URA Cognitiva conforme descrito na DF.
+3 - A URA Congnitiva informa que entendeu que deseja falar sobre Contratação de Pacotes;
+4 - A URA Cognitiva pede para aguardar enquanto verifica a internet;
+5 - A URA Cognitiva informa que está com velocidade reduzida porque já consumiu o pacote,
 mas pode contratar um pacote adicional e verifica se existem pacotes disponiveis;
-A URA Cognitiva lista e oferece os pacotes disponíveis ao cliente;
-URA informa que precisa da senha única;
-URA informa o pacote não foi contratado;
-A URA Cognitiva agradece e encerra a ligação.</t>
+6 - A URA Cognitiva lista e oferece os pacotes disponíveis ao cliente;
+7 - URA informa que precisa da senha única;
+8 - URA informa o pacote não foi contratado;
+9 - A URA Cognitiva agradece e encerra a ligação.</t>
   </si>
   <si>
     <t>17</t>
@@ -526,16 +526,16 @@
 Quer algo mais.</t>
   </si>
   <si>
-    <t>Chamada é encaminhada para a URA Cognitiva;
-Ouvir a saudacão da URA Cognitiva conforme descrito na DF.
-A URA Congnitiva informa que entendeu que deseja falar sobre Contratação de Pacotes;
-A URA Cognitiva pede para aguardar enquanto verifica a internet;
-A URA Cognitiva informa que está com velocidade reduzida porque já consumiu o pacote,
+    <t>1 - Chamada é encaminhada para a URA Cognitiva;
+2 - Ouvir a saudacão da URA Cognitiva conforme descrito na DF.
+3 - A URA Congnitiva informa que entendeu que deseja falar sobre Contratação de Pacotes;
+4 - A URA Cognitiva pede para aguardar enquanto verifica a internet;
+5 - A URA Cognitiva informa que está com velocidade reduzida porque já consumiu o pacote,
 mas pode contratar um pacote adicional e verifica se existem pacotes disponiveis;
-A URA Cognitiva lista e oferece os pacotes disponíveis ao cliente;
-URA informa que precisa da senha única;
-URA Informa que não foi possível confirmar os dados do cliente e não vai poder prosseguir;
-A URA Cognitiva transfere para o desambiguador.</t>
+6 - A URA Cognitiva lista e oferece os pacotes disponíveis ao cliente;
+7 - URA informa que precisa da senha única;
+8 - URA Informa que não foi possível confirmar os dados do cliente e não vai poder prosseguir;
+9 - A URA Cognitiva transfere para o desambiguador.</t>
   </si>
   <si>
     <t>18</t>
@@ -559,16 +559,16 @@
 Não quer mais nada.</t>
   </si>
   <si>
-    <t>Chamada é encaminhada para a URA Cognitiva;
-Ouvir a saudacão da URA Cognitiva conforme descrito na DF.
-A URA Congnitiva informa que entendeu que deseja falar sobre Contratação de Pacotes;
-A URA Cognitiva pede para aguardar enquanto verifica a internet;
-A URA Cognitiva informa que está com velocidade reduzida porque já consumiu o pacote,
+    <t>1 - Chamada é encaminhada para a URA Cognitiva;
+2 - Ouvir a saudacão da URA Cognitiva conforme descrito na DF.
+3 - A URA Congnitiva informa que entendeu que deseja falar sobre Contratação de Pacotes;
+4 - A URA Cognitiva pede para aguardar enquanto verifica a internet;
+5 - A URA Cognitiva informa que está com velocidade reduzida porque já consumiu o pacote,
 mas pode contratar um pacote adicional e verifica se existem pacotes disponiveis;
-A URA Cognitiva lista e oferece os pacotes disponíveis ao cliente;
-URA informa que precisa da senha única;
-URA Informa que não foi possível confirmar os dados do cliente e não vai poder prosseguir;
-A URA Cognitiva agradece e encerra a ligação.</t>
+6 - A URA Cognitiva lista e oferece os pacotes disponíveis ao cliente;
+7 - URA informa que precisa da senha única;
+8 - URA Informa que não foi possível confirmar os dados do cliente e não vai poder prosseguir;
+9 - A URA Cognitiva agradece e encerra a ligação.</t>
   </si>
   <si>
     <t>19</t>
@@ -592,15 +592,15 @@
 Quer algo mais.</t>
   </si>
   <si>
-    <t>Chamada é encaminhada para a URA Cognitiva;
-Ouvir a saudacão da URA Cognitiva conforme descrito na DF.
-A URA Congnitiva informa que entendeu que deseja falar sobre Contratação de Pacotes;
-A URA Cognitiva pede para aguardar enquanto verifica a internet;
-A URA Cognitiva informa que está com velocidade reduzida porque já consumiu o pacote,
+    <t>1 - Chamada é encaminhada para a URA Cognitiva;
+2 - Ouvir a saudacão da URA Cognitiva conforme descrito na DF.
+3 - A URA Congnitiva informa que entendeu que deseja falar sobre Contratação de Pacotes;
+4 - A URA Cognitiva pede para aguardar enquanto verifica a internet;
+5 - A URA Cognitiva informa que está com velocidade reduzida porque já consumiu o pacote,
 mas pode contratar um pacote adicional e verifica se existem pacotes disponiveis;
-A URA Cognitiva lista e oferece os pacotes disponíveis ao cliente;
-A URA Cognitiva informa que não efetuou a contratação;
-A URA Cognitiva transfere para o desambiguador.</t>
+6 - A URA Cognitiva lista e oferece os pacotes disponíveis ao cliente;
+7 - A URA Cognitiva informa que não efetuou a contratação;
+8 - A URA Cognitiva transfere para o desambiguador.</t>
   </si>
   <si>
     <t>20</t>
@@ -624,15 +624,15 @@
 Não quer mais nada.</t>
   </si>
   <si>
-    <t>Chamada é encaminhada para a URA Cognitiva;
-Ouvir a saudacão da URA Cognitiva conforme descrito na DF.
-A URA Congnitiva informa que entendeu que deseja falar sobre Contratação de Pacotes;
-A URA Cognitiva pede para aguardar enquanto verifica a internet;
-A URA Cognitiva informa que está com velocidade reduzida porque já consumiu o pacote,
+    <t>1 - Chamada é encaminhada para a URA Cognitiva;
+2 - Ouvir a saudacão da URA Cognitiva conforme descrito na DF.
+3 - A URA Congnitiva informa que entendeu que deseja falar sobre Contratação de Pacotes;
+4 - A URA Cognitiva pede para aguardar enquanto verifica a internet;
+5 - A URA Cognitiva informa que está com velocidade reduzida porque já consumiu o pacote,
 mas pode contratar um pacote adicional e verifica se existem pacotes disponiveis;
-A URA Cognitiva lista e oferece os pacotes disponíveis ao cliente;
-A URA Cognitiva informa que não efetuou a contratação;
-A URA Cognitiva agradece e encerra a ligação.</t>
+6 - A URA Cognitiva lista e oferece os pacotes disponíveis ao cliente;
+7 - A URA Cognitiva informa que não efetuou a contratação;
+8 - A URA Cognitiva agradece e encerra a ligação.</t>
   </si>
   <si>
     <t>21</t>
@@ -658,16 +658,16 @@
 Quer algo mais.</t>
   </si>
   <si>
-    <t>Chamada é encaminhada para a URA Cognitiva;
-Ouvir a saudacão da URA Cognitiva conforme descrito na DF.
-A URA Congnitiva informa que entendeu que deseja falar sobre Contratação de Pacotes;
-A URA Cognitiva pede para aguardar enquanto verifica a internet;
-A URA Cognitiva informa que está com velocidade reduzida porque já consumiu o pacote,
+    <t>1 - Chamada é encaminhada para a URA Cognitiva;
+2 - Ouvir a saudacão da URA Cognitiva conforme descrito na DF.
+3 - A URA Congnitiva informa que entendeu que deseja falar sobre Contratação de Pacotes;
+4 - A URA Cognitiva pede para aguardar enquanto verifica a internet;
+5 - A URA Cognitiva informa que está com velocidade reduzida porque já consumiu o pacote,
 mas pode contratar um pacote adicional e verifica se existem pacotes disponiveis;
-A URA Cognitiva lista e oferece os pacotes disponíveis ao cliente;
-A URA Cognitiva informa que no momento estas são as únicas opções disponíveis;
-URA informa o pacote foi contratado;
-A URA Cognitiva transfere para o desambiguador.</t>
+6 - A URA Cognitiva lista e oferece os pacotes disponíveis ao cliente;
+7 - A URA Cognitiva informa que no momento estas são as únicas opções disponíveis;
+8 - URA informa o pacote foi contratado;
+9 - A URA Cognitiva transfere para o desambiguador.</t>
   </si>
   <si>
     <t>22</t>
@@ -693,16 +693,16 @@
 Não quer mais nada.</t>
   </si>
   <si>
-    <t>Chamada é encaminhada para a URA Cognitiva;
-Ouvir a saudacão da URA Cognitiva conforme descrito na DF.
-A URA Congnitiva informa que entendeu que deseja falar sobre Contratação de Pacotes;
-A URA Cognitiva pede para aguardar enquanto verifica a internet;
-A URA Cognitiva informa que está com velocidade reduzida porque já consumiu o pacote,
+    <t>1 - Chamada é encaminhada para a URA Cognitiva;
+2 - Ouvir a saudacão da URA Cognitiva conforme descrito na DF.
+3 - A URA Congnitiva informa que entendeu que deseja falar sobre Contratação de Pacotes;
+4 - A URA Cognitiva pede para aguardar enquanto verifica a internet;
+5 - A URA Cognitiva informa que está com velocidade reduzida porque já consumiu o pacote,
 mas pode contratar um pacote adicional e verifica se existem pacotes disponiveis;
-A URA Cognitiva lista e oferece os pacotes disponíveis ao cliente;
-A URA Cognitiva informa que no momento estas são as únicas opções disponíveis;
-URA informa o pacote foi contratado;
-A URA Cognitiva agradece e encerra a ligação.</t>
+6 - A URA Cognitiva lista e oferece os pacotes disponíveis ao cliente;
+7 - A URA Cognitiva informa que no momento estas são as únicas opções disponíveis;
+8 - URA informa o pacote foi contratado;
+9 - A URA Cognitiva agradece e encerra a ligação.</t>
   </si>
   <si>
     <t>23</t>
@@ -728,16 +728,16 @@
 Quer algo mais.</t>
   </si>
   <si>
-    <t>Chamada é encaminhada para a URA Cognitiva;
-Ouvir a saudacão da URA Cognitiva conforme descrito na DF.
-A URA Congnitiva informa que entendeu que deseja falar sobre Contratação de Pacotes;
-A URA Cognitiva pede para aguardar enquanto verifica a internet;
-A URA Cognitiva informa que está com velocidade reduzida porque já consumiu o pacote,
+    <t>1 - Chamada é encaminhada para a URA Cognitiva;
+2 - Ouvir a saudacão da URA Cognitiva conforme descrito na DF.
+3 - A URA Congnitiva informa que entendeu que deseja falar sobre Contratação de Pacotes;
+4 - A URA Cognitiva pede para aguardar enquanto verifica a internet;
+5 - A URA Cognitiva informa que está com velocidade reduzida porque já consumiu o pacote,
 mas pode contratar um pacote adicional e verifica se existem pacotes disponiveis;
-A URA Cognitiva lista e oferece os pacotes disponíveis ao cliente;
-A URA Cognitiva informa que no momento estas são as únicas opções disponíveis;
-URA informa o pacote não foi contratado;
-A URA Cognitiva transfere para o desambiguador.</t>
+6 - A URA Cognitiva lista e oferece os pacotes disponíveis ao cliente;
+7 - A URA Cognitiva informa que no momento estas são as únicas opções disponíveis;
+8 - URA informa o pacote não foi contratado;
+9 - A URA Cognitiva transfere para o desambiguador.</t>
   </si>
   <si>
     <t>24</t>
@@ -763,16 +763,16 @@
 Não quer mais nada.</t>
   </si>
   <si>
-    <t>Chamada é encaminhada para a URA Cognitiva;
-Ouvir a saudacão da URA Cognitiva conforme descrito na DF.
-A URA Congnitiva informa que entendeu que deseja falar sobre Contratação de Pacotes;
-A URA Cognitiva pede para aguardar enquanto verifica a internet;
-A URA Cognitiva informa que está com velocidade reduzida porque já consumiu o pacote,
+    <t>1 - Chamada é encaminhada para a URA Cognitiva;
+2 - Ouvir a saudacão da URA Cognitiva conforme descrito na DF.
+3 - A URA Congnitiva informa que entendeu que deseja falar sobre Contratação de Pacotes;
+4 - A URA Cognitiva pede para aguardar enquanto verifica a internet;
+5 - A URA Cognitiva informa que está com velocidade reduzida porque já consumiu o pacote,
 mas pode contratar um pacote adicional e verifica se existem pacotes disponiveis;
-A URA Cognitiva lista e oferece os pacotes disponíveis ao cliente;
-A URA Cognitiva informa que no momento estas são as únicas opções disponíveis;
-URA informa o pacote não foi contratado;
-A URA Cognitiva agradece e encerra a ligação.</t>
+6 - A URA Cognitiva lista e oferece os pacotes disponíveis ao cliente;
+7 - A URA Cognitiva informa que no momento estas são as únicas opções disponíveis;
+8 - URA informa o pacote não foi contratado;
+9 - A URA Cognitiva agradece e encerra a ligação.</t>
   </si>
   <si>
     <t>25</t>
@@ -799,17 +799,17 @@
 Quer algo mais.</t>
   </si>
   <si>
-    <t>Chamada é encaminhada para a URA Cognitiva;
-Ouvir a saudacão da URA Cognitiva conforme descrito na DF.
-A URA Congnitiva informa que entendeu que deseja falar sobre Contratação de Pacotes;
-A URA Cognitiva pede para aguardar enquanto verifica a internet;
-A URA Cognitiva informa que está com velocidade reduzida porque já consumiu o pacote,
+    <t>1 - Chamada é encaminhada para a URA Cognitiva;
+2 - Ouvir a saudacão da URA Cognitiva conforme descrito na DF.
+3 - A URA Congnitiva informa que entendeu que deseja falar sobre Contratação de Pacotes;
+4 - A URA Cognitiva pede para aguardar enquanto verifica a internet;
+5 - A URA Cognitiva informa que está com velocidade reduzida porque já consumiu o pacote,
 mas pode contratar um pacote adicional e verifica se existem pacotes disponiveis;
-A URA Cognitiva lista e oferece os pacotes disponíveis ao cliente;
-A URA Cognitiva informa que no momento estas são as únicas opções disponíveis;
-URA informa que precisa da senha única;
-URA informa o pacote foi contratado;
-A URA Cognitiva transfere para o desambiguador.</t>
+6 - A URA Cognitiva lista e oferece os pacotes disponíveis ao cliente;
+7 - A URA Cognitiva informa que no momento estas são as únicas opções disponíveis;
+8 - URA informa que precisa da senha única;
+9 - URA informa o pacote foi contratado;
+10 - A URA Cognitiva transfere para o desambiguador.</t>
   </si>
   <si>
     <t>26</t>
@@ -836,17 +836,17 @@
 Não quer mais nada.</t>
   </si>
   <si>
-    <t>Chamada é encaminhada para a URA Cognitiva;
-Ouvir a saudacão da URA Cognitiva conforme descrito na DF.
-A URA Congnitiva informa que entendeu que deseja falar sobre Contratação de Pacotes;
-A URA Cognitiva pede para aguardar enquanto verifica a internet;
-A URA Cognitiva informa que está com velocidade reduzida porque já consumiu o pacote,
+    <t>1 - Chamada é encaminhada para a URA Cognitiva;
+2 - Ouvir a saudacão da URA Cognitiva conforme descrito na DF.
+3 - A URA Congnitiva informa que entendeu que deseja falar sobre Contratação de Pacotes;
+4 - A URA Cognitiva pede para aguardar enquanto verifica a internet;
+5 - A URA Cognitiva informa que está com velocidade reduzida porque já consumiu o pacote,
 mas pode contratar um pacote adicional e verifica se existem pacotes disponiveis;
-A URA Cognitiva lista e oferece os pacotes disponíveis ao cliente;
-A URA Cognitiva informa que no momento estas são as únicas opções disponíveis;
-URA informa que precisa da senha única;
-URA informa o pacote foi contratado;
-A URA Cognitiva agradece e encerra a ligação.</t>
+6 - A URA Cognitiva lista e oferece os pacotes disponíveis ao cliente;
+7 - A URA Cognitiva informa que no momento estas são as únicas opções disponíveis;
+8 - URA informa que precisa da senha única;
+9 - URA informa o pacote foi contratado;
+10 - A URA Cognitiva agradece e encerra a ligação.</t>
   </si>
   <si>
     <t>27</t>
@@ -873,17 +873,17 @@
 Quer algo mais.</t>
   </si>
   <si>
-    <t>Chamada é encaminhada para a URA Cognitiva;
-Ouvir a saudacão da URA Cognitiva conforme descrito na DF.
-A URA Congnitiva informa que entendeu que deseja falar sobre Contratação de Pacotes;
-A URA Cognitiva pede para aguardar enquanto verifica a internet;
-A URA Cognitiva informa que está com velocidade reduzida porque já consumiu o pacote,
+    <t>1 - Chamada é encaminhada para a URA Cognitiva;
+2 - Ouvir a saudacão da URA Cognitiva conforme descrito na DF.
+3 - A URA Congnitiva informa que entendeu que deseja falar sobre Contratação de Pacotes;
+4 - A URA Cognitiva pede para aguardar enquanto verifica a internet;
+5 - A URA Cognitiva informa que está com velocidade reduzida porque já consumiu o pacote,
 mas pode contratar um pacote adicional e verifica se existem pacotes disponiveis;
-A URA Cognitiva lista e oferece os pacotes disponíveis ao cliente;
-A URA Cognitiva informa que no momento estas são as únicas opções disponíveis;
-URA informa que precisa da senha única;
-URA informa o pacote não foi contratado;
-A URA Cognitiva transfere para o desambiguador.</t>
+6 - A URA Cognitiva lista e oferece os pacotes disponíveis ao cliente;
+7 - A URA Cognitiva informa que no momento estas são as únicas opções disponíveis;
+8 - URA informa que precisa da senha única;
+9 - URA informa o pacote não foi contratado;
+10 - A URA Cognitiva transfere para o desambiguador.</t>
   </si>
   <si>
     <t>28</t>
@@ -910,17 +910,17 @@
 Não quer mais nada.</t>
   </si>
   <si>
-    <t>Chamada é encaminhada para a URA Cognitiva;
-Ouvir a saudacão da URA Cognitiva conforme descrito na DF.
-A URA Congnitiva informa que entendeu que deseja falar sobre Contratação de Pacotes;
-A URA Cognitiva pede para aguardar enquanto verifica a internet;
-A URA Cognitiva informa que está com velocidade reduzida porque já consumiu o pacote,
+    <t>1 - Chamada é encaminhada para a URA Cognitiva;
+2 - Ouvir a saudacão da URA Cognitiva conforme descrito na DF.
+3 - A URA Congnitiva informa que entendeu que deseja falar sobre Contratação de Pacotes;
+4 - A URA Cognitiva pede para aguardar enquanto verifica a internet;
+5 - A URA Cognitiva informa que está com velocidade reduzida porque já consumiu o pacote,
 mas pode contratar um pacote adicional e verifica se existem pacotes disponiveis;
-A URA Cognitiva lista e oferece os pacotes disponíveis ao cliente;
-A URA Cognitiva informa que no momento estas são as únicas opções disponíveis;
-URA informa que precisa da senha única;
-URA informa o pacote não foi contratado;
-A URA Cognitiva agradece e encerra a ligação.</t>
+6 - A URA Cognitiva lista e oferece os pacotes disponíveis ao cliente;
+7 - A URA Cognitiva informa que no momento estas são as únicas opções disponíveis;
+8 - URA informa que precisa da senha única;
+9 - URA informa o pacote não foi contratado;
+10 - A URA Cognitiva agradece e encerra a ligação.</t>
   </si>
   <si>
     <t>29</t>
@@ -946,17 +946,17 @@
 Quer algo mais.</t>
   </si>
   <si>
-    <t>Chamada é encaminhada para a URA Cognitiva;
-Ouvir a saudacão da URA Cognitiva conforme descrito na DF.
-A URA Congnitiva informa que entendeu que deseja falar sobre Contratação de Pacotes;
-A URA Cognitiva pede para aguardar enquanto verifica a internet;
-A URA Cognitiva informa que está com velocidade reduzida porque já consumiu o pacote,
+    <t>1 - Chamada é encaminhada para a URA Cognitiva;
+2 - Ouvir a saudacão da URA Cognitiva conforme descrito na DF.
+3 - A URA Congnitiva informa que entendeu que deseja falar sobre Contratação de Pacotes;
+4 - A URA Cognitiva pede para aguardar enquanto verifica a internet;
+5 - A URA Cognitiva informa que está com velocidade reduzida porque já consumiu o pacote,
 mas pode contratar um pacote adicional e verifica se existem pacotes disponiveis;
-A URA Cognitiva lista e oferece os pacotes disponíveis ao cliente;
-A URA Cognitiva informa que no momento estas são as únicas opções disponíveis;
-URA informa que precisa da senha única;
-URA Informa que não foi possível confirmar os dados do cliente e não vai poder prosseguir;
-A URA Cognitiva transfere para o desambiguador.</t>
+6 - A URA Cognitiva lista e oferece os pacotes disponíveis ao cliente;
+7 - A URA Cognitiva informa que no momento estas são as únicas opções disponíveis;
+8 - URA informa que precisa da senha única;
+9 - URA Informa que não foi possível confirmar os dados do cliente e não vai poder prosseguir;
+10 - A URA Cognitiva transfere para o desambiguador.</t>
   </si>
   <si>
     <t>30</t>
@@ -982,17 +982,17 @@
 Não quer mais nada.</t>
   </si>
   <si>
-    <t>Chamada é encaminhada para a URA Cognitiva;
-Ouvir a saudacão da URA Cognitiva conforme descrito na DF.
-A URA Congnitiva informa que entendeu que deseja falar sobre Contratação de Pacotes;
-A URA Cognitiva pede para aguardar enquanto verifica a internet;
-A URA Cognitiva informa que está com velocidade reduzida porque já consumiu o pacote,
+    <t>1 - Chamada é encaminhada para a URA Cognitiva;
+2 - Ouvir a saudacão da URA Cognitiva conforme descrito na DF.
+3 - A URA Congnitiva informa que entendeu que deseja falar sobre Contratação de Pacotes;
+4 - A URA Cognitiva pede para aguardar enquanto verifica a internet;
+5 - A URA Cognitiva informa que está com velocidade reduzida porque já consumiu o pacote,
 mas pode contratar um pacote adicional e verifica se existem pacotes disponiveis;
-A URA Cognitiva lista e oferece os pacotes disponíveis ao cliente;
-A URA Cognitiva informa que no momento estas são as únicas opções disponíveis;
-URA informa que precisa da senha única;
-URA Informa que não foi possível confirmar os dados do cliente e não vai poder prosseguir;
-A URA Cognitiva agradece e encerra a ligação.</t>
+6 - A URA Cognitiva lista e oferece os pacotes disponíveis ao cliente;
+7 - A URA Cognitiva informa que no momento estas são as únicas opções disponíveis;
+8 - URA informa que precisa da senha única;
+9 - URA Informa que não foi possível confirmar os dados do cliente e não vai poder prosseguir;
+10 - A URA Cognitiva agradece e encerra a ligação.</t>
   </si>
   <si>
     <t>31</t>
@@ -1018,16 +1018,16 @@
 Quer algo mais.</t>
   </si>
   <si>
-    <t>Chamada é encaminhada para a URA Cognitiva;
-Ouvir a saudacão da URA Cognitiva conforme descrito na DF.
-A URA Congnitiva informa que entendeu que deseja falar sobre Contratação de Pacotes;
-A URA Cognitiva pede para aguardar enquanto verifica a internet;
-A URA Cognitiva informa que está com velocidade reduzida porque já consumiu o pacote,
+    <t>1 - Chamada é encaminhada para a URA Cognitiva;
+2 - Ouvir a saudacão da URA Cognitiva conforme descrito na DF.
+3 - A URA Congnitiva informa que entendeu que deseja falar sobre Contratação de Pacotes;
+4 - A URA Cognitiva pede para aguardar enquanto verifica a internet;
+5 - A URA Cognitiva informa que está com velocidade reduzida porque já consumiu o pacote,
 mas pode contratar um pacote adicional e verifica se existem pacotes disponiveis;
-A URA Cognitiva lista e oferece os pacotes disponíveis ao cliente;
-A URA Cognitiva informa que no momento estas são as únicas opções disponíveis;
-A URA Cognitiva informa que não efetuou a contratação;
-A URA Cognitiva transfere para o desambiguador.</t>
+6 - A URA Cognitiva lista e oferece os pacotes disponíveis ao cliente;
+7 - A URA Cognitiva informa que no momento estas são as únicas opções disponíveis;
+8 - A URA Cognitiva informa que não efetuou a contratação;
+9 - A URA Cognitiva transfere para o desambiguador.</t>
   </si>
   <si>
     <t>32</t>
@@ -1053,16 +1053,16 @@
 Não quer mais nada.</t>
   </si>
   <si>
-    <t>Chamada é encaminhada para a URA Cognitiva;
-Ouvir a saudacão da URA Cognitiva conforme descrito na DF.
-A URA Congnitiva informa que entendeu que deseja falar sobre Contratação de Pacotes;
-A URA Cognitiva pede para aguardar enquanto verifica a internet;
-A URA Cognitiva informa que está com velocidade reduzida porque já consumiu o pacote,
+    <t>1 - Chamada é encaminhada para a URA Cognitiva;
+2 - Ouvir a saudacão da URA Cognitiva conforme descrito na DF.
+3 - A URA Congnitiva informa que entendeu que deseja falar sobre Contratação de Pacotes;
+4 - A URA Cognitiva pede para aguardar enquanto verifica a internet;
+5 - A URA Cognitiva informa que está com velocidade reduzida porque já consumiu o pacote,
 mas pode contratar um pacote adicional e verifica se existem pacotes disponiveis;
-A URA Cognitiva lista e oferece os pacotes disponíveis ao cliente;
-A URA Cognitiva informa que no momento estas são as únicas opções disponíveis;
-A URA Cognitiva informa que não efetuou a contratação;
-A URA Cognitiva agradece e encerra a ligação.</t>
+6 - A URA Cognitiva lista e oferece os pacotes disponíveis ao cliente;
+7 - A URA Cognitiva informa que no momento estas são as únicas opções disponíveis;
+8 - A URA Cognitiva informa que não efetuou a contratação;
+9 - A URA Cognitiva agradece e encerra a ligação.</t>
   </si>
   <si>
     <t>33</t>
@@ -1085,15 +1085,15 @@
 Quer algo mais.</t>
   </si>
   <si>
-    <t>Chamada é encaminhada para a URA Cognitiva;
-Ouvir a saudacão da URA Cognitiva conforme descrito na DF.
-A URA Congnitiva informa que entendeu que deseja falar sobre Contratação de Pacotes;
-A URA Cognitiva pede para aguardar enquanto verifica a internet;
-A URA Cognitiva informa que está com velocidade reduzida porque já consumiu o pacote,
+    <t>1 - Chamada é encaminhada para a URA Cognitiva;
+2 - Ouvir a saudacão da URA Cognitiva conforme descrito na DF.
+3 - A URA Congnitiva informa que entendeu que deseja falar sobre Contratação de Pacotes;
+4 - A URA Cognitiva pede para aguardar enquanto verifica a internet;
+5 - A URA Cognitiva informa que está com velocidade reduzida porque já consumiu o pacote,
 mas pode contratar um pacote adicional e verifica se existem pacotes disponiveis;
-A URA Cognitiva lista e oferece os pacotes disponíveis ao cliente;
-A URA Cognitiva informa que no momento estas são as únicas opções disponíveis;
-A URA Cognitiva transfere para o desambiguador.</t>
+6 - A URA Cognitiva lista e oferece os pacotes disponíveis ao cliente;
+7 - A URA Cognitiva informa que no momento estas são as únicas opções disponíveis;
+8 - A URA Cognitiva transfere para o desambiguador.</t>
   </si>
   <si>
     <t>34</t>
@@ -1116,15 +1116,15 @@
 Não quer mais nada.</t>
   </si>
   <si>
-    <t>Chamada é encaminhada para a URA Cognitiva;
-Ouvir a saudacão da URA Cognitiva conforme descrito na DF.
-A URA Congnitiva informa que entendeu que deseja falar sobre Contratação de Pacotes;
-A URA Cognitiva pede para aguardar enquanto verifica a internet;
-A URA Cognitiva informa que está com velocidade reduzida porque já consumiu o pacote,
+    <t>1 - Chamada é encaminhada para a URA Cognitiva;
+2 - Ouvir a saudacão da URA Cognitiva conforme descrito na DF.
+3 - A URA Congnitiva informa que entendeu que deseja falar sobre Contratação de Pacotes;
+4 - A URA Cognitiva pede para aguardar enquanto verifica a internet;
+5 - A URA Cognitiva informa que está com velocidade reduzida porque já consumiu o pacote,
 mas pode contratar um pacote adicional e verifica se existem pacotes disponiveis;
-A URA Cognitiva lista e oferece os pacotes disponíveis ao cliente;
-A URA Cognitiva informa que no momento estas são as únicas opções disponíveis;
-A URA Cognitiva agradece e encerra a ligação.</t>
+6 - A URA Cognitiva lista e oferece os pacotes disponíveis ao cliente;
+7 - A URA Cognitiva informa que no momento estas são as únicas opções disponíveis;
+8 - A URA Cognitiva agradece e encerra a ligação.</t>
   </si>
   <si>
     <t>35</t>
@@ -1184,12 +1184,12 @@
 Quer algo mais.</t>
   </si>
   <si>
-    <t>Chamada é encaminhada para a URA Cognitiva;
-Ouvir a saudacão da URA Cognitiva conforme descrito na DF.
-A URA Congnitiva informa que entendeu que deseja falar sobre Contratação de Pacotes;
-A URA Cognitiva pede para aguardar enquanto verifica a internet;
-A URA Cognitiva informa que não existem pacotes disponiveis no momento;
-A URA Cognitiva transfere para o desambiguador.</t>
+    <t>1 - Chamada é encaminhada para a URA Cognitiva;
+2 - Ouvir a saudacão da URA Cognitiva conforme descrito na DF.
+3 - A URA Congnitiva informa que entendeu que deseja falar sobre Contratação de Pacotes;
+4 - A URA Cognitiva pede para aguardar enquanto verifica a internet;
+5 - A URA Cognitiva informa que não existem pacotes disponiveis no momento;
+6 - A URA Cognitiva transfere para o desambiguador.</t>
   </si>
   <si>
     <t>38</t>
@@ -1209,12 +1209,12 @@
 Não quer mais nada.</t>
   </si>
   <si>
-    <t>Chamada é encaminhada para a URA Cognitiva;
-Ouvir a saudacão da URA Cognitiva conforme descrito na DF.
-A URA Congnitiva informa que entendeu que deseja falar sobre Contratação de Pacotes;
-A URA Cognitiva pede para aguardar enquanto verifica a internet;
-A URA Cognitiva informa que não existem pacotes disponiveis no momento;
-A URA Cognitiva agradece e encerra a ligação.</t>
+    <t>1 - Chamada é encaminhada para a URA Cognitiva;
+2 - Ouvir a saudacão da URA Cognitiva conforme descrito na DF.
+3 - A URA Congnitiva informa que entendeu que deseja falar sobre Contratação de Pacotes;
+4 - A URA Cognitiva pede para aguardar enquanto verifica a internet;
+5 - A URA Cognitiva informa que não existem pacotes disponiveis no momento;
+6 - A URA Cognitiva agradece e encerra a ligação.</t>
   </si>
   <si>
     <t>39</t>
@@ -1238,13 +1238,13 @@
 Quer algo mais.</t>
   </si>
   <si>
-    <t>Chamada é encaminhada para a URA Cognitiva;
-Ouvir a saudacão da URA Cognitiva conforme descrito na DF.
-A URA Congnitiva informa que entendeu que deseja falar sobre Contratação de Pacotes;
-A URA Cognitiva pede para aguardar enquanto verifica a internet;
-A URA Cognitiva lista e oferece os pacotes disponíveis ao cliente;
-URA informa o pacote foi contratado;
-A URA Cognitiva transfere para o desambiguador.</t>
+    <t>1 - Chamada é encaminhada para a URA Cognitiva;
+2 - Ouvir a saudacão da URA Cognitiva conforme descrito na DF.
+3 - A URA Congnitiva informa que entendeu que deseja falar sobre Contratação de Pacotes;
+4 - A URA Cognitiva pede para aguardar enquanto verifica a internet;
+5 - A URA Cognitiva lista e oferece os pacotes disponíveis ao cliente;
+6 - URA informa o pacote foi contratado;
+7 - A URA Cognitiva transfere para o desambiguador.</t>
   </si>
   <si>
     <t>40</t>
@@ -1268,13 +1268,13 @@
 Não quer mais nada.</t>
   </si>
   <si>
-    <t>Chamada é encaminhada para a URA Cognitiva;
-Ouvir a saudacão da URA Cognitiva conforme descrito na DF.
-A URA Congnitiva informa que entendeu que deseja falar sobre Contratação de Pacotes;
-A URA Cognitiva pede para aguardar enquanto verifica a internet;
-A URA Cognitiva lista e oferece os pacotes disponíveis ao cliente;
-URA informa o pacote foi contratado;
-A URA Cognitiva agradece e encerra a ligação.</t>
+    <t>1 - Chamada é encaminhada para a URA Cognitiva;
+2 - Ouvir a saudacão da URA Cognitiva conforme descrito na DF.
+3 - A URA Congnitiva informa que entendeu que deseja falar sobre Contratação de Pacotes;
+4 - A URA Cognitiva pede para aguardar enquanto verifica a internet;
+5 - A URA Cognitiva lista e oferece os pacotes disponíveis ao cliente;
+6 - URA informa o pacote foi contratado;
+7 - A URA Cognitiva agradece e encerra a ligação.</t>
   </si>
   <si>
     <t>41</t>
@@ -1298,13 +1298,13 @@
 Quer algo mais.</t>
   </si>
   <si>
-    <t>Chamada é encaminhada para a URA Cognitiva;
-Ouvir a saudacão da URA Cognitiva conforme descrito na DF.
-A URA Congnitiva informa que entendeu que deseja falar sobre Contratação de Pacotes;
-A URA Cognitiva pede para aguardar enquanto verifica a internet;
-A URA Cognitiva lista e oferece os pacotes disponíveis ao cliente;
-URA informa o pacote não foi contratado;
-A URA Cognitiva transfere para o desambiguador.</t>
+    <t>1 - Chamada é encaminhada para a URA Cognitiva;
+2 - Ouvir a saudacão da URA Cognitiva conforme descrito na DF.
+3 - A URA Congnitiva informa que entendeu que deseja falar sobre Contratação de Pacotes;
+4 - A URA Cognitiva pede para aguardar enquanto verifica a internet;
+5 - A URA Cognitiva lista e oferece os pacotes disponíveis ao cliente;
+6 - URA informa o pacote não foi contratado;
+7 - A URA Cognitiva transfere para o desambiguador.</t>
   </si>
   <si>
     <t>42</t>
@@ -1328,13 +1328,13 @@
 Não quer mais nada.</t>
   </si>
   <si>
-    <t>Chamada é encaminhada para a URA Cognitiva;
-Ouvir a saudacão da URA Cognitiva conforme descrito na DF.
-A URA Congnitiva informa que entendeu que deseja falar sobre Contratação de Pacotes;
-A URA Cognitiva pede para aguardar enquanto verifica a internet;
-A URA Cognitiva lista e oferece os pacotes disponíveis ao cliente;
-URA informa o pacote não foi contratado;
-A URA Cognitiva agradece e encerra a ligação.</t>
+    <t>1 - Chamada é encaminhada para a URA Cognitiva;
+2 - Ouvir a saudacão da URA Cognitiva conforme descrito na DF.
+3 - A URA Congnitiva informa que entendeu que deseja falar sobre Contratação de Pacotes;
+4 - A URA Cognitiva pede para aguardar enquanto verifica a internet;
+5 - A URA Cognitiva lista e oferece os pacotes disponíveis ao cliente;
+6 - URA informa o pacote não foi contratado;
+7 - A URA Cognitiva agradece e encerra a ligação.</t>
   </si>
   <si>
     <t>43</t>
@@ -1359,14 +1359,14 @@
 Quer algo mais.</t>
   </si>
   <si>
-    <t>Chamada é encaminhada para a URA Cognitiva;
-Ouvir a saudacão da URA Cognitiva conforme descrito na DF.
-A URA Congnitiva informa que entendeu que deseja falar sobre Contratação de Pacotes;
-A URA Cognitiva pede para aguardar enquanto verifica a internet;
-A URA Cognitiva lista e oferece os pacotes disponíveis ao cliente;
-URA informa que precisa da senha única;
-URA informa o pacote foi contratado;
-A URA Cognitiva transfere para o desambiguador.</t>
+    <t>1 - Chamada é encaminhada para a URA Cognitiva;
+2 - Ouvir a saudacão da URA Cognitiva conforme descrito na DF.
+3 - A URA Congnitiva informa que entendeu que deseja falar sobre Contratação de Pacotes;
+4 - A URA Cognitiva pede para aguardar enquanto verifica a internet;
+5 - A URA Cognitiva lista e oferece os pacotes disponíveis ao cliente;
+6 - URA informa que precisa da senha única;
+7 - URA informa o pacote foi contratado;
+8 - A URA Cognitiva transfere para o desambiguador.</t>
   </si>
   <si>
     <t>44</t>
@@ -1391,14 +1391,14 @@
 Não quer mais nada.</t>
   </si>
   <si>
-    <t>Chamada é encaminhada para a URA Cognitiva;
-Ouvir a saudacão da URA Cognitiva conforme descrito na DF.
-A URA Congnitiva informa que entendeu que deseja falar sobre Contratação de Pacotes;
-A URA Cognitiva pede para aguardar enquanto verifica a internet;
-A URA Cognitiva lista e oferece os pacotes disponíveis ao cliente;
-URA informa que precisa da senha única;
-URA informa o pacote foi contratado;
-A URA Cognitiva agradece e encerra a ligação.</t>
+    <t>1 - Chamada é encaminhada para a URA Cognitiva;
+2 - Ouvir a saudacão da URA Cognitiva conforme descrito na DF.
+3 - A URA Congnitiva informa que entendeu que deseja falar sobre Contratação de Pacotes;
+4 - A URA Cognitiva pede para aguardar enquanto verifica a internet;
+5 - A URA Cognitiva lista e oferece os pacotes disponíveis ao cliente;
+6 - URA informa que precisa da senha única;
+7 - URA informa o pacote foi contratado;
+8 - A URA Cognitiva agradece e encerra a ligação.</t>
   </si>
   <si>
     <t>45</t>
@@ -1423,14 +1423,14 @@
 Quer algo mais.</t>
   </si>
   <si>
-    <t>Chamada é encaminhada para a URA Cognitiva;
-Ouvir a saudacão da URA Cognitiva conforme descrito na DF.
-A URA Congnitiva informa que entendeu que deseja falar sobre Contratação de Pacotes;
-A URA Cognitiva pede para aguardar enquanto verifica a internet;
-A URA Cognitiva lista e oferece os pacotes disponíveis ao cliente;
-URA informa que precisa da senha única;
-URA informa o pacote não foi contratado;
-A URA Cognitiva transfere para o desambiguador.</t>
+    <t>1 - Chamada é encaminhada para a URA Cognitiva;
+2 - Ouvir a saudacão da URA Cognitiva conforme descrito na DF.
+3 - A URA Congnitiva informa que entendeu que deseja falar sobre Contratação de Pacotes;
+4 - A URA Cognitiva pede para aguardar enquanto verifica a internet;
+5 - A URA Cognitiva lista e oferece os pacotes disponíveis ao cliente;
+6 - URA informa que precisa da senha única;
+7 - URA informa o pacote não foi contratado;
+8 - A URA Cognitiva transfere para o desambiguador.</t>
   </si>
   <si>
     <t>46</t>
@@ -1455,14 +1455,14 @@
 Não quer mais nada.</t>
   </si>
   <si>
-    <t>Chamada é encaminhada para a URA Cognitiva;
-Ouvir a saudacão da URA Cognitiva conforme descrito na DF.
-A URA Congnitiva informa que entendeu que deseja falar sobre Contratação de Pacotes;
-A URA Cognitiva pede para aguardar enquanto verifica a internet;
-A URA Cognitiva lista e oferece os pacotes disponíveis ao cliente;
-URA informa que precisa da senha única;
-URA informa o pacote não foi contratado;
-A URA Cognitiva agradece e encerra a ligação.</t>
+    <t>1 - Chamada é encaminhada para a URA Cognitiva;
+2 - Ouvir a saudacão da URA Cognitiva conforme descrito na DF.
+3 - A URA Congnitiva informa que entendeu que deseja falar sobre Contratação de Pacotes;
+4 - A URA Cognitiva pede para aguardar enquanto verifica a internet;
+5 - A URA Cognitiva lista e oferece os pacotes disponíveis ao cliente;
+6 - URA informa que precisa da senha única;
+7 - URA informa o pacote não foi contratado;
+8 - A URA Cognitiva agradece e encerra a ligação.</t>
   </si>
   <si>
     <t>47</t>
@@ -1486,14 +1486,14 @@
 Quer algo mais.</t>
   </si>
   <si>
-    <t>Chamada é encaminhada para a URA Cognitiva;
-Ouvir a saudacão da URA Cognitiva conforme descrito na DF.
-A URA Congnitiva informa que entendeu que deseja falar sobre Contratação de Pacotes;
-A URA Cognitiva pede para aguardar enquanto verifica a internet;
-A URA Cognitiva lista e oferece os pacotes disponíveis ao cliente;
-URA informa que precisa da senha única;
-URA Informa que não foi possível confirmar os dados do cliente e não vai poder prosseguir;
-A URA Cognitiva transfere para o desambiguador.</t>
+    <t>1 - Chamada é encaminhada para a URA Cognitiva;
+2 - Ouvir a saudacão da URA Cognitiva conforme descrito na DF.
+3 - A URA Congnitiva informa que entendeu que deseja falar sobre Contratação de Pacotes;
+4 - A URA Cognitiva pede para aguardar enquanto verifica a internet;
+5 - A URA Cognitiva lista e oferece os pacotes disponíveis ao cliente;
+6 - URA informa que precisa da senha única;
+7 - URA Informa que não foi possível confirmar os dados do cliente e não vai poder prosseguir;
+8 - A URA Cognitiva transfere para o desambiguador.</t>
   </si>
   <si>
     <t>48</t>
@@ -1517,14 +1517,14 @@
 Não quer mais nada.</t>
   </si>
   <si>
-    <t>Chamada é encaminhada para a URA Cognitiva;
-Ouvir a saudacão da URA Cognitiva conforme descrito na DF.
-A URA Congnitiva informa que entendeu que deseja falar sobre Contratação de Pacotes;
-A URA Cognitiva pede para aguardar enquanto verifica a internet;
-A URA Cognitiva lista e oferece os pacotes disponíveis ao cliente;
-URA informa que precisa da senha única;
-URA Informa que não foi possível confirmar os dados do cliente e não vai poder prosseguir;
-A URA Cognitiva agradece e encerra a ligação.</t>
+    <t>1 - Chamada é encaminhada para a URA Cognitiva;
+2 - Ouvir a saudacão da URA Cognitiva conforme descrito na DF.
+3 - A URA Congnitiva informa que entendeu que deseja falar sobre Contratação de Pacotes;
+4 - A URA Cognitiva pede para aguardar enquanto verifica a internet;
+5 - A URA Cognitiva lista e oferece os pacotes disponíveis ao cliente;
+6 - URA informa que precisa da senha única;
+7 - URA Informa que não foi possível confirmar os dados do cliente e não vai poder prosseguir;
+8 - A URA Cognitiva agradece e encerra a ligação.</t>
   </si>
   <si>
     <t>49</t>
@@ -1548,13 +1548,13 @@
 Quer algo mais.</t>
   </si>
   <si>
-    <t>Chamada é encaminhada para a URA Cognitiva;
-Ouvir a saudacão da URA Cognitiva conforme descrito na DF.
-A URA Congnitiva informa que entendeu que deseja falar sobre Contratação de Pacotes;
-A URA Cognitiva pede para aguardar enquanto verifica a internet;
-A URA Cognitiva lista e oferece os pacotes disponíveis ao cliente;
-A URA Cognitiva informa que não efetuou a contratação;
-A URA Cognitiva transfere para o desambiguador.</t>
+    <t>1 - Chamada é encaminhada para a URA Cognitiva;
+2 - Ouvir a saudacão da URA Cognitiva conforme descrito na DF.
+3 - A URA Congnitiva informa que entendeu que deseja falar sobre Contratação de Pacotes;
+4 - A URA Cognitiva pede para aguardar enquanto verifica a internet;
+5 - A URA Cognitiva lista e oferece os pacotes disponíveis ao cliente;
+6 - A URA Cognitiva informa que não efetuou a contratação;
+7 - A URA Cognitiva transfere para o desambiguador.</t>
   </si>
   <si>
     <t>50</t>
@@ -1578,13 +1578,13 @@
 Não quer mais nada.</t>
   </si>
   <si>
-    <t>Chamada é encaminhada para a URA Cognitiva;
-Ouvir a saudacão da URA Cognitiva conforme descrito na DF.
-A URA Congnitiva informa que entendeu que deseja falar sobre Contratação de Pacotes;
-A URA Cognitiva pede para aguardar enquanto verifica a internet;
-A URA Cognitiva lista e oferece os pacotes disponíveis ao cliente;
-A URA Cognitiva informa que não efetuou a contratação;
-A URA Cognitiva agradece e encerra a ligação.</t>
+    <t>1 - Chamada é encaminhada para a URA Cognitiva;
+2 - Ouvir a saudacão da URA Cognitiva conforme descrito na DF.
+3 - A URA Congnitiva informa que entendeu que deseja falar sobre Contratação de Pacotes;
+4 - A URA Cognitiva pede para aguardar enquanto verifica a internet;
+5 - A URA Cognitiva lista e oferece os pacotes disponíveis ao cliente;
+6 - A URA Cognitiva informa que não efetuou a contratação;
+7 - A URA Cognitiva agradece e encerra a ligação.</t>
   </si>
   <si>
     <t>51</t>
@@ -1610,14 +1610,14 @@
 Quer algo mais.</t>
   </si>
   <si>
-    <t>Chamada é encaminhada para a URA Cognitiva;
-Ouvir a saudacão da URA Cognitiva conforme descrito na DF.
-A URA Congnitiva informa que entendeu que deseja falar sobre Contratação de Pacotes;
-A URA Cognitiva pede para aguardar enquanto verifica a internet;
-A URA Cognitiva lista e oferece os pacotes disponíveis ao cliente;
-A URA Cognitiva informa que no momento estas são as únicas opções disponíveis;
-URA informa o pacote foi contratado;
-A URA Cognitiva transfere para o desambiguador.</t>
+    <t>1 - Chamada é encaminhada para a URA Cognitiva;
+2 - Ouvir a saudacão da URA Cognitiva conforme descrito na DF.
+3 - A URA Congnitiva informa que entendeu que deseja falar sobre Contratação de Pacotes;
+4 - A URA Cognitiva pede para aguardar enquanto verifica a internet;
+5 - A URA Cognitiva lista e oferece os pacotes disponíveis ao cliente;
+6 - A URA Cognitiva informa que no momento estas são as únicas opções disponíveis;
+7 - URA informa o pacote foi contratado;
+8 - A URA Cognitiva transfere para o desambiguador.</t>
   </si>
   <si>
     <t>52</t>
@@ -1643,14 +1643,14 @@
 Não quer mais nada.</t>
   </si>
   <si>
-    <t>Chamada é encaminhada para a URA Cognitiva;
-Ouvir a saudacão da URA Cognitiva conforme descrito na DF.
-A URA Congnitiva informa que entendeu que deseja falar sobre Contratação de Pacotes;
-A URA Cognitiva pede para aguardar enquanto verifica a internet;
-A URA Cognitiva lista e oferece os pacotes disponíveis ao cliente;
-A URA Cognitiva informa que no momento estas são as únicas opções disponíveis;
-URA informa o pacote foi contratado;
-A URA Cognitiva agradece e encerra a ligação.</t>
+    <t>1 - Chamada é encaminhada para a URA Cognitiva;
+2 - Ouvir a saudacão da URA Cognitiva conforme descrito na DF.
+3 - A URA Congnitiva informa que entendeu que deseja falar sobre Contratação de Pacotes;
+4 - A URA Cognitiva pede para aguardar enquanto verifica a internet;
+5 - A URA Cognitiva lista e oferece os pacotes disponíveis ao cliente;
+6 - A URA Cognitiva informa que no momento estas são as únicas opções disponíveis;
+7 - URA informa o pacote foi contratado;
+8 - A URA Cognitiva agradece e encerra a ligação.</t>
   </si>
   <si>
     <t>53</t>
@@ -1676,14 +1676,14 @@
 Quer algo mais.</t>
   </si>
   <si>
-    <t>Chamada é encaminhada para a URA Cognitiva;
-Ouvir a saudacão da URA Cognitiva conforme descrito na DF.
-A URA Congnitiva informa que entendeu que deseja falar sobre Contratação de Pacotes;
-A URA Cognitiva pede para aguardar enquanto verifica a internet;
-A URA Cognitiva lista e oferece os pacotes disponíveis ao cliente;
-A URA Cognitiva informa que no momento estas são as únicas opções disponíveis;
-URA informa o pacote não foi contratado;
-A URA Cognitiva transfere para o desambiguador.</t>
+    <t>1 - Chamada é encaminhada para a URA Cognitiva;
+2 - Ouvir a saudacão da URA Cognitiva conforme descrito na DF.
+3 - A URA Congnitiva informa que entendeu que deseja falar sobre Contratação de Pacotes;
+4 - A URA Cognitiva pede para aguardar enquanto verifica a internet;
+5 - A URA Cognitiva lista e oferece os pacotes disponíveis ao cliente;
+6 - A URA Cognitiva informa que no momento estas são as únicas opções disponíveis;
+7 - URA informa o pacote não foi contratado;
+8 - A URA Cognitiva transfere para o desambiguador.</t>
   </si>
   <si>
     <t>54</t>
@@ -1709,14 +1709,14 @@
 Não quer mais nada.</t>
   </si>
   <si>
-    <t>Chamada é encaminhada para a URA Cognitiva;
-Ouvir a saudacão da URA Cognitiva conforme descrito na DF.
-A URA Congnitiva informa que entendeu que deseja falar sobre Contratação de Pacotes;
-A URA Cognitiva pede para aguardar enquanto verifica a internet;
-A URA Cognitiva lista e oferece os pacotes disponíveis ao cliente;
-A URA Cognitiva informa que no momento estas são as únicas opções disponíveis;
-URA informa o pacote não foi contratado;
-A URA Cognitiva agradece e encerra a ligação.</t>
+    <t>1 - Chamada é encaminhada para a URA Cognitiva;
+2 - Ouvir a saudacão da URA Cognitiva conforme descrito na DF.
+3 - A URA Congnitiva informa que entendeu que deseja falar sobre Contratação de Pacotes;
+4 - A URA Cognitiva pede para aguardar enquanto verifica a internet;
+5 - A URA Cognitiva lista e oferece os pacotes disponíveis ao cliente;
+6 - A URA Cognitiva informa que no momento estas são as únicas opções disponíveis;
+7 - URA informa o pacote não foi contratado;
+8 - A URA Cognitiva agradece e encerra a ligação.</t>
   </si>
   <si>
     <t>55</t>
@@ -1743,15 +1743,15 @@
 Quer algo mais.</t>
   </si>
   <si>
-    <t>Chamada é encaminhada para a URA Cognitiva;
-Ouvir a saudacão da URA Cognitiva conforme descrito na DF.
-A URA Congnitiva informa que entendeu que deseja falar sobre Contratação de Pacotes;
-A URA Cognitiva pede para aguardar enquanto verifica a internet;
-A URA Cognitiva lista e oferece os pacotes disponíveis ao cliente;
-A URA Cognitiva informa que no momento estas são as únicas opções disponíveis;
-URA informa que precisa da senha única;
-URA informa o pacote foi contratado;
-A URA Cognitiva transfere para o desambiguador.</t>
+    <t>1 - Chamada é encaminhada para a URA Cognitiva;
+2 - Ouvir a saudacão da URA Cognitiva conforme descrito na DF.
+3 - A URA Congnitiva informa que entendeu que deseja falar sobre Contratação de Pacotes;
+4 - A URA Cognitiva pede para aguardar enquanto verifica a internet;
+5 - A URA Cognitiva lista e oferece os pacotes disponíveis ao cliente;
+6 - A URA Cognitiva informa que no momento estas são as únicas opções disponíveis;
+7 - URA informa que precisa da senha única;
+8 - URA informa o pacote foi contratado;
+9 - A URA Cognitiva transfere para o desambiguador.</t>
   </si>
   <si>
     <t>56</t>
@@ -1778,15 +1778,15 @@
 Não quer mais nada.</t>
   </si>
   <si>
-    <t>Chamada é encaminhada para a URA Cognitiva;
-Ouvir a saudacão da URA Cognitiva conforme descrito na DF.
-A URA Congnitiva informa que entendeu que deseja falar sobre Contratação de Pacotes;
-A URA Cognitiva pede para aguardar enquanto verifica a internet;
-A URA Cognitiva lista e oferece os pacotes disponíveis ao cliente;
-A URA Cognitiva informa que no momento estas são as únicas opções disponíveis;
-URA informa que precisa da senha única;
-URA informa o pacote foi contratado;
-A URA Cognitiva agradece e encerra a ligação.</t>
+    <t>1 - Chamada é encaminhada para a URA Cognitiva;
+2 - Ouvir a saudacão da URA Cognitiva conforme descrito na DF.
+3 - A URA Congnitiva informa que entendeu que deseja falar sobre Contratação de Pacotes;
+4 - A URA Cognitiva pede para aguardar enquanto verifica a internet;
+5 - A URA Cognitiva lista e oferece os pacotes disponíveis ao cliente;
+6 - A URA Cognitiva informa que no momento estas são as únicas opções disponíveis;
+7 - URA informa que precisa da senha única;
+8 - URA informa o pacote foi contratado;
+9 - A URA Cognitiva agradece e encerra a ligação.</t>
   </si>
   <si>
     <t>57</t>
@@ -1813,15 +1813,15 @@
 Quer algo mais.</t>
   </si>
   <si>
-    <t>Chamada é encaminhada para a URA Cognitiva;
-Ouvir a saudacão da URA Cognitiva conforme descrito na DF.
-A URA Congnitiva informa que entendeu que deseja falar sobre Contratação de Pacotes;
-A URA Cognitiva pede para aguardar enquanto verifica a internet;
-A URA Cognitiva lista e oferece os pacotes disponíveis ao cliente;
-A URA Cognitiva informa que no momento estas são as únicas opções disponíveis;
-URA informa que precisa da senha única;
-URA informa o pacote não foi contratado;
-A URA Cognitiva transfere para o desambiguador.</t>
+    <t>1 - Chamada é encaminhada para a URA Cognitiva;
+2 - Ouvir a saudacão da URA Cognitiva conforme descrito na DF.
+3 - A URA Congnitiva informa que entendeu que deseja falar sobre Contratação de Pacotes;
+4 - A URA Cognitiva pede para aguardar enquanto verifica a internet;
+5 - A URA Cognitiva lista e oferece os pacotes disponíveis ao cliente;
+6 - A URA Cognitiva informa que no momento estas são as únicas opções disponíveis;
+7 - URA informa que precisa da senha única;
+8 - URA informa o pacote não foi contratado;
+9 - A URA Cognitiva transfere para o desambiguador.</t>
   </si>
   <si>
     <t>58</t>
@@ -1848,15 +1848,15 @@
 Não quer mais nada.</t>
   </si>
   <si>
-    <t>Chamada é encaminhada para a URA Cognitiva;
-Ouvir a saudacão da URA Cognitiva conforme descrito na DF.
-A URA Congnitiva informa que entendeu que deseja falar sobre Contratação de Pacotes;
-A URA Cognitiva pede para aguardar enquanto verifica a internet;
-A URA Cognitiva lista e oferece os pacotes disponíveis ao cliente;
-A URA Cognitiva informa que no momento estas são as únicas opções disponíveis;
-URA informa que precisa da senha única;
-URA informa o pacote não foi contratado;
-A URA Cognitiva agradece e encerra a ligação.</t>
+    <t>1 - Chamada é encaminhada para a URA Cognitiva;
+2 - Ouvir a saudacão da URA Cognitiva conforme descrito na DF.
+3 - A URA Congnitiva informa que entendeu que deseja falar sobre Contratação de Pacotes;
+4 - A URA Cognitiva pede para aguardar enquanto verifica a internet;
+5 - A URA Cognitiva lista e oferece os pacotes disponíveis ao cliente;
+6 - A URA Cognitiva informa que no momento estas são as únicas opções disponíveis;
+7 - URA informa que precisa da senha única;
+8 - URA informa o pacote não foi contratado;
+9 - A URA Cognitiva agradece e encerra a ligação.</t>
   </si>
   <si>
     <t>59</t>
@@ -1882,15 +1882,15 @@
 Quer algo mais.</t>
   </si>
   <si>
-    <t>Chamada é encaminhada para a URA Cognitiva;
-Ouvir a saudacão da URA Cognitiva conforme descrito na DF.
-A URA Congnitiva informa que entendeu que deseja falar sobre Contratação de Pacotes;
-A URA Cognitiva pede para aguardar enquanto verifica a internet;
-A URA Cognitiva lista e oferece os pacotes disponíveis ao cliente;
-A URA Cognitiva informa que no momento estas são as únicas opções disponíveis;
-URA informa que precisa da senha única;
-URA Informa que não foi possível confirmar os dados do cliente e não vai poder prosseguir;
-A URA Cognitiva transfere para o desambiguador.</t>
+    <t>1 - Chamada é encaminhada para a URA Cognitiva;
+2 - Ouvir a saudacão da URA Cognitiva conforme descrito na DF.
+3 - A URA Congnitiva informa que entendeu que deseja falar sobre Contratação de Pacotes;
+4 - A URA Cognitiva pede para aguardar enquanto verifica a internet;
+5 - A URA Cognitiva lista e oferece os pacotes disponíveis ao cliente;
+6 - A URA Cognitiva informa que no momento estas são as únicas opções disponíveis;
+7 - URA informa que precisa da senha única;
+8 - URA Informa que não foi possível confirmar os dados do cliente e não vai poder prosseguir;
+9 - A URA Cognitiva transfere para o desambiguador.</t>
   </si>
   <si>
     <t>60</t>
@@ -1916,15 +1916,15 @@
 Não quer mais nada.</t>
   </si>
   <si>
-    <t>Chamada é encaminhada para a URA Cognitiva;
-Ouvir a saudacão da URA Cognitiva conforme descrito na DF.
-A URA Congnitiva informa que entendeu que deseja falar sobre Contratação de Pacotes;
-A URA Cognitiva pede para aguardar enquanto verifica a internet;
-A URA Cognitiva lista e oferece os pacotes disponíveis ao cliente;
-A URA Cognitiva informa que no momento estas são as únicas opções disponíveis;
-URA informa que precisa da senha única;
-URA Informa que não foi possível confirmar os dados do cliente e não vai poder prosseguir;
-A URA Cognitiva agradece e encerra a ligação.</t>
+    <t>1 - Chamada é encaminhada para a URA Cognitiva;
+2 - Ouvir a saudacão da URA Cognitiva conforme descrito na DF.
+3 - A URA Congnitiva informa que entendeu que deseja falar sobre Contratação de Pacotes;
+4 - A URA Cognitiva pede para aguardar enquanto verifica a internet;
+5 - A URA Cognitiva lista e oferece os pacotes disponíveis ao cliente;
+6 - A URA Cognitiva informa que no momento estas são as únicas opções disponíveis;
+7 - URA informa que precisa da senha única;
+8 - URA Informa que não foi possível confirmar os dados do cliente e não vai poder prosseguir;
+9 - A URA Cognitiva agradece e encerra a ligação.</t>
   </si>
   <si>
     <t>61</t>
@@ -1950,14 +1950,14 @@
 Quer algo mais.</t>
   </si>
   <si>
-    <t>Chamada é encaminhada para a URA Cognitiva;
-Ouvir a saudacão da URA Cognitiva conforme descrito na DF.
-A URA Congnitiva informa que entendeu que deseja falar sobre Contratação de Pacotes;
-A URA Cognitiva pede para aguardar enquanto verifica a internet;
-A URA Cognitiva lista e oferece os pacotes disponíveis ao cliente;
-A URA Cognitiva informa que no momento estas são as únicas opções disponíveis;
-A URA Cognitiva informa que não efetuou a contratação;
-A URA Cognitiva transfere para o desambiguador.</t>
+    <t>1 - Chamada é encaminhada para a URA Cognitiva;
+2 - Ouvir a saudacão da URA Cognitiva conforme descrito na DF.
+3 - A URA Congnitiva informa que entendeu que deseja falar sobre Contratação de Pacotes;
+4 - A URA Cognitiva pede para aguardar enquanto verifica a internet;
+5 - A URA Cognitiva lista e oferece os pacotes disponíveis ao cliente;
+6 - A URA Cognitiva informa que no momento estas são as únicas opções disponíveis;
+7 - A URA Cognitiva informa que não efetuou a contratação;
+8 - A URA Cognitiva transfere para o desambiguador.</t>
   </si>
   <si>
     <t>62</t>
@@ -1983,14 +1983,14 @@
 Não quer mais nada.</t>
   </si>
   <si>
-    <t>Chamada é encaminhada para a URA Cognitiva;
-Ouvir a saudacão da URA Cognitiva conforme descrito na DF.
-A URA Congnitiva informa que entendeu que deseja falar sobre Contratação de Pacotes;
-A URA Cognitiva pede para aguardar enquanto verifica a internet;
-A URA Cognitiva lista e oferece os pacotes disponíveis ao cliente;
-A URA Cognitiva informa que no momento estas são as únicas opções disponíveis;
-A URA Cognitiva informa que não efetuou a contratação;
-A URA Cognitiva agradece e encerra a ligação.</t>
+    <t>1 - Chamada é encaminhada para a URA Cognitiva;
+2 - Ouvir a saudacão da URA Cognitiva conforme descrito na DF.
+3 - A URA Congnitiva informa que entendeu que deseja falar sobre Contratação de Pacotes;
+4 - A URA Cognitiva pede para aguardar enquanto verifica a internet;
+5 - A URA Cognitiva lista e oferece os pacotes disponíveis ao cliente;
+6 - A URA Cognitiva informa que no momento estas são as únicas opções disponíveis;
+7 - A URA Cognitiva informa que não efetuou a contratação;
+8 - A URA Cognitiva agradece e encerra a ligação.</t>
   </si>
   <si>
     <t>63</t>
@@ -2013,13 +2013,13 @@
 Quer algo mais.</t>
   </si>
   <si>
-    <t>Chamada é encaminhada para a URA Cognitiva;
-Ouvir a saudacão da URA Cognitiva conforme descrito na DF.
-A URA Congnitiva informa que entendeu que deseja falar sobre Contratação de Pacotes;
-A URA Cognitiva pede para aguardar enquanto verifica a internet;
-A URA Cognitiva lista e oferece os pacotes disponíveis ao cliente;
-A URA Cognitiva informa que no momento estas são as únicas opções disponíveis;
-A URA Cognitiva transfere para o desambiguador.</t>
+    <t>1 - Chamada é encaminhada para a URA Cognitiva;
+2 - Ouvir a saudacão da URA Cognitiva conforme descrito na DF.
+3 - A URA Congnitiva informa que entendeu que deseja falar sobre Contratação de Pacotes;
+4 - A URA Cognitiva pede para aguardar enquanto verifica a internet;
+5 - A URA Cognitiva lista e oferece os pacotes disponíveis ao cliente;
+6 - A URA Cognitiva informa que no momento estas são as únicas opções disponíveis;
+7 - A URA Cognitiva transfere para o desambiguador.</t>
   </si>
   <si>
     <t>64</t>
@@ -2042,13 +2042,13 @@
 Não quer mais nada.</t>
   </si>
   <si>
-    <t>Chamada é encaminhada para a URA Cognitiva;
-Ouvir a saudacão da URA Cognitiva conforme descrito na DF.
-A URA Congnitiva informa que entendeu que deseja falar sobre Contratação de Pacotes;
-A URA Cognitiva pede para aguardar enquanto verifica a internet;
-A URA Cognitiva lista e oferece os pacotes disponíveis ao cliente;
-A URA Cognitiva informa que no momento estas são as únicas opções disponíveis;
-A URA Cognitiva agradece e encerra a ligação.</t>
+    <t>1 - Chamada é encaminhada para a URA Cognitiva;
+2 - Ouvir a saudacão da URA Cognitiva conforme descrito na DF.
+3 - A URA Congnitiva informa que entendeu que deseja falar sobre Contratação de Pacotes;
+4 - A URA Cognitiva pede para aguardar enquanto verifica a internet;
+5 - A URA Cognitiva lista e oferece os pacotes disponíveis ao cliente;
+6 - A URA Cognitiva informa que no momento estas são as únicas opções disponíveis;
+7 - A URA Cognitiva agradece e encerra a ligação.</t>
   </si>
   <si>
     <t>65</t>
@@ -2106,13 +2106,13 @@
 Quer algo mais.</t>
   </si>
   <si>
-    <t>Chamada é encaminhada para a URA Cognitiva;
-Ouvir a saudacão da URA Cognitiva conforme descrito na DF.
-A URA Congnitiva informa que entendeu que deseja falar sobre Contratação de Pacotes;
-A URA Cognitiva pede para aguardar enquanto verifica a internet;
-A URA Cognitiva informa que o pacote de dados foi consumido e,
+    <t>1 - Chamada é encaminhada para a URA Cognitiva;
+2 - Ouvir a saudacão da URA Cognitiva conforme descrito na DF.
+3 - A URA Congnitiva informa que entendeu que deseja falar sobre Contratação de Pacotes;
+4 - A URA Cognitiva pede para aguardar enquanto verifica a internet;
+5 - A URA Cognitiva informa que o pacote de dados foi consumido e,
 que por não ser o titular, não poderá contratar um novo pacote;
-A URA Cognitiva transfere para o desambiguador.</t>
+6 - A URA Cognitiva transfere para o desambiguador.</t>
   </si>
   <si>
     <t>68</t>
@@ -2130,13 +2130,13 @@
 Não quer mais nada.</t>
   </si>
   <si>
-    <t>Chamada é encaminhada para a URA Cognitiva;
-Ouvir a saudacão da URA Cognitiva conforme descrito na DF.
-A URA Congnitiva informa que entendeu que deseja falar sobre Contratação de Pacotes;
-A URA Cognitiva pede para aguardar enquanto verifica a internet;
-A URA Cognitiva informa que o pacote de dados foi consumido e,
+    <t>1 - Chamada é encaminhada para a URA Cognitiva;
+2 - Ouvir a saudacão da URA Cognitiva conforme descrito na DF.
+3 - A URA Congnitiva informa que entendeu que deseja falar sobre Contratação de Pacotes;
+4 - A URA Cognitiva pede para aguardar enquanto verifica a internet;
+5 - A URA Cognitiva informa que o pacote de dados foi consumido e,
 que por não ser o titular, não poderá contratar um novo pacote;
-A URA Cognitiva agradece e encerra a ligação.</t>
+6 - A URA Cognitiva agradece e encerra a ligação.</t>
   </si>
   <si>
     <t>69</t>
@@ -3511,16 +3511,16 @@
 Quer algo mais.</t>
   </si>
   <si>
-    <t>Chamada é encaminhada para a URA Cognitiva;
-Ouvir a saudacão da URA Cognitiva conforme descrito na DF.
-A URA Congnitiva informa que entendeu que deseja falar sobre Contratação de Pacotes;
-A URA Cognitiva pede para aguardar enquanto verifica a internet;
-A URA Cognitiva informa que já existe um pacote ativo e que só é possível contratar
+    <t>1 - Chamada é encaminhada para a URA Cognitiva;
+2 - Ouvir a saudacão da URA Cognitiva conforme descrito na DF.
+3 - A URA Congnitiva informa que entendeu que deseja falar sobre Contratação de Pacotes;
+4 - A URA Cognitiva pede para aguardar enquanto verifica a internet;
+5 - A URA Cognitiva informa que já existe um pacote ativo e que só é possível contratar
 um novo depois de consumi-lo;
-A URA Cognitiva informa que está com velocidade reduzida porque já consumiu o pacote,
+6 - A URA Cognitiva informa que está com velocidade reduzida porque já consumiu o pacote,
 mas pode contratar um pacote adicional e verifica se existem pacotes disponiveis;
-A URA Cognitiva informa que não existem pacotes disponiveis no momento;
-A URA Cognitiva transfere para o desambiguador.</t>
+7 - A URA Cognitiva informa que não existem pacotes disponiveis no momento;
+8 - A URA Cognitiva transfere para o desambiguador.</t>
   </si>
   <si>
     <t>134</t>
@@ -3537,16 +3537,16 @@
 Não quer mais nada.</t>
   </si>
   <si>
-    <t>Chamada é encaminhada para a URA Cognitiva;
-Ouvir a saudacão da URA Cognitiva conforme descrito na DF.
-A URA Congnitiva informa que entendeu que deseja falar sobre Contratação de Pacotes;
-A URA Cognitiva pede para aguardar enquanto verifica a internet;
-A URA Cognitiva informa que já existe um pacote ativo e que só é possível contratar
+    <t>1 - Chamada é encaminhada para a URA Cognitiva;
+2 - Ouvir a saudacão da URA Cognitiva conforme descrito na DF.
+3 - A URA Congnitiva informa que entendeu que deseja falar sobre Contratação de Pacotes;
+4 - A URA Cognitiva pede para aguardar enquanto verifica a internet;
+5 - A URA Cognitiva informa que já existe um pacote ativo e que só é possível contratar
 um novo depois de consumi-lo;
-A URA Cognitiva informa que está com velocidade reduzida porque já consumiu o pacote,
+6 - A URA Cognitiva informa que está com velocidade reduzida porque já consumiu o pacote,
 mas pode contratar um pacote adicional e verifica se existem pacotes disponiveis;
-A URA Cognitiva informa que não existem pacotes disponiveis no momento;
-A URA Cognitiva agradece e encerra a ligação.</t>
+7 - A URA Cognitiva informa que não existem pacotes disponiveis no momento;
+8 - A URA Cognitiva agradece e encerra a ligação.</t>
   </si>
   <si>
     <t>135</t>
@@ -3567,17 +3567,17 @@
 Quer algo mais.</t>
   </si>
   <si>
-    <t>Chamada é encaminhada para a URA Cognitiva;
-Ouvir a saudacão da URA Cognitiva conforme descrito na DF.
-A URA Congnitiva informa que entendeu que deseja falar sobre Contratação de Pacotes;
-A URA Cognitiva pede para aguardar enquanto verifica a internet;
-A URA Cognitiva informa que já existe um pacote ativo e que só é possível contratar
+    <t>1 - Chamada é encaminhada para a URA Cognitiva;
+2 - Ouvir a saudacão da URA Cognitiva conforme descrito na DF.
+3 - A URA Congnitiva informa que entendeu que deseja falar sobre Contratação de Pacotes;
+4 - A URA Cognitiva pede para aguardar enquanto verifica a internet;
+5 - A URA Cognitiva informa que já existe um pacote ativo e que só é possível contratar
 um novo depois de consumi-lo;
-A URA Cognitiva informa que está com velocidade reduzida porque já consumiu o pacote,
+6 - A URA Cognitiva informa que está com velocidade reduzida porque já consumiu o pacote,
 mas pode contratar um pacote adicional e verifica se existem pacotes disponiveis;
-A URA Cognitiva lista e oferece os pacotes disponíveis ao cliente;
-URA informa o pacote foi contratado;
-A URA Cognitiva transfere para o desambiguador.</t>
+7 - A URA Cognitiva lista e oferece os pacotes disponíveis ao cliente;
+8 - URA informa o pacote foi contratado;
+9 - A URA Cognitiva transfere para o desambiguador.</t>
   </si>
   <si>
     <t>136</t>
@@ -3598,17 +3598,17 @@
 Não quer mais nada.</t>
   </si>
   <si>
-    <t>Chamada é encaminhada para a URA Cognitiva;
-Ouvir a saudacão da URA Cognitiva conforme descrito na DF.
-A URA Congnitiva informa que entendeu que deseja falar sobre Contratação de Pacotes;
-A URA Cognitiva pede para aguardar enquanto verifica a internet;
-A URA Cognitiva informa que já existe um pacote ativo e que só é possível contratar
+    <t>1 - Chamada é encaminhada para a URA Cognitiva;
+2 - Ouvir a saudacão da URA Cognitiva conforme descrito na DF.
+3 - A URA Congnitiva informa que entendeu que deseja falar sobre Contratação de Pacotes;
+4 - A URA Cognitiva pede para aguardar enquanto verifica a internet;
+5 - A URA Cognitiva informa que já existe um pacote ativo e que só é possível contratar
 um novo depois de consumi-lo;
-A URA Cognitiva informa que está com velocidade reduzida porque já consumiu o pacote,
+6 - A URA Cognitiva informa que está com velocidade reduzida porque já consumiu o pacote,
 mas pode contratar um pacote adicional e verifica se existem pacotes disponiveis;
-A URA Cognitiva lista e oferece os pacotes disponíveis ao cliente;
-URA informa o pacote foi contratado;
-A URA Cognitiva agradece e encerra a ligação.</t>
+7 - A URA Cognitiva lista e oferece os pacotes disponíveis ao cliente;
+8 - URA informa o pacote foi contratado;
+9 - A URA Cognitiva agradece e encerra a ligação.</t>
   </si>
   <si>
     <t>137</t>
@@ -3629,17 +3629,17 @@
 Quer algo mais.</t>
   </si>
   <si>
-    <t>Chamada é encaminhada para a URA Cognitiva;
-Ouvir a saudacão da URA Cognitiva conforme descrito na DF.
-A URA Congnitiva informa que entendeu que deseja falar sobre Contratação de Pacotes;
-A URA Cognitiva pede para aguardar enquanto verifica a internet;
-A URA Cognitiva informa que já existe um pacote ativo e que só é possível contratar
+    <t>1 - Chamada é encaminhada para a URA Cognitiva;
+2 - Ouvir a saudacão da URA Cognitiva conforme descrito na DF.
+3 - A URA Congnitiva informa que entendeu que deseja falar sobre Contratação de Pacotes;
+4 - A URA Cognitiva pede para aguardar enquanto verifica a internet;
+5 - A URA Cognitiva informa que já existe um pacote ativo e que só é possível contratar
 um novo depois de consumi-lo;
-A URA Cognitiva informa que está com velocidade reduzida porque já consumiu o pacote,
+6 - A URA Cognitiva informa que está com velocidade reduzida porque já consumiu o pacote,
 mas pode contratar um pacote adicional e verifica se existem pacotes disponiveis;
-A URA Cognitiva lista e oferece os pacotes disponíveis ao cliente;
-URA informa o pacote não foi contratado;
-A URA Cognitiva transfere para o desambiguador.</t>
+7 - A URA Cognitiva lista e oferece os pacotes disponíveis ao cliente;
+8 - URA informa o pacote não foi contratado;
+9 - A URA Cognitiva transfere para o desambiguador.</t>
   </si>
   <si>
     <t>138</t>
@@ -3660,17 +3660,17 @@
 Não quer mais nada.</t>
   </si>
   <si>
-    <t>Chamada é encaminhada para a URA Cognitiva;
-Ouvir a saudacão da URA Cognitiva conforme descrito na DF.
-A URA Congnitiva informa que entendeu que deseja falar sobre Contratação de Pacotes;
-A URA Cognitiva pede para aguardar enquanto verifica a internet;
-A URA Cognitiva informa que já existe um pacote ativo e que só é possível contratar
+    <t>1 - Chamada é encaminhada para a URA Cognitiva;
+2 - Ouvir a saudacão da URA Cognitiva conforme descrito na DF.
+3 - A URA Congnitiva informa que entendeu que deseja falar sobre Contratação de Pacotes;
+4 - A URA Cognitiva pede para aguardar enquanto verifica a internet;
+5 - A URA Cognitiva informa que já existe um pacote ativo e que só é possível contratar
 um novo depois de consumi-lo;
-A URA Cognitiva informa que está com velocidade reduzida porque já consumiu o pacote,
+6 - A URA Cognitiva informa que está com velocidade reduzida porque já consumiu o pacote,
 mas pode contratar um pacote adicional e verifica se existem pacotes disponiveis;
-A URA Cognitiva lista e oferece os pacotes disponíveis ao cliente;
-URA informa o pacote não foi contratado;
-A URA Cognitiva agradece e encerra a ligação.</t>
+7 - A URA Cognitiva lista e oferece os pacotes disponíveis ao cliente;
+8 - URA informa o pacote não foi contratado;
+9 - A URA Cognitiva agradece e encerra a ligação.</t>
   </si>
   <si>
     <t>139</t>
@@ -3692,18 +3692,18 @@
 Quer algo mais.</t>
   </si>
   <si>
-    <t>Chamada é encaminhada para a URA Cognitiva;
-Ouvir a saudacão da URA Cognitiva conforme descrito na DF.
-A URA Congnitiva informa que entendeu que deseja falar sobre Contratação de Pacotes;
-A URA Cognitiva pede para aguardar enquanto verifica a internet;
-A URA Cognitiva informa que já existe um pacote ativo e que só é possível contratar
+    <t>1 - Chamada é encaminhada para a URA Cognitiva;
+2 - Ouvir a saudacão da URA Cognitiva conforme descrito na DF.
+3 - A URA Congnitiva informa que entendeu que deseja falar sobre Contratação de Pacotes;
+4 - A URA Cognitiva pede para aguardar enquanto verifica a internet;
+5 - A URA Cognitiva informa que já existe um pacote ativo e que só é possível contratar
 um novo depois de consumi-lo;
-A URA Cognitiva informa que está com velocidade reduzida porque já consumiu o pacote,
+6 - A URA Cognitiva informa que está com velocidade reduzida porque já consumiu o pacote,
 mas pode contratar um pacote adicional e verifica se existem pacotes disponiveis;
-A URA Cognitiva lista e oferece os pacotes disponíveis ao cliente;
-URA informa que precisa da senha única;
-URA informa o pacote foi contratado;
-A URA Cognitiva transfere para o desambiguador.</t>
+7 - A URA Cognitiva lista e oferece os pacotes disponíveis ao cliente;
+8 - URA informa que precisa da senha única;
+9 - URA informa o pacote foi contratado;
+10 - A URA Cognitiva transfere para o desambiguador.</t>
   </si>
   <si>
     <t>140</t>
@@ -3725,18 +3725,18 @@
 Não quer mais nada.</t>
   </si>
   <si>
-    <t>Chamada é encaminhada para a URA Cognitiva;
-Ouvir a saudacão da URA Cognitiva conforme descrito na DF.
-A URA Congnitiva informa que entendeu que deseja falar sobre Contratação de Pacotes;
-A URA Cognitiva pede para aguardar enquanto verifica a internet;
-A URA Cognitiva informa que já existe um pacote ativo e que só é possível contratar
+    <t>1 - Chamada é encaminhada para a URA Cognitiva;
+2 - Ouvir a saudacão da URA Cognitiva conforme descrito na DF.
+3 - A URA Congnitiva informa que entendeu que deseja falar sobre Contratação de Pacotes;
+4 - A URA Cognitiva pede para aguardar enquanto verifica a internet;
+5 - A URA Cognitiva informa que já existe um pacote ativo e que só é possível contratar
 um novo depois de consumi-lo;
-A URA Cognitiva informa que está com velocidade reduzida porque já consumiu o pacote,
+6 - A URA Cognitiva informa que está com velocidade reduzida porque já consumiu o pacote,
 mas pode contratar um pacote adicional e verifica se existem pacotes disponiveis;
-A URA Cognitiva lista e oferece os pacotes disponíveis ao cliente;
-URA informa que precisa da senha única;
-URA informa o pacote foi contratado;
-A URA Cognitiva agradece e encerra a ligação.</t>
+7 - A URA Cognitiva lista e oferece os pacotes disponíveis ao cliente;
+8 - URA informa que precisa da senha única;
+9 - URA informa o pacote foi contratado;
+10 - A URA Cognitiva agradece e encerra a ligação.</t>
   </si>
   <si>
     <t>141</t>
@@ -3758,18 +3758,18 @@
 Quer algo mais.</t>
   </si>
   <si>
-    <t>Chamada é encaminhada para a URA Cognitiva;
-Ouvir a saudacão da URA Cognitiva conforme descrito na DF.
-A URA Congnitiva informa que entendeu que deseja falar sobre Contratação de Pacotes;
-A URA Cognitiva pede para aguardar enquanto verifica a internet;
-A URA Cognitiva informa que já existe um pacote ativo e que só é possível contratar
+    <t>1 - Chamada é encaminhada para a URA Cognitiva;
+2 - Ouvir a saudacão da URA Cognitiva conforme descrito na DF.
+3 - A URA Congnitiva informa que entendeu que deseja falar sobre Contratação de Pacotes;
+4 - A URA Cognitiva pede para aguardar enquanto verifica a internet;
+5 - A URA Cognitiva informa que já existe um pacote ativo e que só é possível contratar
 um novo depois de consumi-lo;
-A URA Cognitiva informa que está com velocidade reduzida porque já consumiu o pacote,
+6 - A URA Cognitiva informa que está com velocidade reduzida porque já consumiu o pacote,
 mas pode contratar um pacote adicional e verifica se existem pacotes disponiveis;
-A URA Cognitiva lista e oferece os pacotes disponíveis ao cliente;
-URA informa que precisa da senha única;
-URA informa o pacote não foi contratado;
-A URA Cognitiva transfere para o desambiguador.</t>
+7 - A URA Cognitiva lista e oferece os pacotes disponíveis ao cliente;
+8 - URA informa que precisa da senha única;
+9 - URA informa o pacote não foi contratado;
+10 - A URA Cognitiva transfere para o desambiguador.</t>
   </si>
   <si>
     <t>142</t>
@@ -3791,18 +3791,18 @@
 Não quer mais nada.</t>
   </si>
   <si>
-    <t>Chamada é encaminhada para a URA Cognitiva;
-Ouvir a saudacão da URA Cognitiva conforme descrito na DF.
-A URA Congnitiva informa que entendeu que deseja falar sobre Contratação de Pacotes;
-A URA Cognitiva pede para aguardar enquanto verifica a internet;
-A URA Cognitiva informa que já existe um pacote ativo e que só é possível contratar
+    <t>1 - Chamada é encaminhada para a URA Cognitiva;
+2 - Ouvir a saudacão da URA Cognitiva conforme descrito na DF.
+3 - A URA Congnitiva informa que entendeu que deseja falar sobre Contratação de Pacotes;
+4 - A URA Cognitiva pede para aguardar enquanto verifica a internet;
+5 - A URA Cognitiva informa que já existe um pacote ativo e que só é possível contratar
 um novo depois de consumi-lo;
-A URA Cognitiva informa que está com velocidade reduzida porque já consumiu o pacote,
+6 - A URA Cognitiva informa que está com velocidade reduzida porque já consumiu o pacote,
 mas pode contratar um pacote adicional e verifica se existem pacotes disponiveis;
-A URA Cognitiva lista e oferece os pacotes disponíveis ao cliente;
-URA informa que precisa da senha única;
-URA informa o pacote não foi contratado;
-A URA Cognitiva agradece e encerra a ligação.</t>
+7 - A URA Cognitiva lista e oferece os pacotes disponíveis ao cliente;
+8 - URA informa que precisa da senha única;
+9 - URA informa o pacote não foi contratado;
+10 - A URA Cognitiva agradece e encerra a ligação.</t>
   </si>
   <si>
     <t>143</t>
@@ -3823,18 +3823,18 @@
 Quer algo mais.</t>
   </si>
   <si>
-    <t>Chamada é encaminhada para a URA Cognitiva;
-Ouvir a saudacão da URA Cognitiva conforme descrito na DF.
-A URA Congnitiva informa que entendeu que deseja falar sobre Contratação de Pacotes;
-A URA Cognitiva pede para aguardar enquanto verifica a internet;
-A URA Cognitiva informa que já existe um pacote ativo e que só é possível contratar
+    <t>1 - Chamada é encaminhada para a URA Cognitiva;
+2 - Ouvir a saudacão da URA Cognitiva conforme descrito na DF.
+3 - A URA Congnitiva informa que entendeu que deseja falar sobre Contratação de Pacotes;
+4 - A URA Cognitiva pede para aguardar enquanto verifica a internet;
+5 - A URA Cognitiva informa que já existe um pacote ativo e que só é possível contratar
 um novo depois de consumi-lo;
-A URA Cognitiva informa que está com velocidade reduzida porque já consumiu o pacote,
+6 - A URA Cognitiva informa que está com velocidade reduzida porque já consumiu o pacote,
 mas pode contratar um pacote adicional e verifica se existem pacotes disponiveis;
-A URA Cognitiva lista e oferece os pacotes disponíveis ao cliente;
-URA informa que precisa da senha única;
-URA Informa que não foi possível confirmar os dados do cliente e não vai poder prosseguir;
-A URA Cognitiva transfere para o desambiguador.</t>
+7 - A URA Cognitiva lista e oferece os pacotes disponíveis ao cliente;
+8 - URA informa que precisa da senha única;
+9 - URA Informa que não foi possível confirmar os dados do cliente e não vai poder prosseguir;
+10 - A URA Cognitiva transfere para o desambiguador.</t>
   </si>
   <si>
     <t>144</t>
@@ -3855,18 +3855,18 @@
 Não quer mais nada.</t>
   </si>
   <si>
-    <t>Chamada é encaminhada para a URA Cognitiva;
-Ouvir a saudacão da URA Cognitiva conforme descrito na DF.
-A URA Congnitiva informa que entendeu que deseja falar sobre Contratação de Pacotes;
-A URA Cognitiva pede para aguardar enquanto verifica a internet;
-A URA Cognitiva informa que já existe um pacote ativo e que só é possível contratar
+    <t>1 - Chamada é encaminhada para a URA Cognitiva;
+2 - Ouvir a saudacão da URA Cognitiva conforme descrito na DF.
+3 - A URA Congnitiva informa que entendeu que deseja falar sobre Contratação de Pacotes;
+4 - A URA Cognitiva pede para aguardar enquanto verifica a internet;
+5 - A URA Cognitiva informa que já existe um pacote ativo e que só é possível contratar
 um novo depois de consumi-lo;
-A URA Cognitiva informa que está com velocidade reduzida porque já consumiu o pacote,
+6 - A URA Cognitiva informa que está com velocidade reduzida porque já consumiu o pacote,
 mas pode contratar um pacote adicional e verifica se existem pacotes disponiveis;
-A URA Cognitiva lista e oferece os pacotes disponíveis ao cliente;
-URA informa que precisa da senha única;
-URA Informa que não foi possível confirmar os dados do cliente e não vai poder prosseguir;
-A URA Cognitiva agradece e encerra a ligação.</t>
+7 - A URA Cognitiva lista e oferece os pacotes disponíveis ao cliente;
+8 - URA informa que precisa da senha única;
+9 - URA Informa que não foi possível confirmar os dados do cliente e não vai poder prosseguir;
+10 - A URA Cognitiva agradece e encerra a ligação.</t>
   </si>
   <si>
     <t>145</t>
@@ -3887,17 +3887,17 @@
 Quer algo mais.</t>
   </si>
   <si>
-    <t>Chamada é encaminhada para a URA Cognitiva;
-Ouvir a saudacão da URA Cognitiva conforme descrito na DF.
-A URA Congnitiva informa que entendeu que deseja falar sobre Contratação de Pacotes;
-A URA Cognitiva pede para aguardar enquanto verifica a internet;
-A URA Cognitiva informa que já existe um pacote ativo e que só é possível contratar
+    <t>1 - Chamada é encaminhada para a URA Cognitiva;
+2 - Ouvir a saudacão da URA Cognitiva conforme descrito na DF.
+3 - A URA Congnitiva informa que entendeu que deseja falar sobre Contratação de Pacotes;
+4 - A URA Cognitiva pede para aguardar enquanto verifica a internet;
+5 - A URA Cognitiva informa que já existe um pacote ativo e que só é possível contratar
 um novo depois de consumi-lo;
-A URA Cognitiva informa que está com velocidade reduzida porque já consumiu o pacote,
+6 - A URA Cognitiva informa que está com velocidade reduzida porque já consumiu o pacote,
 mas pode contratar um pacote adicional e verifica se existem pacotes disponiveis;
-A URA Cognitiva lista e oferece os pacotes disponíveis ao cliente;
-A URA Cognitiva informa que não efetuou a contratação;
-A URA Cognitiva transfere para o desambiguador.</t>
+7 - A URA Cognitiva lista e oferece os pacotes disponíveis ao cliente;
+8 - A URA Cognitiva informa que não efetuou a contratação;
+9 - A URA Cognitiva transfere para o desambiguador.</t>
   </si>
   <si>
     <t>146</t>
@@ -3918,17 +3918,17 @@
 Não quer mais nada.</t>
   </si>
   <si>
-    <t>Chamada é encaminhada para a URA Cognitiva;
-Ouvir a saudacão da URA Cognitiva conforme descrito na DF.
-A URA Congnitiva informa que entendeu que deseja falar sobre Contratação de Pacotes;
-A URA Cognitiva pede para aguardar enquanto verifica a internet;
-A URA Cognitiva informa que já existe um pacote ativo e que só é possível contratar
+    <t>1 - Chamada é encaminhada para a URA Cognitiva;
+2 - Ouvir a saudacão da URA Cognitiva conforme descrito na DF.
+3 - A URA Congnitiva informa que entendeu que deseja falar sobre Contratação de Pacotes;
+4 - A URA Cognitiva pede para aguardar enquanto verifica a internet;
+5 - A URA Cognitiva informa que já existe um pacote ativo e que só é possível contratar
 um novo depois de consumi-lo;
-A URA Cognitiva informa que está com velocidade reduzida porque já consumiu o pacote,
+6 - A URA Cognitiva informa que está com velocidade reduzida porque já consumiu o pacote,
 mas pode contratar um pacote adicional e verifica se existem pacotes disponiveis;
-A URA Cognitiva lista e oferece os pacotes disponíveis ao cliente;
-A URA Cognitiva informa que não efetuou a contratação;
-A URA Cognitiva agradece e encerra a ligação.</t>
+7 - A URA Cognitiva lista e oferece os pacotes disponíveis ao cliente;
+8 - A URA Cognitiva informa que não efetuou a contratação;
+9 - A URA Cognitiva agradece e encerra a ligação.</t>
   </si>
   <si>
     <t>147</t>
@@ -3951,18 +3951,18 @@
 Quer algo mais.</t>
   </si>
   <si>
-    <t>Chamada é encaminhada para a URA Cognitiva;
-Ouvir a saudacão da URA Cognitiva conforme descrito na DF.
-A URA Congnitiva informa que entendeu que deseja falar sobre Contratação de Pacotes;
-A URA Cognitiva pede para aguardar enquanto verifica a internet;
-A URA Cognitiva informa que já existe um pacote ativo e que só é possível contratar
+    <t>1 - Chamada é encaminhada para a URA Cognitiva;
+2 - Ouvir a saudacão da URA Cognitiva conforme descrito na DF.
+3 - A URA Congnitiva informa que entendeu que deseja falar sobre Contratação de Pacotes;
+4 - A URA Cognitiva pede para aguardar enquanto verifica a internet;
+5 - A URA Cognitiva informa que já existe um pacote ativo e que só é possível contratar
 um novo depois de consumi-lo;
-A URA Cognitiva informa que está com velocidade reduzida porque já consumiu o pacote,
+6 - A URA Cognitiva informa que está com velocidade reduzida porque já consumiu o pacote,
 mas pode contratar um pacote adicional e verifica se existem pacotes disponiveis;
-A URA Cognitiva lista e oferece os pacotes disponíveis ao cliente;
-A URA Cognitiva informa que no momento estas são as únicas opções disponíveis;
-URA informa o pacote foi contratado;
-A URA Cognitiva transfere para o desambiguador.</t>
+7 - A URA Cognitiva lista e oferece os pacotes disponíveis ao cliente;
+8 - A URA Cognitiva informa que no momento estas são as únicas opções disponíveis;
+9 - URA informa o pacote foi contratado;
+10 - A URA Cognitiva transfere para o desambiguador.</t>
   </si>
   <si>
     <t>148</t>
@@ -3985,18 +3985,18 @@
 Não quer mais nada.</t>
   </si>
   <si>
-    <t>Chamada é encaminhada para a URA Cognitiva;
-Ouvir a saudacão da URA Cognitiva conforme descrito na DF.
-A URA Congnitiva informa que entendeu que deseja falar sobre Contratação de Pacotes;
-A URA Cognitiva pede para aguardar enquanto verifica a internet;
-A URA Cognitiva informa que já existe um pacote ativo e que só é possível contratar
+    <t>1 - Chamada é encaminhada para a URA Cognitiva;
+2 - Ouvir a saudacão da URA Cognitiva conforme descrito na DF.
+3 - A URA Congnitiva informa que entendeu que deseja falar sobre Contratação de Pacotes;
+4 - A URA Cognitiva pede para aguardar enquanto verifica a internet;
+5 - A URA Cognitiva informa que já existe um pacote ativo e que só é possível contratar
 um novo depois de consumi-lo;
-A URA Cognitiva informa que está com velocidade reduzida porque já consumiu o pacote,
+6 - A URA Cognitiva informa que está com velocidade reduzida porque já consumiu o pacote,
 mas pode contratar um pacote adicional e verifica se existem pacotes disponiveis;
-A URA Cognitiva lista e oferece os pacotes disponíveis ao cliente;
-A URA Cognitiva informa que no momento estas são as únicas opções disponíveis;
-URA informa o pacote foi contratado;
-A URA Cognitiva agradece e encerra a ligação.</t>
+7 - A URA Cognitiva lista e oferece os pacotes disponíveis ao cliente;
+8 - A URA Cognitiva informa que no momento estas são as únicas opções disponíveis;
+9 - URA informa o pacote foi contratado;
+10 - A URA Cognitiva agradece e encerra a ligação.</t>
   </si>
   <si>
     <t>149</t>
@@ -4019,18 +4019,18 @@
 Quer algo mais.</t>
   </si>
   <si>
-    <t>Chamada é encaminhada para a URA Cognitiva;
-Ouvir a saudacão da URA Cognitiva conforme descrito na DF.
-A URA Congnitiva informa que entendeu que deseja falar sobre Contratação de Pacotes;
-A URA Cognitiva pede para aguardar enquanto verifica a internet;
-A URA Cognitiva informa que já existe um pacote ativo e que só é possível contratar
+    <t>1 - Chamada é encaminhada para a URA Cognitiva;
+2 - Ouvir a saudacão da URA Cognitiva conforme descrito na DF.
+3 - A URA Congnitiva informa que entendeu que deseja falar sobre Contratação de Pacotes;
+4 - A URA Cognitiva pede para aguardar enquanto verifica a internet;
+5 - A URA Cognitiva informa que já existe um pacote ativo e que só é possível contratar
 um novo depois de consumi-lo;
-A URA Cognitiva informa que está com velocidade reduzida porque já consumiu o pacote,
+6 - A URA Cognitiva informa que está com velocidade reduzida porque já consumiu o pacote,
 mas pode contratar um pacote adicional e verifica se existem pacotes disponiveis;
-A URA Cognitiva lista e oferece os pacotes disponíveis ao cliente;
-A URA Cognitiva informa que no momento estas são as únicas opções disponíveis;
-URA informa o pacote não foi contratado;
-A URA Cognitiva transfere para o desambiguador.</t>
+7 - A URA Cognitiva lista e oferece os pacotes disponíveis ao cliente;
+8 - A URA Cognitiva informa que no momento estas são as únicas opções disponíveis;
+9 - URA informa o pacote não foi contratado;
+10 - A URA Cognitiva transfere para o desambiguador.</t>
   </si>
   <si>
     <t>150</t>
@@ -4053,18 +4053,18 @@
 Não quer mais nada.</t>
   </si>
   <si>
-    <t>Chamada é encaminhada para a URA Cognitiva;
-Ouvir a saudacão da URA Cognitiva conforme descrito na DF.
-A URA Congnitiva informa que entendeu que deseja falar sobre Contratação de Pacotes;
-A URA Cognitiva pede para aguardar enquanto verifica a internet;
-A URA Cognitiva informa que já existe um pacote ativo e que só é possível contratar
+    <t>1 - Chamada é encaminhada para a URA Cognitiva;
+2 - Ouvir a saudacão da URA Cognitiva conforme descrito na DF.
+3 - A URA Congnitiva informa que entendeu que deseja falar sobre Contratação de Pacotes;
+4 - A URA Cognitiva pede para aguardar enquanto verifica a internet;
+5 - A URA Cognitiva informa que já existe um pacote ativo e que só é possível contratar
 um novo depois de consumi-lo;
-A URA Cognitiva informa que está com velocidade reduzida porque já consumiu o pacote,
+6 - A URA Cognitiva informa que está com velocidade reduzida porque já consumiu o pacote,
 mas pode contratar um pacote adicional e verifica se existem pacotes disponiveis;
-A URA Cognitiva lista e oferece os pacotes disponíveis ao cliente;
-A URA Cognitiva informa que no momento estas são as únicas opções disponíveis;
-URA informa o pacote não foi contratado;
-A URA Cognitiva agradece e encerra a ligação.</t>
+7 - A URA Cognitiva lista e oferece os pacotes disponíveis ao cliente;
+8 - A URA Cognitiva informa que no momento estas são as únicas opções disponíveis;
+9 - URA informa o pacote não foi contratado;
+10 - A URA Cognitiva agradece e encerra a ligação.</t>
   </si>
   <si>
     <t>151</t>
@@ -4088,19 +4088,19 @@
 Quer algo mais.</t>
   </si>
   <si>
-    <t>Chamada é encaminhada para a URA Cognitiva;
-Ouvir a saudacão da URA Cognitiva conforme descrito na DF.
-A URA Congnitiva informa que entendeu que deseja falar sobre Contratação de Pacotes;
-A URA Cognitiva pede para aguardar enquanto verifica a internet;
-A URA Cognitiva informa que já existe um pacote ativo e que só é possível contratar
+    <t>1 - Chamada é encaminhada para a URA Cognitiva;
+2 - Ouvir a saudacão da URA Cognitiva conforme descrito na DF.
+3 - A URA Congnitiva informa que entendeu que deseja falar sobre Contratação de Pacotes;
+4 - A URA Cognitiva pede para aguardar enquanto verifica a internet;
+5 - A URA Cognitiva informa que já existe um pacote ativo e que só é possível contratar
 um novo depois de consumi-lo;
-A URA Cognitiva informa que está com velocidade reduzida porque já consumiu o pacote,
+6 - A URA Cognitiva informa que está com velocidade reduzida porque já consumiu o pacote,
 mas pode contratar um pacote adicional e verifica se existem pacotes disponiveis;
-A URA Cognitiva lista e oferece os pacotes disponíveis ao cliente;
-A URA Cognitiva informa que no momento estas são as únicas opções disponíveis;
-URA informa que precisa da senha única;
-URA informa o pacote foi contratado;
-A URA Cognitiva transfere para o desambiguador.</t>
+7 - A URA Cognitiva lista e oferece os pacotes disponíveis ao cliente;
+8 - A URA Cognitiva informa que no momento estas são as únicas opções disponíveis;
+9 - URA informa que precisa da senha única;
+10 - URA informa o pacote foi contratado;
+11 - A URA Cognitiva transfere para o desambiguador.</t>
   </si>
   <si>
     <t>152</t>
@@ -4124,19 +4124,19 @@
 Não quer mais nada.</t>
   </si>
   <si>
-    <t>Chamada é encaminhada para a URA Cognitiva;
-Ouvir a saudacão da URA Cognitiva conforme descrito na DF.
-A URA Congnitiva informa que entendeu que deseja falar sobre Contratação de Pacotes;
-A URA Cognitiva pede para aguardar enquanto verifica a internet;
-A URA Cognitiva informa que já existe um pacote ativo e que só é possível contratar
+    <t>1 - Chamada é encaminhada para a URA Cognitiva;
+2 - Ouvir a saudacão da URA Cognitiva conforme descrito na DF.
+3 - A URA Congnitiva informa que entendeu que deseja falar sobre Contratação de Pacotes;
+4 - A URA Cognitiva pede para aguardar enquanto verifica a internet;
+5 - A URA Cognitiva informa que já existe um pacote ativo e que só é possível contratar
 um novo depois de consumi-lo;
-A URA Cognitiva informa que está com velocidade reduzida porque já consumiu o pacote,
+6 - A URA Cognitiva informa que está com velocidade reduzida porque já consumiu o pacote,
 mas pode contratar um pacote adicional e verifica se existem pacotes disponiveis;
-A URA Cognitiva lista e oferece os pacotes disponíveis ao cliente;
-A URA Cognitiva informa que no momento estas são as únicas opções disponíveis;
-URA informa que precisa da senha única;
-URA informa o pacote foi contratado;
-A URA Cognitiva agradece e encerra a ligação.</t>
+7 - A URA Cognitiva lista e oferece os pacotes disponíveis ao cliente;
+8 - A URA Cognitiva informa que no momento estas são as únicas opções disponíveis;
+9 - URA informa que precisa da senha única;
+10 - URA informa o pacote foi contratado;
+11 - A URA Cognitiva agradece e encerra a ligação.</t>
   </si>
   <si>
     <t>153</t>
@@ -4160,19 +4160,19 @@
 Quer algo mais.</t>
   </si>
   <si>
-    <t>Chamada é encaminhada para a URA Cognitiva;
-Ouvir a saudacão da URA Cognitiva conforme descrito na DF.
-A URA Congnitiva informa que entendeu que deseja falar sobre Contratação de Pacotes;
-A URA Cognitiva pede para aguardar enquanto verifica a internet;
-A URA Cognitiva informa que já existe um pacote ativo e que só é possível contratar
+    <t>1 - Chamada é encaminhada para a URA Cognitiva;
+2 - Ouvir a saudacão da URA Cognitiva conforme descrito na DF.
+3 - A URA Congnitiva informa que entendeu que deseja falar sobre Contratação de Pacotes;
+4 - A URA Cognitiva pede para aguardar enquanto verifica a internet;
+5 - A URA Cognitiva informa que já existe um pacote ativo e que só é possível contratar
 um novo depois de consumi-lo;
-A URA Cognitiva informa que está com velocidade reduzida porque já consumiu o pacote,
+6 - A URA Cognitiva informa que está com velocidade reduzida porque já consumiu o pacote,
 mas pode contratar um pacote adicional e verifica se existem pacotes disponiveis;
-A URA Cognitiva lista e oferece os pacotes disponíveis ao cliente;
-A URA Cognitiva informa que no momento estas são as únicas opções disponíveis;
-URA informa que precisa da senha única;
-URA informa o pacote não foi contratado;
-A URA Cognitiva transfere para o desambiguador.</t>
+7 - A URA Cognitiva lista e oferece os pacotes disponíveis ao cliente;
+8 - A URA Cognitiva informa que no momento estas são as únicas opções disponíveis;
+9 - URA informa que precisa da senha única;
+10 - URA informa o pacote não foi contratado;
+11 - A URA Cognitiva transfere para o desambiguador.</t>
   </si>
   <si>
     <t>154</t>
@@ -4196,19 +4196,19 @@
 Não quer mais nada.</t>
   </si>
   <si>
-    <t>Chamada é encaminhada para a URA Cognitiva;
-Ouvir a saudacão da URA Cognitiva conforme descrito na DF.
-A URA Congnitiva informa que entendeu que deseja falar sobre Contratação de Pacotes;
-A URA Cognitiva pede para aguardar enquanto verifica a internet;
-A URA Cognitiva informa que já existe um pacote ativo e que só é possível contratar
+    <t>1 - Chamada é encaminhada para a URA Cognitiva;
+2 - Ouvir a saudacão da URA Cognitiva conforme descrito na DF.
+3 - A URA Congnitiva informa que entendeu que deseja falar sobre Contratação de Pacotes;
+4 - A URA Cognitiva pede para aguardar enquanto verifica a internet;
+5 - A URA Cognitiva informa que já existe um pacote ativo e que só é possível contratar
 um novo depois de consumi-lo;
-A URA Cognitiva informa que está com velocidade reduzida porque já consumiu o pacote,
+6 - A URA Cognitiva informa que está com velocidade reduzida porque já consumiu o pacote,
 mas pode contratar um pacote adicional e verifica se existem pacotes disponiveis;
-A URA Cognitiva lista e oferece os pacotes disponíveis ao cliente;
-A URA Cognitiva informa que no momento estas são as únicas opções disponíveis;
-URA informa que precisa da senha única;
-URA informa o pacote não foi contratado;
-A URA Cognitiva agradece e encerra a ligação.</t>
+7 - A URA Cognitiva lista e oferece os pacotes disponíveis ao cliente;
+8 - A URA Cognitiva informa que no momento estas são as únicas opções disponíveis;
+9 - URA informa que precisa da senha única;
+10 - URA informa o pacote não foi contratado;
+11 - A URA Cognitiva agradece e encerra a ligação.</t>
   </si>
   <si>
     <t>155</t>
@@ -4231,19 +4231,19 @@
 Quer algo mais.</t>
   </si>
   <si>
-    <t>Chamada é encaminhada para a URA Cognitiva;
-Ouvir a saudacão da URA Cognitiva conforme descrito na DF.
-A URA Congnitiva informa que entendeu que deseja falar sobre Contratação de Pacotes;
-A URA Cognitiva pede para aguardar enquanto verifica a internet;
-A URA Cognitiva informa que já existe um pacote ativo e que só é possível contratar
+    <t>1 - Chamada é encaminhada para a URA Cognitiva;
+2 - Ouvir a saudacão da URA Cognitiva conforme descrito na DF.
+3 - A URA Congnitiva informa que entendeu que deseja falar sobre Contratação de Pacotes;
+4 - A URA Cognitiva pede para aguardar enquanto verifica a internet;
+5 - A URA Cognitiva informa que já existe um pacote ativo e que só é possível contratar
 um novo depois de consumi-lo;
-A URA Cognitiva informa que está com velocidade reduzida porque já consumiu o pacote,
+6 - A URA Cognitiva informa que está com velocidade reduzida porque já consumiu o pacote,
 mas pode contratar um pacote adicional e verifica se existem pacotes disponiveis;
-A URA Cognitiva lista e oferece os pacotes disponíveis ao cliente;
-A URA Cognitiva informa que no momento estas são as únicas opções disponíveis;
-URA informa que precisa da senha única;
-URA Informa que não foi possível confirmar os dados do cliente e não vai poder prosseguir;
-A URA Cognitiva transfere para o desambiguador.</t>
+7 - A URA Cognitiva lista e oferece os pacotes disponíveis ao cliente;
+8 - A URA Cognitiva informa que no momento estas são as únicas opções disponíveis;
+9 - URA informa que precisa da senha única;
+10 - URA Informa que não foi possível confirmar os dados do cliente e não vai poder prosseguir;
+11 - A URA Cognitiva transfere para o desambiguador.</t>
   </si>
   <si>
     <t>156</t>
@@ -4266,19 +4266,19 @@
 Não quer mais nada.</t>
   </si>
   <si>
-    <t>Chamada é encaminhada para a URA Cognitiva;
-Ouvir a saudacão da URA Cognitiva conforme descrito na DF.
-A URA Congnitiva informa que entendeu que deseja falar sobre Contratação de Pacotes;
-A URA Cognitiva pede para aguardar enquanto verifica a internet;
-A URA Cognitiva informa que já existe um pacote ativo e que só é possível contratar
+    <t>1 - Chamada é encaminhada para a URA Cognitiva;
+2 - Ouvir a saudacão da URA Cognitiva conforme descrito na DF.
+3 - A URA Congnitiva informa que entendeu que deseja falar sobre Contratação de Pacotes;
+4 - A URA Cognitiva pede para aguardar enquanto verifica a internet;
+5 - A URA Cognitiva informa que já existe um pacote ativo e que só é possível contratar
 um novo depois de consumi-lo;
-A URA Cognitiva informa que está com velocidade reduzida porque já consumiu o pacote,
+6 - A URA Cognitiva informa que está com velocidade reduzida porque já consumiu o pacote,
 mas pode contratar um pacote adicional e verifica se existem pacotes disponiveis;
-A URA Cognitiva lista e oferece os pacotes disponíveis ao cliente;
-A URA Cognitiva informa que no momento estas são as únicas opções disponíveis;
-URA informa que precisa da senha única;
-URA Informa que não foi possível confirmar os dados do cliente e não vai poder prosseguir;
-A URA Cognitiva agradece e encerra a ligação.</t>
+7 - A URA Cognitiva lista e oferece os pacotes disponíveis ao cliente;
+8 - A URA Cognitiva informa que no momento estas são as únicas opções disponíveis;
+9 - URA informa que precisa da senha única;
+10 - URA Informa que não foi possível confirmar os dados do cliente e não vai poder prosseguir;
+11 - A URA Cognitiva agradece e encerra a ligação.</t>
   </si>
   <si>
     <t>157</t>
@@ -4301,18 +4301,18 @@
 Quer algo mais.</t>
   </si>
   <si>
-    <t>Chamada é encaminhada para a URA Cognitiva;
-Ouvir a saudacão da URA Cognitiva conforme descrito na DF.
-A URA Congnitiva informa que entendeu que deseja falar sobre Contratação de Pacotes;
-A URA Cognitiva pede para aguardar enquanto verifica a internet;
-A URA Cognitiva informa que já existe um pacote ativo e que só é possível contratar
+    <t>1 - Chamada é encaminhada para a URA Cognitiva;
+2 - Ouvir a saudacão da URA Cognitiva conforme descrito na DF.
+3 - A URA Congnitiva informa que entendeu que deseja falar sobre Contratação de Pacotes;
+4 - A URA Cognitiva pede para aguardar enquanto verifica a internet;
+5 - A URA Cognitiva informa que já existe um pacote ativo e que só é possível contratar
 um novo depois de consumi-lo;
-A URA Cognitiva informa que está com velocidade reduzida porque já consumiu o pacote,
+6 - A URA Cognitiva informa que está com velocidade reduzida porque já consumiu o pacote,
 mas pode contratar um pacote adicional e verifica se existem pacotes disponiveis;
-A URA Cognitiva lista e oferece os pacotes disponíveis ao cliente;
-A URA Cognitiva informa que no momento estas são as únicas opções disponíveis;
-A URA Cognitiva informa que não efetuou a contratação;
-A URA Cognitiva transfere para o desambiguador.</t>
+7 - A URA Cognitiva lista e oferece os pacotes disponíveis ao cliente;
+8 - A URA Cognitiva informa que no momento estas são as únicas opções disponíveis;
+9 - A URA Cognitiva informa que não efetuou a contratação;
+10 - A URA Cognitiva transfere para o desambiguador.</t>
   </si>
   <si>
     <t>158</t>
@@ -4335,18 +4335,18 @@
 Não quer mais nada.</t>
   </si>
   <si>
-    <t>Chamada é encaminhada para a URA Cognitiva;
-Ouvir a saudacão da URA Cognitiva conforme descrito na DF.
-A URA Congnitiva informa que entendeu que deseja falar sobre Contratação de Pacotes;
-A URA Cognitiva pede para aguardar enquanto verifica a internet;
-A URA Cognitiva informa que já existe um pacote ativo e que só é possível contratar
+    <t>1 - Chamada é encaminhada para a URA Cognitiva;
+2 - Ouvir a saudacão da URA Cognitiva conforme descrito na DF.
+3 - A URA Congnitiva informa que entendeu que deseja falar sobre Contratação de Pacotes;
+4 - A URA Cognitiva pede para aguardar enquanto verifica a internet;
+5 - A URA Cognitiva informa que já existe um pacote ativo e que só é possível contratar
 um novo depois de consumi-lo;
-A URA Cognitiva informa que está com velocidade reduzida porque já consumiu o pacote,
+6 - A URA Cognitiva informa que está com velocidade reduzida porque já consumiu o pacote,
 mas pode contratar um pacote adicional e verifica se existem pacotes disponiveis;
-A URA Cognitiva lista e oferece os pacotes disponíveis ao cliente;
-A URA Cognitiva informa que no momento estas são as únicas opções disponíveis;
-A URA Cognitiva informa que não efetuou a contratação;
-A URA Cognitiva agradece e encerra a ligação.</t>
+7 - A URA Cognitiva lista e oferece os pacotes disponíveis ao cliente;
+8 - A URA Cognitiva informa que no momento estas são as únicas opções disponíveis;
+9 - A URA Cognitiva informa que não efetuou a contratação;
+10 - A URA Cognitiva agradece e encerra a ligação.</t>
   </si>
   <si>
     <t>159</t>
@@ -4366,17 +4366,17 @@
 Quer algo mais.</t>
   </si>
   <si>
-    <t>Chamada é encaminhada para a URA Cognitiva;
-Ouvir a saudacão da URA Cognitiva conforme descrito na DF.
-A URA Congnitiva informa que entendeu que deseja falar sobre Contratação de Pacotes;
-A URA Cognitiva pede para aguardar enquanto verifica a internet;
-A URA Cognitiva informa que já existe um pacote ativo e que só é possível contratar
+    <t>1 - Chamada é encaminhada para a URA Cognitiva;
+2 - Ouvir a saudacão da URA Cognitiva conforme descrito na DF.
+3 - A URA Congnitiva informa que entendeu que deseja falar sobre Contratação de Pacotes;
+4 - A URA Cognitiva pede para aguardar enquanto verifica a internet;
+5 - A URA Cognitiva informa que já existe um pacote ativo e que só é possível contratar
 um novo depois de consumi-lo;
-A URA Cognitiva informa que está com velocidade reduzida porque já consumiu o pacote,
+6 - A URA Cognitiva informa que está com velocidade reduzida porque já consumiu o pacote,
 mas pode contratar um pacote adicional e verifica se existem pacotes disponiveis;
-A URA Cognitiva lista e oferece os pacotes disponíveis ao cliente;
-A URA Cognitiva informa que no momento estas são as únicas opções disponíveis;
-A URA Cognitiva transfere para o desambiguador.</t>
+7 - A URA Cognitiva lista e oferece os pacotes disponíveis ao cliente;
+8 - A URA Cognitiva informa que no momento estas são as únicas opções disponíveis;
+9 - A URA Cognitiva transfere para o desambiguador.</t>
   </si>
   <si>
     <t>160</t>
@@ -4396,17 +4396,17 @@
 Não quer mais nada.</t>
   </si>
   <si>
-    <t>Chamada é encaminhada para a URA Cognitiva;
-Ouvir a saudacão da URA Cognitiva conforme descrito na DF.
-A URA Congnitiva informa que entendeu que deseja falar sobre Contratação de Pacotes;
-A URA Cognitiva pede para aguardar enquanto verifica a internet;
-A URA Cognitiva informa que já existe um pacote ativo e que só é possível contratar
+    <t>1 - Chamada é encaminhada para a URA Cognitiva;
+2 - Ouvir a saudacão da URA Cognitiva conforme descrito na DF.
+3 - A URA Congnitiva informa que entendeu que deseja falar sobre Contratação de Pacotes;
+4 - A URA Cognitiva pede para aguardar enquanto verifica a internet;
+5 - A URA Cognitiva informa que já existe um pacote ativo e que só é possível contratar
 um novo depois de consumi-lo;
-A URA Cognitiva informa que está com velocidade reduzida porque já consumiu o pacote,
+6 - A URA Cognitiva informa que está com velocidade reduzida porque já consumiu o pacote,
 mas pode contratar um pacote adicional e verifica se existem pacotes disponiveis;
-A URA Cognitiva lista e oferece os pacotes disponíveis ao cliente;
-A URA Cognitiva informa que no momento estas são as únicas opções disponíveis;
-A URA Cognitiva agradece e encerra a ligação.</t>
+7 - A URA Cognitiva lista e oferece os pacotes disponíveis ao cliente;
+8 - A URA Cognitiva informa que no momento estas são as únicas opções disponíveis;
+9 - A URA Cognitiva agradece e encerra a ligação.</t>
   </si>
   <si>
     <t>161</t>
@@ -4457,14 +4457,14 @@
 Quer algo mais.</t>
   </si>
   <si>
-    <t>Chamada é encaminhada para a URA Cognitiva;
-Ouvir a saudacão da URA Cognitiva conforme descrito na DF.
-A URA Congnitiva informa que entendeu que deseja falar sobre Contratação de Pacotes;
-A URA Cognitiva pede para aguardar enquanto verifica a internet;
-A URA Cognitiva informa que já existe um pacote ativo e que só é possível contratar
+    <t>1 - Chamada é encaminhada para a URA Cognitiva;
+2 - Ouvir a saudacão da URA Cognitiva conforme descrito na DF.
+3 - A URA Congnitiva informa que entendeu que deseja falar sobre Contratação de Pacotes;
+4 - A URA Cognitiva pede para aguardar enquanto verifica a internet;
+5 - A URA Cognitiva informa que já existe um pacote ativo e que só é possível contratar
 um novo depois de consumi-lo;
-A URA Cognitiva informa que não existem pacotes disponiveis no momento;
-A URA Cognitiva transfere para o desambiguador.</t>
+6 - A URA Cognitiva informa que não existem pacotes disponiveis no momento;
+7 - A URA Cognitiva transfere para o desambiguador.</t>
   </si>
   <si>
     <t>164</t>
@@ -4481,14 +4481,14 @@
 Não quer mais nada.</t>
   </si>
   <si>
-    <t>Chamada é encaminhada para a URA Cognitiva;
-Ouvir a saudacão da URA Cognitiva conforme descrito na DF.
-A URA Congnitiva informa que entendeu que deseja falar sobre Contratação de Pacotes;
-A URA Cognitiva pede para aguardar enquanto verifica a internet;
-A URA Cognitiva informa que já existe um pacote ativo e que só é possível contratar
+    <t>1 - Chamada é encaminhada para a URA Cognitiva;
+2 - Ouvir a saudacão da URA Cognitiva conforme descrito na DF.
+3 - A URA Congnitiva informa que entendeu que deseja falar sobre Contratação de Pacotes;
+4 - A URA Cognitiva pede para aguardar enquanto verifica a internet;
+5 - A URA Cognitiva informa que já existe um pacote ativo e que só é possível contratar
 um novo depois de consumi-lo;
-A URA Cognitiva informa que não existem pacotes disponiveis no momento;
-A URA Cognitiva agradece e encerra a ligação.</t>
+6 - A URA Cognitiva informa que não existem pacotes disponiveis no momento;
+7 - A URA Cognitiva agradece e encerra a ligação.</t>
   </si>
   <si>
     <t>165</t>
@@ -4509,15 +4509,15 @@
 Quer algo mais.</t>
   </si>
   <si>
-    <t>Chamada é encaminhada para a URA Cognitiva;
-Ouvir a saudacão da URA Cognitiva conforme descrito na DF.
-A URA Congnitiva informa que entendeu que deseja falar sobre Contratação de Pacotes;
-A URA Cognitiva pede para aguardar enquanto verifica a internet;
-A URA Cognitiva informa que já existe um pacote ativo e que só é possível contratar
+    <t>1 - Chamada é encaminhada para a URA Cognitiva;
+2 - Ouvir a saudacão da URA Cognitiva conforme descrito na DF.
+3 - A URA Congnitiva informa que entendeu que deseja falar sobre Contratação de Pacotes;
+4 - A URA Cognitiva pede para aguardar enquanto verifica a internet;
+5 - A URA Cognitiva informa que já existe um pacote ativo e que só é possível contratar
 um novo depois de consumi-lo;
-A URA Cognitiva lista e oferece os pacotes disponíveis ao cliente;
-URA informa o pacote foi contratado;
-A URA Cognitiva transfere para o desambiguador.</t>
+6 - A URA Cognitiva lista e oferece os pacotes disponíveis ao cliente;
+7 - URA informa o pacote foi contratado;
+8 - A URA Cognitiva transfere para o desambiguador.</t>
   </si>
   <si>
     <t>166</t>
@@ -4538,15 +4538,15 @@
 Não quer mais nada.</t>
   </si>
   <si>
-    <t>Chamada é encaminhada para a URA Cognitiva;
-Ouvir a saudacão da URA Cognitiva conforme descrito na DF.
-A URA Congnitiva informa que entendeu que deseja falar sobre Contratação de Pacotes;
-A URA Cognitiva pede para aguardar enquanto verifica a internet;
-A URA Cognitiva informa que já existe um pacote ativo e que só é possível contratar
+    <t>1 - Chamada é encaminhada para a URA Cognitiva;
+2 - Ouvir a saudacão da URA Cognitiva conforme descrito na DF.
+3 - A URA Congnitiva informa que entendeu que deseja falar sobre Contratação de Pacotes;
+4 - A URA Cognitiva pede para aguardar enquanto verifica a internet;
+5 - A URA Cognitiva informa que já existe um pacote ativo e que só é possível contratar
 um novo depois de consumi-lo;
-A URA Cognitiva lista e oferece os pacotes disponíveis ao cliente;
-URA informa o pacote foi contratado;
-A URA Cognitiva agradece e encerra a ligação.</t>
+6 - A URA Cognitiva lista e oferece os pacotes disponíveis ao cliente;
+7 - URA informa o pacote foi contratado;
+8 - A URA Cognitiva agradece e encerra a ligação.</t>
   </si>
   <si>
     <t>167</t>
@@ -4567,15 +4567,15 @@
 Quer algo mais.</t>
   </si>
   <si>
-    <t>Chamada é encaminhada para a URA Cognitiva;
-Ouvir a saudacão da URA Cognitiva conforme descrito na DF.
-A URA Congnitiva informa que entendeu que deseja falar sobre Contratação de Pacotes;
-A URA Cognitiva pede para aguardar enquanto verifica a internet;
-A URA Cognitiva informa que já existe um pacote ativo e que só é possível contratar
+    <t>1 - Chamada é encaminhada para a URA Cognitiva;
+2 - Ouvir a saudacão da URA Cognitiva conforme descrito na DF.
+3 - A URA Congnitiva informa que entendeu que deseja falar sobre Contratação de Pacotes;
+4 - A URA Cognitiva pede para aguardar enquanto verifica a internet;
+5 - A URA Cognitiva informa que já existe um pacote ativo e que só é possível contratar
 um novo depois de consumi-lo;
-A URA Cognitiva lista e oferece os pacotes disponíveis ao cliente;
-URA informa o pacote não foi contratado;
-A URA Cognitiva transfere para o desambiguador.</t>
+6 - A URA Cognitiva lista e oferece os pacotes disponíveis ao cliente;
+7 - URA informa o pacote não foi contratado;
+8 - A URA Cognitiva transfere para o desambiguador.</t>
   </si>
   <si>
     <t>168</t>
@@ -4596,15 +4596,15 @@
 Não quer mais nada.</t>
   </si>
   <si>
-    <t>Chamada é encaminhada para a URA Cognitiva;
-Ouvir a saudacão da URA Cognitiva conforme descrito na DF.
-A URA Congnitiva informa que entendeu que deseja falar sobre Contratação de Pacotes;
-A URA Cognitiva pede para aguardar enquanto verifica a internet;
-A URA Cognitiva informa que já existe um pacote ativo e que só é possível contratar
+    <t>1 - Chamada é encaminhada para a URA Cognitiva;
+2 - Ouvir a saudacão da URA Cognitiva conforme descrito na DF.
+3 - A URA Congnitiva informa que entendeu que deseja falar sobre Contratação de Pacotes;
+4 - A URA Cognitiva pede para aguardar enquanto verifica a internet;
+5 - A URA Cognitiva informa que já existe um pacote ativo e que só é possível contratar
 um novo depois de consumi-lo;
-A URA Cognitiva lista e oferece os pacotes disponíveis ao cliente;
-URA informa o pacote não foi contratado;
-A URA Cognitiva agradece e encerra a ligação.</t>
+6 - A URA Cognitiva lista e oferece os pacotes disponíveis ao cliente;
+7 - URA informa o pacote não foi contratado;
+8 - A URA Cognitiva agradece e encerra a ligação.</t>
   </si>
   <si>
     <t>169</t>
@@ -4626,16 +4626,16 @@
 Quer algo mais.</t>
   </si>
   <si>
-    <t>Chamada é encaminhada para a URA Cognitiva;
-Ouvir a saudacão da URA Cognitiva conforme descrito na DF.
-A URA Congnitiva informa que entendeu que deseja falar sobre Contratação de Pacotes;
-A URA Cognitiva pede para aguardar enquanto verifica a internet;
-A URA Cognitiva informa que já existe um pacote ativo e que só é possível contratar
+    <t>1 - Chamada é encaminhada para a URA Cognitiva;
+2 - Ouvir a saudacão da URA Cognitiva conforme descrito na DF.
+3 - A URA Congnitiva informa que entendeu que deseja falar sobre Contratação de Pacotes;
+4 - A URA Cognitiva pede para aguardar enquanto verifica a internet;
+5 - A URA Cognitiva informa que já existe um pacote ativo e que só é possível contratar
 um novo depois de consumi-lo;
-A URA Cognitiva lista e oferece os pacotes disponíveis ao cliente;
-URA informa que precisa da senha única;
-URA informa o pacote foi contratado;
-A URA Cognitiva transfere para o desambiguador.</t>
+6 - A URA Cognitiva lista e oferece os pacotes disponíveis ao cliente;
+7 - URA informa que precisa da senha única;
+8 - URA informa o pacote foi contratado;
+9 - A URA Cognitiva transfere para o desambiguador.</t>
   </si>
   <si>
     <t>170</t>
@@ -4657,16 +4657,16 @@
 Não quer mais nada.</t>
   </si>
   <si>
-    <t>Chamada é encaminhada para a URA Cognitiva;
-Ouvir a saudacão da URA Cognitiva conforme descrito na DF.
-A URA Congnitiva informa que entendeu que deseja falar sobre Contratação de Pacotes;
-A URA Cognitiva pede para aguardar enquanto verifica a internet;
-A URA Cognitiva informa que já existe um pacote ativo e que só é possível contratar
+    <t>1 - Chamada é encaminhada para a URA Cognitiva;
+2 - Ouvir a saudacão da URA Cognitiva conforme descrito na DF.
+3 - A URA Congnitiva informa que entendeu que deseja falar sobre Contratação de Pacotes;
+4 - A URA Cognitiva pede para aguardar enquanto verifica a internet;
+5 - A URA Cognitiva informa que já existe um pacote ativo e que só é possível contratar
 um novo depois de consumi-lo;
-A URA Cognitiva lista e oferece os pacotes disponíveis ao cliente;
-URA informa que precisa da senha única;
-URA informa o pacote foi contratado;
-A URA Cognitiva agradece e encerra a ligação.</t>
+6 - A URA Cognitiva lista e oferece os pacotes disponíveis ao cliente;
+7 - URA informa que precisa da senha única;
+8 - URA informa o pacote foi contratado;
+9 - A URA Cognitiva agradece e encerra a ligação.</t>
   </si>
   <si>
     <t>171</t>
@@ -4688,16 +4688,16 @@
 Quer algo mais.</t>
   </si>
   <si>
-    <t>Chamada é encaminhada para a URA Cognitiva;
-Ouvir a saudacão da URA Cognitiva conforme descrito na DF.
-A URA Congnitiva informa que entendeu que deseja falar sobre Contratação de Pacotes;
-A URA Cognitiva pede para aguardar enquanto verifica a internet;
-A URA Cognitiva informa que já existe um pacote ativo e que só é possível contratar
+    <t>1 - Chamada é encaminhada para a URA Cognitiva;
+2 - Ouvir a saudacão da URA Cognitiva conforme descrito na DF.
+3 - A URA Congnitiva informa que entendeu que deseja falar sobre Contratação de Pacotes;
+4 - A URA Cognitiva pede para aguardar enquanto verifica a internet;
+5 - A URA Cognitiva informa que já existe um pacote ativo e que só é possível contratar
 um novo depois de consumi-lo;
-A URA Cognitiva lista e oferece os pacotes disponíveis ao cliente;
-URA informa que precisa da senha única;
-URA informa o pacote não foi contratado;
-A URA Cognitiva transfere para o desambiguador.</t>
+6 - A URA Cognitiva lista e oferece os pacotes disponíveis ao cliente;
+7 - URA informa que precisa da senha única;
+8 - URA informa o pacote não foi contratado;
+9 - A URA Cognitiva transfere para o desambiguador.</t>
   </si>
   <si>
     <t>172</t>
@@ -4719,16 +4719,16 @@
 Não quer mais nada.</t>
   </si>
   <si>
-    <t>Chamada é encaminhada para a URA Cognitiva;
-Ouvir a saudacão da URA Cognitiva conforme descrito na DF.
-A URA Congnitiva informa que entendeu que deseja falar sobre Contratação de Pacotes;
-A URA Cognitiva pede para aguardar enquanto verifica a internet;
-A URA Cognitiva informa que já existe um pacote ativo e que só é possível contratar
+    <t>1 - Chamada é encaminhada para a URA Cognitiva;
+2 - Ouvir a saudacão da URA Cognitiva conforme descrito na DF.
+3 - A URA Congnitiva informa que entendeu que deseja falar sobre Contratação de Pacotes;
+4 - A URA Cognitiva pede para aguardar enquanto verifica a internet;
+5 - A URA Cognitiva informa que já existe um pacote ativo e que só é possível contratar
 um novo depois de consumi-lo;
-A URA Cognitiva lista e oferece os pacotes disponíveis ao cliente;
-URA informa que precisa da senha única;
-URA informa o pacote não foi contratado;
-A URA Cognitiva agradece e encerra a ligação.</t>
+6 - A URA Cognitiva lista e oferece os pacotes disponíveis ao cliente;
+7 - URA informa que precisa da senha única;
+8 - URA informa o pacote não foi contratado;
+9 - A URA Cognitiva agradece e encerra a ligação.</t>
   </si>
   <si>
     <t>173</t>
@@ -4749,16 +4749,16 @@
 Quer algo mais.</t>
   </si>
   <si>
-    <t>Chamada é encaminhada para a URA Cognitiva;
-Ouvir a saudacão da URA Cognitiva conforme descrito na DF.
-A URA Congnitiva informa que entendeu que deseja falar sobre Contratação de Pacotes;
-A URA Cognitiva pede para aguardar enquanto verifica a internet;
-A URA Cognitiva informa que já existe um pacote ativo e que só é possível contratar
+    <t>1 - Chamada é encaminhada para a URA Cognitiva;
+2 - Ouvir a saudacão da URA Cognitiva conforme descrito na DF.
+3 - A URA Congnitiva informa que entendeu que deseja falar sobre Contratação de Pacotes;
+4 - A URA Cognitiva pede para aguardar enquanto verifica a internet;
+5 - A URA Cognitiva informa que já existe um pacote ativo e que só é possível contratar
 um novo depois de consumi-lo;
-A URA Cognitiva lista e oferece os pacotes disponíveis ao cliente;
-URA informa que precisa da senha única;
-URA Informa que não foi possível confirmar os dados do cliente e não vai poder prosseguir;
-A URA Cognitiva transfere para o desambiguador.</t>
+6 - A URA Cognitiva lista e oferece os pacotes disponíveis ao cliente;
+7 - URA informa que precisa da senha única;
+8 - URA Informa que não foi possível confirmar os dados do cliente e não vai poder prosseguir;
+9 - A URA Cognitiva transfere para o desambiguador.</t>
   </si>
   <si>
     <t>174</t>
@@ -4779,16 +4779,16 @@
 Não quer mais nada.</t>
   </si>
   <si>
-    <t>Chamada é encaminhada para a URA Cognitiva;
-Ouvir a saudacão da URA Cognitiva conforme descrito na DF.
-A URA Congnitiva informa que entendeu que deseja falar sobre Contratação de Pacotes;
-A URA Cognitiva pede para aguardar enquanto verifica a internet;
-A URA Cognitiva informa que já existe um pacote ativo e que só é possível contratar
+    <t>1 - Chamada é encaminhada para a URA Cognitiva;
+2 - Ouvir a saudacão da URA Cognitiva conforme descrito na DF.
+3 - A URA Congnitiva informa que entendeu que deseja falar sobre Contratação de Pacotes;
+4 - A URA Cognitiva pede para aguardar enquanto verifica a internet;
+5 - A URA Cognitiva informa que já existe um pacote ativo e que só é possível contratar
 um novo depois de consumi-lo;
-A URA Cognitiva lista e oferece os pacotes disponíveis ao cliente;
-URA informa que precisa da senha única;
-URA Informa que não foi possível confirmar os dados do cliente e não vai poder prosseguir;
-A URA Cognitiva agradece e encerra a ligação.</t>
+6 - A URA Cognitiva lista e oferece os pacotes disponíveis ao cliente;
+7 - URA informa que precisa da senha única;
+8 - URA Informa que não foi possível confirmar os dados do cliente e não vai poder prosseguir;
+9 - A URA Cognitiva agradece e encerra a ligação.</t>
   </si>
   <si>
     <t>175</t>
@@ -4809,15 +4809,15 @@
 Quer algo mais.</t>
   </si>
   <si>
-    <t>Chamada é encaminhada para a URA Cognitiva;
-Ouvir a saudacão da URA Cognitiva conforme descrito na DF.
-A URA Congnitiva informa que entendeu que deseja falar sobre Contratação de Pacotes;
-A URA Cognitiva pede para aguardar enquanto verifica a internet;
-A URA Cognitiva informa que já existe um pacote ativo e que só é possível contratar
+    <t>1 - Chamada é encaminhada para a URA Cognitiva;
+2 - Ouvir a saudacão da URA Cognitiva conforme descrito na DF.
+3 - A URA Congnitiva informa que entendeu que deseja falar sobre Contratação de Pacotes;
+4 - A URA Cognitiva pede para aguardar enquanto verifica a internet;
+5 - A URA Cognitiva informa que já existe um pacote ativo e que só é possível contratar
 um novo depois de consumi-lo;
-A URA Cognitiva lista e oferece os pacotes disponíveis ao cliente;
-A URA Cognitiva informa que não efetuou a contratação;
-A URA Cognitiva transfere para o desambiguador.</t>
+6 - A URA Cognitiva lista e oferece os pacotes disponíveis ao cliente;
+7 - A URA Cognitiva informa que não efetuou a contratação;
+8 - A URA Cognitiva transfere para o desambiguador.</t>
   </si>
   <si>
     <t>176</t>
@@ -4838,15 +4838,15 @@
 Não quer mais nada.</t>
   </si>
   <si>
-    <t>Chamada é encaminhada para a URA Cognitiva;
-Ouvir a saudacão da URA Cognitiva conforme descrito na DF.
-A URA Congnitiva informa que entendeu que deseja falar sobre Contratação de Pacotes;
-A URA Cognitiva pede para aguardar enquanto verifica a internet;
-A URA Cognitiva informa que já existe um pacote ativo e que só é possível contratar
+    <t>1 - Chamada é encaminhada para a URA Cognitiva;
+2 - Ouvir a saudacão da URA Cognitiva conforme descrito na DF.
+3 - A URA Congnitiva informa que entendeu que deseja falar sobre Contratação de Pacotes;
+4 - A URA Cognitiva pede para aguardar enquanto verifica a internet;
+5 - A URA Cognitiva informa que já existe um pacote ativo e que só é possível contratar
 um novo depois de consumi-lo;
-A URA Cognitiva lista e oferece os pacotes disponíveis ao cliente;
-A URA Cognitiva informa que não efetuou a contratação;
-A URA Cognitiva agradece e encerra a ligação.</t>
+6 - A URA Cognitiva lista e oferece os pacotes disponíveis ao cliente;
+7 - A URA Cognitiva informa que não efetuou a contratação;
+8 - A URA Cognitiva agradece e encerra a ligação.</t>
   </si>
   <si>
     <t>177</t>
@@ -4869,16 +4869,16 @@
 Quer algo mais.</t>
   </si>
   <si>
-    <t>Chamada é encaminhada para a URA Cognitiva;
-Ouvir a saudacão da URA Cognitiva conforme descrito na DF.
-A URA Congnitiva informa que entendeu que deseja falar sobre Contratação de Pacotes;
-A URA Cognitiva pede para aguardar enquanto verifica a internet;
-A URA Cognitiva informa que já existe um pacote ativo e que só é possível contratar
+    <t>1 - Chamada é encaminhada para a URA Cognitiva;
+2 - Ouvir a saudacão da URA Cognitiva conforme descrito na DF.
+3 - A URA Congnitiva informa que entendeu que deseja falar sobre Contratação de Pacotes;
+4 - A URA Cognitiva pede para aguardar enquanto verifica a internet;
+5 - A URA Cognitiva informa que já existe um pacote ativo e que só é possível contratar
 um novo depois de consumi-lo;
-A URA Cognitiva lista e oferece os pacotes disponíveis ao cliente;
-A URA Cognitiva informa que no momento estas são as únicas opções disponíveis;
-URA informa o pacote foi contratado;
-A URA Cognitiva transfere para o desambiguador.</t>
+6 - A URA Cognitiva lista e oferece os pacotes disponíveis ao cliente;
+7 - A URA Cognitiva informa que no momento estas são as únicas opções disponíveis;
+8 - URA informa o pacote foi contratado;
+9 - A URA Cognitiva transfere para o desambiguador.</t>
   </si>
   <si>
     <t>178</t>
@@ -4901,16 +4901,16 @@
 Não quer mais nada.</t>
   </si>
   <si>
-    <t>Chamada é encaminhada para a URA Cognitiva;
-Ouvir a saudacão da URA Cognitiva conforme descrito na DF.
-A URA Congnitiva informa que entendeu que deseja falar sobre Contratação de Pacotes;
-A URA Cognitiva pede para aguardar enquanto verifica a internet;
-A URA Cognitiva informa que já existe um pacote ativo e que só é possível contratar
+    <t>1 - Chamada é encaminhada para a URA Cognitiva;
+2 - Ouvir a saudacão da URA Cognitiva conforme descrito na DF.
+3 - A URA Congnitiva informa que entendeu que deseja falar sobre Contratação de Pacotes;
+4 - A URA Cognitiva pede para aguardar enquanto verifica a internet;
+5 - A URA Cognitiva informa que já existe um pacote ativo e que só é possível contratar
 um novo depois de consumi-lo;
-A URA Cognitiva lista e oferece os pacotes disponíveis ao cliente;
-A URA Cognitiva informa que no momento estas são as únicas opções disponíveis;
-URA informa o pacote foi contratado;
-A URA Cognitiva agradece e encerra a ligação.</t>
+6 - A URA Cognitiva lista e oferece os pacotes disponíveis ao cliente;
+7 - A URA Cognitiva informa que no momento estas são as únicas opções disponíveis;
+8 - URA informa o pacote foi contratado;
+9 - A URA Cognitiva agradece e encerra a ligação.</t>
   </si>
   <si>
     <t>179</t>
@@ -4933,16 +4933,16 @@
 Quer algo mais.</t>
   </si>
   <si>
-    <t>Chamada é encaminhada para a URA Cognitiva;
-Ouvir a saudacão da URA Cognitiva conforme descrito na DF.
-A URA Congnitiva informa que entendeu que deseja falar sobre Contratação de Pacotes;
-A URA Cognitiva pede para aguardar enquanto verifica a internet;
-A URA Cognitiva informa que já existe um pacote ativo e que só é possível contratar
+    <t>1 - Chamada é encaminhada para a URA Cognitiva;
+2 - Ouvir a saudacão da URA Cognitiva conforme descrito na DF.
+3 - A URA Congnitiva informa que entendeu que deseja falar sobre Contratação de Pacotes;
+4 - A URA Cognitiva pede para aguardar enquanto verifica a internet;
+5 - A URA Cognitiva informa que já existe um pacote ativo e que só é possível contratar
 um novo depois de consumi-lo;
-A URA Cognitiva lista e oferece os pacotes disponíveis ao cliente;
-A URA Cognitiva informa que no momento estas são as únicas opções disponíveis;
-URA informa o pacote não foi contratado;
-A URA Cognitiva transfere para o desambiguador.</t>
+6 - A URA Cognitiva lista e oferece os pacotes disponíveis ao cliente;
+7 - A URA Cognitiva informa que no momento estas são as únicas opções disponíveis;
+8 - URA informa o pacote não foi contratado;
+9 - A URA Cognitiva transfere para o desambiguador.</t>
   </si>
   <si>
     <t>180</t>
@@ -4965,16 +4965,16 @@
 Não quer mais nada.</t>
   </si>
   <si>
-    <t>Chamada é encaminhada para a URA Cognitiva;
-Ouvir a saudacão da URA Cognitiva conforme descrito na DF.
-A URA Congnitiva informa que entendeu que deseja falar sobre Contratação de Pacotes;
-A URA Cognitiva pede para aguardar enquanto verifica a internet;
-A URA Cognitiva informa que já existe um pacote ativo e que só é possível contratar
+    <t>1 - Chamada é encaminhada para a URA Cognitiva;
+2 - Ouvir a saudacão da URA Cognitiva conforme descrito na DF.
+3 - A URA Congnitiva informa que entendeu que deseja falar sobre Contratação de Pacotes;
+4 - A URA Cognitiva pede para aguardar enquanto verifica a internet;
+5 - A URA Cognitiva informa que já existe um pacote ativo e que só é possível contratar
 um novo depois de consumi-lo;
-A URA Cognitiva lista e oferece os pacotes disponíveis ao cliente;
-A URA Cognitiva informa que no momento estas são as únicas opções disponíveis;
-URA informa o pacote não foi contratado;
-A URA Cognitiva agradece e encerra a ligação.</t>
+6 - A URA Cognitiva lista e oferece os pacotes disponíveis ao cliente;
+7 - A URA Cognitiva informa que no momento estas são as únicas opções disponíveis;
+8 - URA informa o pacote não foi contratado;
+9 - A URA Cognitiva agradece e encerra a ligação.</t>
   </si>
   <si>
     <t>181</t>
@@ -4998,17 +4998,17 @@
 Quer algo mais.</t>
   </si>
   <si>
-    <t>Chamada é encaminhada para a URA Cognitiva;
-Ouvir a saudacão da URA Cognitiva conforme descrito na DF.
-A URA Congnitiva informa que entendeu que deseja falar sobre Contratação de Pacotes;
-A URA Cognitiva pede para aguardar enquanto verifica a internet;
-A URA Cognitiva informa que já existe um pacote ativo e que só é possível contratar
+    <t>1 - Chamada é encaminhada para a URA Cognitiva;
+2 - Ouvir a saudacão da URA Cognitiva conforme descrito na DF.
+3 - A URA Congnitiva informa que entendeu que deseja falar sobre Contratação de Pacotes;
+4 - A URA Cognitiva pede para aguardar enquanto verifica a internet;
+5 - A URA Cognitiva informa que já existe um pacote ativo e que só é possível contratar
 um novo depois de consumi-lo;
-A URA Cognitiva lista e oferece os pacotes disponíveis ao cliente;
-A URA Cognitiva informa que no momento estas são as únicas opções disponíveis;
-URA informa que precisa da senha única;
-URA informa o pacote foi contratado;
-A URA Cognitiva transfere para o desambiguador.</t>
+6 - A URA Cognitiva lista e oferece os pacotes disponíveis ao cliente;
+7 - A URA Cognitiva informa que no momento estas são as únicas opções disponíveis;
+8 - URA informa que precisa da senha única;
+9 - URA informa o pacote foi contratado;
+10 - A URA Cognitiva transfere para o desambiguador.</t>
   </si>
   <si>
     <t>182</t>
@@ -5032,17 +5032,17 @@
 Não quer mais nada.</t>
   </si>
   <si>
-    <t>Chamada é encaminhada para a URA Cognitiva;
-Ouvir a saudacão da URA Cognitiva conforme descrito na DF.
-A URA Congnitiva informa que entendeu que deseja falar sobre Contratação de Pacotes;
-A URA Cognitiva pede para aguardar enquanto verifica a internet;
-A URA Cognitiva informa que já existe um pacote ativo e que só é possível contratar
+    <t>1 - Chamada é encaminhada para a URA Cognitiva;
+2 - Ouvir a saudacão da URA Cognitiva conforme descrito na DF.
+3 - A URA Congnitiva informa que entendeu que deseja falar sobre Contratação de Pacotes;
+4 - A URA Cognitiva pede para aguardar enquanto verifica a internet;
+5 - A URA Cognitiva informa que já existe um pacote ativo e que só é possível contratar
 um novo depois de consumi-lo;
-A URA Cognitiva lista e oferece os pacotes disponíveis ao cliente;
-A URA Cognitiva informa que no momento estas são as únicas opções disponíveis;
-URA informa que precisa da senha única;
-URA informa o pacote foi contratado;
-A URA Cognitiva agradece e encerra a ligação.</t>
+6 - A URA Cognitiva lista e oferece os pacotes disponíveis ao cliente;
+7 - A URA Cognitiva informa que no momento estas são as únicas opções disponíveis;
+8 - URA informa que precisa da senha única;
+9 - URA informa o pacote foi contratado;
+10 - A URA Cognitiva agradece e encerra a ligação.</t>
   </si>
   <si>
     <t>183</t>
@@ -5066,17 +5066,17 @@
 Quer algo mais.</t>
   </si>
   <si>
-    <t>Chamada é encaminhada para a URA Cognitiva;
-Ouvir a saudacão da URA Cognitiva conforme descrito na DF.
-A URA Congnitiva informa que entendeu que deseja falar sobre Contratação de Pacotes;
-A URA Cognitiva pede para aguardar enquanto verifica a internet;
-A URA Cognitiva informa que já existe um pacote ativo e que só é possível contratar
+    <t>1 - Chamada é encaminhada para a URA Cognitiva;
+2 - Ouvir a saudacão da URA Cognitiva conforme descrito na DF.
+3 - A URA Congnitiva informa que entendeu que deseja falar sobre Contratação de Pacotes;
+4 - A URA Cognitiva pede para aguardar enquanto verifica a internet;
+5 - A URA Cognitiva informa que já existe um pacote ativo e que só é possível contratar
 um novo depois de consumi-lo;
-A URA Cognitiva lista e oferece os pacotes disponíveis ao cliente;
-A URA Cognitiva informa que no momento estas são as únicas opções disponíveis;
-URA informa que precisa da senha única;
-URA informa o pacote não foi contratado;
-A URA Cognitiva transfere para o desambiguador.</t>
+6 - A URA Cognitiva lista e oferece os pacotes disponíveis ao cliente;
+7 - A URA Cognitiva informa que no momento estas são as únicas opções disponíveis;
+8 - URA informa que precisa da senha única;
+9 - URA informa o pacote não foi contratado;
+10 - A URA Cognitiva transfere para o desambiguador.</t>
   </si>
   <si>
     <t>184</t>
@@ -5100,17 +5100,17 @@
 Não quer mais nada.</t>
   </si>
   <si>
-    <t>Chamada é encaminhada para a URA Cognitiva;
-Ouvir a saudacão da URA Cognitiva conforme descrito na DF.
-A URA Congnitiva informa que entendeu que deseja falar sobre Contratação de Pacotes;
-A URA Cognitiva pede para aguardar enquanto verifica a internet;
-A URA Cognitiva informa que já existe um pacote ativo e que só é possível contratar
+    <t>1 - Chamada é encaminhada para a URA Cognitiva;
+2 - Ouvir a saudacão da URA Cognitiva conforme descrito na DF.
+3 - A URA Congnitiva informa que entendeu que deseja falar sobre Contratação de Pacotes;
+4 - A URA Cognitiva pede para aguardar enquanto verifica a internet;
+5 - A URA Cognitiva informa que já existe um pacote ativo e que só é possível contratar
 um novo depois de consumi-lo;
-A URA Cognitiva lista e oferece os pacotes disponíveis ao cliente;
-A URA Cognitiva informa que no momento estas são as únicas opções disponíveis;
-URA informa que precisa da senha única;
-URA informa o pacote não foi contratado;
-A URA Cognitiva agradece e encerra a ligação.</t>
+6 - A URA Cognitiva lista e oferece os pacotes disponíveis ao cliente;
+7 - A URA Cognitiva informa que no momento estas são as únicas opções disponíveis;
+8 - URA informa que precisa da senha única;
+9 - URA informa o pacote não foi contratado;
+10 - A URA Cognitiva agradece e encerra a ligação.</t>
   </si>
   <si>
     <t>185</t>
@@ -5133,17 +5133,17 @@
 Quer algo mais.</t>
   </si>
   <si>
-    <t>Chamada é encaminhada para a URA Cognitiva;
-Ouvir a saudacão da URA Cognitiva conforme descrito na DF.
-A URA Congnitiva informa que entendeu que deseja falar sobre Contratação de Pacotes;
-A URA Cognitiva pede para aguardar enquanto verifica a internet;
-A URA Cognitiva informa que já existe um pacote ativo e que só é possível contratar
+    <t>1 - Chamada é encaminhada para a URA Cognitiva;
+2 - Ouvir a saudacão da URA Cognitiva conforme descrito na DF.
+3 - A URA Congnitiva informa que entendeu que deseja falar sobre Contratação de Pacotes;
+4 - A URA Cognitiva pede para aguardar enquanto verifica a internet;
+5 - A URA Cognitiva informa que já existe um pacote ativo e que só é possível contratar
 um novo depois de consumi-lo;
-A URA Cognitiva lista e oferece os pacotes disponíveis ao cliente;
-A URA Cognitiva informa que no momento estas são as únicas opções disponíveis;
-URA informa que precisa da senha única;
-URA Informa que não foi possível confirmar os dados do cliente e não vai poder prosseguir;
-A URA Cognitiva transfere para o desambiguador.</t>
+6 - A URA Cognitiva lista e oferece os pacotes disponíveis ao cliente;
+7 - A URA Cognitiva informa que no momento estas são as únicas opções disponíveis;
+8 - URA informa que precisa da senha única;
+9 - URA Informa que não foi possível confirmar os dados do cliente e não vai poder prosseguir;
+10 - A URA Cognitiva transfere para o desambiguador.</t>
   </si>
   <si>
     <t>186</t>
@@ -5166,17 +5166,17 @@
 Não quer mais nada.</t>
   </si>
   <si>
-    <t>Chamada é encaminhada para a URA Cognitiva;
-Ouvir a saudacão da URA Cognitiva conforme descrito na DF.
-A URA Congnitiva informa que entendeu que deseja falar sobre Contratação de Pacotes;
-A URA Cognitiva pede para aguardar enquanto verifica a internet;
-A URA Cognitiva informa que já existe um pacote ativo e que só é possível contratar
+    <t>1 - Chamada é encaminhada para a URA Cognitiva;
+2 - Ouvir a saudacão da URA Cognitiva conforme descrito na DF.
+3 - A URA Congnitiva informa que entendeu que deseja falar sobre Contratação de Pacotes;
+4 - A URA Cognitiva pede para aguardar enquanto verifica a internet;
+5 - A URA Cognitiva informa que já existe um pacote ativo e que só é possível contratar
 um novo depois de consumi-lo;
-A URA Cognitiva lista e oferece os pacotes disponíveis ao cliente;
-A URA Cognitiva informa que no momento estas são as únicas opções disponíveis;
-URA informa que precisa da senha única;
-URA Informa que não foi possível confirmar os dados do cliente e não vai poder prosseguir;
-A URA Cognitiva agradece e encerra a ligação.</t>
+6 - A URA Cognitiva lista e oferece os pacotes disponíveis ao cliente;
+7 - A URA Cognitiva informa que no momento estas são as únicas opções disponíveis;
+8 - URA informa que precisa da senha única;
+9 - URA Informa que não foi possível confirmar os dados do cliente e não vai poder prosseguir;
+10 - A URA Cognitiva agradece e encerra a ligação.</t>
   </si>
   <si>
     <t>187</t>
@@ -5199,16 +5199,16 @@
 Quer algo mais.</t>
   </si>
   <si>
-    <t>Chamada é encaminhada para a URA Cognitiva;
-Ouvir a saudacão da URA Cognitiva conforme descrito na DF.
-A URA Congnitiva informa que entendeu que deseja falar sobre Contratação de Pacotes;
-A URA Cognitiva pede para aguardar enquanto verifica a internet;
-A URA Cognitiva informa que já existe um pacote ativo e que só é possível contratar
+    <t>1 - Chamada é encaminhada para a URA Cognitiva;
+2 - Ouvir a saudacão da URA Cognitiva conforme descrito na DF.
+3 - A URA Congnitiva informa que entendeu que deseja falar sobre Contratação de Pacotes;
+4 - A URA Cognitiva pede para aguardar enquanto verifica a internet;
+5 - A URA Cognitiva informa que já existe um pacote ativo e que só é possível contratar
 um novo depois de consumi-lo;
-A URA Cognitiva lista e oferece os pacotes disponíveis ao cliente;
-A URA Cognitiva informa que no momento estas são as únicas opções disponíveis;
-A URA Cognitiva informa que não efetuou a contratação;
-A URA Cognitiva transfere para o desambiguador.</t>
+6 - A URA Cognitiva lista e oferece os pacotes disponíveis ao cliente;
+7 - A URA Cognitiva informa que no momento estas são as únicas opções disponíveis;
+8 - A URA Cognitiva informa que não efetuou a contratação;
+9 - A URA Cognitiva transfere para o desambiguador.</t>
   </si>
   <si>
     <t>188</t>
@@ -5231,16 +5231,16 @@
 Não quer mais nada.</t>
   </si>
   <si>
-    <t>Chamada é encaminhada para a URA Cognitiva;
-Ouvir a saudacão da URA Cognitiva conforme descrito na DF.
-A URA Congnitiva informa que entendeu que deseja falar sobre Contratação de Pacotes;
-A URA Cognitiva pede para aguardar enquanto verifica a internet;
-A URA Cognitiva informa que já existe um pacote ativo e que só é possível contratar
+    <t>1 - Chamada é encaminhada para a URA Cognitiva;
+2 - Ouvir a saudacão da URA Cognitiva conforme descrito na DF.
+3 - A URA Congnitiva informa que entendeu que deseja falar sobre Contratação de Pacotes;
+4 - A URA Cognitiva pede para aguardar enquanto verifica a internet;
+5 - A URA Cognitiva informa que já existe um pacote ativo e que só é possível contratar
 um novo depois de consumi-lo;
-A URA Cognitiva lista e oferece os pacotes disponíveis ao cliente;
-A URA Cognitiva informa que no momento estas são as únicas opções disponíveis;
-A URA Cognitiva informa que não efetuou a contratação;
-A URA Cognitiva agradece e encerra a ligação.</t>
+6 - A URA Cognitiva lista e oferece os pacotes disponíveis ao cliente;
+7 - A URA Cognitiva informa que no momento estas são as únicas opções disponíveis;
+8 - A URA Cognitiva informa que não efetuou a contratação;
+9 - A URA Cognitiva agradece e encerra a ligação.</t>
   </si>
   <si>
     <t>189</t>
@@ -5260,15 +5260,15 @@
 Quer algo mais.</t>
   </si>
   <si>
-    <t>Chamada é encaminhada para a URA Cognitiva;
-Ouvir a saudacão da URA Cognitiva conforme descrito na DF.
-A URA Congnitiva informa que entendeu que deseja falar sobre Contratação de Pacotes;
-A URA Cognitiva pede para aguardar enquanto verifica a internet;
-A URA Cognitiva informa que já existe um pacote ativo e que só é possível contratar
+    <t>1 - Chamada é encaminhada para a URA Cognitiva;
+2 - Ouvir a saudacão da URA Cognitiva conforme descrito na DF.
+3 - A URA Congnitiva informa que entendeu que deseja falar sobre Contratação de Pacotes;
+4 - A URA Cognitiva pede para aguardar enquanto verifica a internet;
+5 - A URA Cognitiva informa que já existe um pacote ativo e que só é possível contratar
 um novo depois de consumi-lo;
-A URA Cognitiva lista e oferece os pacotes disponíveis ao cliente;
-A URA Cognitiva informa que no momento estas são as únicas opções disponíveis;
-A URA Cognitiva transfere para o desambiguador.</t>
+6 - A URA Cognitiva lista e oferece os pacotes disponíveis ao cliente;
+7 - A URA Cognitiva informa que no momento estas são as únicas opções disponíveis;
+8 - A URA Cognitiva transfere para o desambiguador.</t>
   </si>
   <si>
     <t>190</t>
@@ -5288,15 +5288,15 @@
 Não quer mais nada.</t>
   </si>
   <si>
-    <t>Chamada é encaminhada para a URA Cognitiva;
-Ouvir a saudacão da URA Cognitiva conforme descrito na DF.
-A URA Congnitiva informa que entendeu que deseja falar sobre Contratação de Pacotes;
-A URA Cognitiva pede para aguardar enquanto verifica a internet;
-A URA Cognitiva informa que já existe um pacote ativo e que só é possível contratar
+    <t>1 - Chamada é encaminhada para a URA Cognitiva;
+2 - Ouvir a saudacão da URA Cognitiva conforme descrito na DF.
+3 - A URA Congnitiva informa que entendeu que deseja falar sobre Contratação de Pacotes;
+4 - A URA Cognitiva pede para aguardar enquanto verifica a internet;
+5 - A URA Cognitiva informa que já existe um pacote ativo e que só é possível contratar
 um novo depois de consumi-lo;
-A URA Cognitiva lista e oferece os pacotes disponíveis ao cliente;
-A URA Cognitiva informa que no momento estas são as únicas opções disponíveis;
-A URA Cognitiva agradece e encerra a ligação.</t>
+6 - A URA Cognitiva lista e oferece os pacotes disponíveis ao cliente;
+7 - A URA Cognitiva informa que no momento estas são as únicas opções disponíveis;
+8 - A URA Cognitiva agradece e encerra a ligação.</t>
   </si>
   <si>
     <t>191</t>
@@ -5407,13 +5407,13 @@
   <cellXfs count="5">
     <xf applyFont="1" fontId="0"/>
     <xf applyFont="1" fontId="0" applyBorder="1" borderId="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf applyFont="1" fontId="1" applyFill="1" fillId="2" applyBorder="1" borderId="2" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf applyFont="1" fontId="0" applyBorder="1" borderId="2" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf applyFont="1" fontId="0" applyBorder="1" borderId="2" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>

</xml_diff>

<commit_message>
zeroPadding no id, caso FlowMap possua scenarioPrefix
</commit_message>
<xml_diff>
--- a/maps/contratarPacoteDados/exportedScenarios/scenarios.xlsx
+++ b/maps/contratarPacoteDados/exportedScenarios/scenarios.xlsx
@@ -58,7 +58,7 @@
     <t>Status Reteste</t>
   </si>
   <si>
-    <t>1</t>
+    <t>02.001</t>
   </si>
   <si>
     <t>Contratação de Pacote de Dados</t>
@@ -85,7 +85,7 @@
 5 - A URA Cognitiva transfere para o desambiguador.</t>
   </si>
   <si>
-    <t>2</t>
+    <t>02.002</t>
   </si>
   <si>
     <t>Veio de #desambiguadorContrataçãoPacoteDados
@@ -103,7 +103,7 @@
 5 - A URA Cognitiva agradece e encerra a ligação.</t>
   </si>
   <si>
-    <t>3</t>
+    <t>02.003</t>
   </si>
   <si>
     <t>Veio de #desambiguadorContrataçãoPacoteDados
@@ -122,7 +122,7 @@
 5 - A URA Cognitiva transfere para o desambiguador.</t>
   </si>
   <si>
-    <t>4</t>
+    <t>02.004</t>
   </si>
   <si>
     <t>Veio de #desambiguadorContrataçãoPacoteDados
@@ -141,7 +141,7 @@
 5 - A URA Cognitiva agradece e encerra a ligação.</t>
   </si>
   <si>
-    <t>5</t>
+    <t>02.005</t>
   </si>
   <si>
     <t>Veio de #desambiguadorContrataçãoPacoteDados
@@ -164,7 +164,7 @@
 6 - A URA Cognitiva transfere para o desambiguador.</t>
   </si>
   <si>
-    <t>6</t>
+    <t>02.006</t>
   </si>
   <si>
     <t>Veio de #desambiguadorContrataçãoPacoteDados
@@ -187,7 +187,7 @@
 6 - A URA Cognitiva agradece e encerra a ligação.</t>
   </si>
   <si>
-    <t>7</t>
+    <t>02.007</t>
   </si>
   <si>
     <t>Veio de #desambiguadorContrataçãoPacoteDados
@@ -214,7 +214,7 @@
 7 - A URA Cognitiva transfere para o desambiguador.</t>
   </si>
   <si>
-    <t>8</t>
+    <t>02.008</t>
   </si>
   <si>
     <t>Veio de #desambiguadorContrataçãoPacoteDados
@@ -241,7 +241,7 @@
 7 - A URA Cognitiva agradece e encerra a ligação.</t>
   </si>
   <si>
-    <t>9</t>
+    <t>02.009</t>
   </si>
   <si>
     <t>Veio de #desambiguadorContrataçãoPacoteDados
@@ -273,7 +273,7 @@
 8 - A URA Cognitiva transfere para o desambiguador.</t>
   </si>
   <si>
-    <t>10</t>
+    <t>02.010</t>
   </si>
   <si>
     <t>Veio de #desambiguadorContrataçãoPacoteDados
@@ -305,7 +305,7 @@
 8 - A URA Cognitiva agradece e encerra a ligação.</t>
   </si>
   <si>
-    <t>11</t>
+    <t>02.011</t>
   </si>
   <si>
     <t>Veio de #desambiguadorContrataçãoPacoteDados
@@ -337,7 +337,7 @@
 8 - A URA Cognitiva transfere para o desambiguador.</t>
   </si>
   <si>
-    <t>12</t>
+    <t>02.012</t>
   </si>
   <si>
     <t>Veio de #desambiguadorContrataçãoPacoteDados
@@ -369,7 +369,7 @@
 8 - A URA Cognitiva agradece e encerra a ligação.</t>
   </si>
   <si>
-    <t>13</t>
+    <t>02.013</t>
   </si>
   <si>
     <t>Veio de #desambiguadorContrataçãoPacoteDados
@@ -403,7 +403,7 @@
 9 - A URA Cognitiva transfere para o desambiguador.</t>
   </si>
   <si>
-    <t>14</t>
+    <t>02.014</t>
   </si>
   <si>
     <t>Veio de #desambiguadorContrataçãoPacoteDados
@@ -437,7 +437,7 @@
 9 - A URA Cognitiva agradece e encerra a ligação.</t>
   </si>
   <si>
-    <t>15</t>
+    <t>02.015</t>
   </si>
   <si>
     <t>Veio de #desambiguadorContrataçãoPacoteDados
@@ -471,7 +471,7 @@
 9 - A URA Cognitiva transfere para o desambiguador.</t>
   </si>
   <si>
-    <t>16</t>
+    <t>02.016</t>
   </si>
   <si>
     <t>Veio de #desambiguadorContrataçãoPacoteDados
@@ -505,7 +505,7 @@
 9 - A URA Cognitiva agradece e encerra a ligação.</t>
   </si>
   <si>
-    <t>17</t>
+    <t>02.017</t>
   </si>
   <si>
     <t>Veio de #desambiguadorContrataçãoPacoteDados
@@ -538,7 +538,7 @@
 9 - A URA Cognitiva transfere para o desambiguador.</t>
   </si>
   <si>
-    <t>18</t>
+    <t>02.018</t>
   </si>
   <si>
     <t>Veio de #desambiguadorContrataçãoPacoteDados
@@ -571,7 +571,7 @@
 9 - A URA Cognitiva agradece e encerra a ligação.</t>
   </si>
   <si>
-    <t>19</t>
+    <t>02.019</t>
   </si>
   <si>
     <t>Veio de #desambiguadorContrataçãoPacoteDados
@@ -603,7 +603,7 @@
 8 - A URA Cognitiva transfere para o desambiguador.</t>
   </si>
   <si>
-    <t>20</t>
+    <t>02.020</t>
   </si>
   <si>
     <t>Veio de #desambiguadorContrataçãoPacoteDados
@@ -635,7 +635,7 @@
 8 - A URA Cognitiva agradece e encerra a ligação.</t>
   </si>
   <si>
-    <t>21</t>
+    <t>02.021</t>
   </si>
   <si>
     <t>Veio de #desambiguadorContrataçãoPacoteDados
@@ -670,7 +670,7 @@
 9 - A URA Cognitiva transfere para o desambiguador.</t>
   </si>
   <si>
-    <t>22</t>
+    <t>02.022</t>
   </si>
   <si>
     <t>Veio de #desambiguadorContrataçãoPacoteDados
@@ -705,7 +705,7 @@
 9 - A URA Cognitiva agradece e encerra a ligação.</t>
   </si>
   <si>
-    <t>23</t>
+    <t>02.023</t>
   </si>
   <si>
     <t>Veio de #desambiguadorContrataçãoPacoteDados
@@ -740,7 +740,7 @@
 9 - A URA Cognitiva transfere para o desambiguador.</t>
   </si>
   <si>
-    <t>24</t>
+    <t>02.024</t>
   </si>
   <si>
     <t>Veio de #desambiguadorContrataçãoPacoteDados
@@ -775,7 +775,7 @@
 9 - A URA Cognitiva agradece e encerra a ligação.</t>
   </si>
   <si>
-    <t>25</t>
+    <t>02.025</t>
   </si>
   <si>
     <t>Veio de #desambiguadorContrataçãoPacoteDados
@@ -812,7 +812,7 @@
 10 - A URA Cognitiva transfere para o desambiguador.</t>
   </si>
   <si>
-    <t>26</t>
+    <t>02.026</t>
   </si>
   <si>
     <t>Veio de #desambiguadorContrataçãoPacoteDados
@@ -849,7 +849,7 @@
 10 - A URA Cognitiva agradece e encerra a ligação.</t>
   </si>
   <si>
-    <t>27</t>
+    <t>02.027</t>
   </si>
   <si>
     <t>Veio de #desambiguadorContrataçãoPacoteDados
@@ -886,7 +886,7 @@
 10 - A URA Cognitiva transfere para o desambiguador.</t>
   </si>
   <si>
-    <t>28</t>
+    <t>02.028</t>
   </si>
   <si>
     <t>Veio de #desambiguadorContrataçãoPacoteDados
@@ -923,7 +923,7 @@
 10 - A URA Cognitiva agradece e encerra a ligação.</t>
   </si>
   <si>
-    <t>29</t>
+    <t>02.029</t>
   </si>
   <si>
     <t>Veio de #desambiguadorContrataçãoPacoteDados
@@ -959,7 +959,7 @@
 10 - A URA Cognitiva transfere para o desambiguador.</t>
   </si>
   <si>
-    <t>30</t>
+    <t>02.030</t>
   </si>
   <si>
     <t>Veio de #desambiguadorContrataçãoPacoteDados
@@ -995,7 +995,7 @@
 10 - A URA Cognitiva agradece e encerra a ligação.</t>
   </si>
   <si>
-    <t>31</t>
+    <t>02.031</t>
   </si>
   <si>
     <t>Veio de #desambiguadorContrataçãoPacoteDados
@@ -1030,7 +1030,7 @@
 9 - A URA Cognitiva transfere para o desambiguador.</t>
   </si>
   <si>
-    <t>32</t>
+    <t>02.032</t>
   </si>
   <si>
     <t>Veio de #desambiguadorContrataçãoPacoteDados
@@ -1065,7 +1065,7 @@
 9 - A URA Cognitiva agradece e encerra a ligação.</t>
   </si>
   <si>
-    <t>33</t>
+    <t>02.033</t>
   </si>
   <si>
     <t>Veio de #desambiguadorContrataçãoPacoteDados
@@ -1096,7 +1096,7 @@
 8 - A URA Cognitiva transfere para o desambiguador.</t>
   </si>
   <si>
-    <t>34</t>
+    <t>02.034</t>
   </si>
   <si>
     <t>Veio de #desambiguadorContrataçãoPacoteDados
@@ -1127,7 +1127,7 @@
 8 - A URA Cognitiva agradece e encerra a ligação.</t>
   </si>
   <si>
-    <t>35</t>
+    <t>02.035</t>
   </si>
   <si>
     <t>Veio de #desambiguadorContrataçãoPacoteDados
@@ -1147,7 +1147,7 @@
 Quer algo mais.</t>
   </si>
   <si>
-    <t>36</t>
+    <t>02.036</t>
   </si>
   <si>
     <t>Veio de #desambiguadorContrataçãoPacoteDados
@@ -1167,7 +1167,7 @@
 Não quer mais nada.</t>
   </si>
   <si>
-    <t>37</t>
+    <t>02.037</t>
   </si>
   <si>
     <t>Veio de #desambiguadorContrataçãoPacoteDados
@@ -1192,7 +1192,7 @@
 6 - A URA Cognitiva transfere para o desambiguador.</t>
   </si>
   <si>
-    <t>38</t>
+    <t>02.038</t>
   </si>
   <si>
     <t>Veio de #desambiguadorContrataçãoPacoteDados
@@ -1217,7 +1217,7 @@
 6 - A URA Cognitiva agradece e encerra a ligação.</t>
   </si>
   <si>
-    <t>39</t>
+    <t>02.039</t>
   </si>
   <si>
     <t>Veio de #desambiguadorContrataçãoPacoteDados
@@ -1247,7 +1247,7 @@
 7 - A URA Cognitiva transfere para o desambiguador.</t>
   </si>
   <si>
-    <t>40</t>
+    <t>02.040</t>
   </si>
   <si>
     <t>Veio de #desambiguadorContrataçãoPacoteDados
@@ -1277,7 +1277,7 @@
 7 - A URA Cognitiva agradece e encerra a ligação.</t>
   </si>
   <si>
-    <t>41</t>
+    <t>02.041</t>
   </si>
   <si>
     <t>Veio de #desambiguadorContrataçãoPacoteDados
@@ -1307,7 +1307,7 @@
 7 - A URA Cognitiva transfere para o desambiguador.</t>
   </si>
   <si>
-    <t>42</t>
+    <t>02.042</t>
   </si>
   <si>
     <t>Veio de #desambiguadorContrataçãoPacoteDados
@@ -1337,7 +1337,7 @@
 7 - A URA Cognitiva agradece e encerra a ligação.</t>
   </si>
   <si>
-    <t>43</t>
+    <t>02.043</t>
   </si>
   <si>
     <t>Veio de #desambiguadorContrataçãoPacoteDados
@@ -1369,7 +1369,7 @@
 8 - A URA Cognitiva transfere para o desambiguador.</t>
   </si>
   <si>
-    <t>44</t>
+    <t>02.044</t>
   </si>
   <si>
     <t>Veio de #desambiguadorContrataçãoPacoteDados
@@ -1401,7 +1401,7 @@
 8 - A URA Cognitiva agradece e encerra a ligação.</t>
   </si>
   <si>
-    <t>45</t>
+    <t>02.045</t>
   </si>
   <si>
     <t>Veio de #desambiguadorContrataçãoPacoteDados
@@ -1433,7 +1433,7 @@
 8 - A URA Cognitiva transfere para o desambiguador.</t>
   </si>
   <si>
-    <t>46</t>
+    <t>02.046</t>
   </si>
   <si>
     <t>Veio de #desambiguadorContrataçãoPacoteDados
@@ -1465,7 +1465,7 @@
 8 - A URA Cognitiva agradece e encerra a ligação.</t>
   </si>
   <si>
-    <t>47</t>
+    <t>02.047</t>
   </si>
   <si>
     <t>Veio de #desambiguadorContrataçãoPacoteDados
@@ -1496,7 +1496,7 @@
 8 - A URA Cognitiva transfere para o desambiguador.</t>
   </si>
   <si>
-    <t>48</t>
+    <t>02.048</t>
   </si>
   <si>
     <t>Veio de #desambiguadorContrataçãoPacoteDados
@@ -1527,7 +1527,7 @@
 8 - A URA Cognitiva agradece e encerra a ligação.</t>
   </si>
   <si>
-    <t>49</t>
+    <t>02.049</t>
   </si>
   <si>
     <t>Veio de #desambiguadorContrataçãoPacoteDados
@@ -1557,7 +1557,7 @@
 7 - A URA Cognitiva transfere para o desambiguador.</t>
   </si>
   <si>
-    <t>50</t>
+    <t>02.050</t>
   </si>
   <si>
     <t>Veio de #desambiguadorContrataçãoPacoteDados
@@ -1587,7 +1587,7 @@
 7 - A URA Cognitiva agradece e encerra a ligação.</t>
   </si>
   <si>
-    <t>51</t>
+    <t>02.051</t>
   </si>
   <si>
     <t>Veio de #desambiguadorContrataçãoPacoteDados
@@ -1620,7 +1620,7 @@
 8 - A URA Cognitiva transfere para o desambiguador.</t>
   </si>
   <si>
-    <t>52</t>
+    <t>02.052</t>
   </si>
   <si>
     <t>Veio de #desambiguadorContrataçãoPacoteDados
@@ -1653,7 +1653,7 @@
 8 - A URA Cognitiva agradece e encerra a ligação.</t>
   </si>
   <si>
-    <t>53</t>
+    <t>02.053</t>
   </si>
   <si>
     <t>Veio de #desambiguadorContrataçãoPacoteDados
@@ -1686,7 +1686,7 @@
 8 - A URA Cognitiva transfere para o desambiguador.</t>
   </si>
   <si>
-    <t>54</t>
+    <t>02.054</t>
   </si>
   <si>
     <t>Veio de #desambiguadorContrataçãoPacoteDados
@@ -1719,7 +1719,7 @@
 8 - A URA Cognitiva agradece e encerra a ligação.</t>
   </si>
   <si>
-    <t>55</t>
+    <t>02.055</t>
   </si>
   <si>
     <t>Veio de #desambiguadorContrataçãoPacoteDados
@@ -1754,7 +1754,7 @@
 9 - A URA Cognitiva transfere para o desambiguador.</t>
   </si>
   <si>
-    <t>56</t>
+    <t>02.056</t>
   </si>
   <si>
     <t>Veio de #desambiguadorContrataçãoPacoteDados
@@ -1789,7 +1789,7 @@
 9 - A URA Cognitiva agradece e encerra a ligação.</t>
   </si>
   <si>
-    <t>57</t>
+    <t>02.057</t>
   </si>
   <si>
     <t>Veio de #desambiguadorContrataçãoPacoteDados
@@ -1824,7 +1824,7 @@
 9 - A URA Cognitiva transfere para o desambiguador.</t>
   </si>
   <si>
-    <t>58</t>
+    <t>02.058</t>
   </si>
   <si>
     <t>Veio de #desambiguadorContrataçãoPacoteDados
@@ -1859,7 +1859,7 @@
 9 - A URA Cognitiva agradece e encerra a ligação.</t>
   </si>
   <si>
-    <t>59</t>
+    <t>02.059</t>
   </si>
   <si>
     <t>Veio de #desambiguadorContrataçãoPacoteDados
@@ -1893,7 +1893,7 @@
 9 - A URA Cognitiva transfere para o desambiguador.</t>
   </si>
   <si>
-    <t>60</t>
+    <t>02.060</t>
   </si>
   <si>
     <t>Veio de #desambiguadorContrataçãoPacoteDados
@@ -1927,7 +1927,7 @@
 9 - A URA Cognitiva agradece e encerra a ligação.</t>
   </si>
   <si>
-    <t>61</t>
+    <t>02.061</t>
   </si>
   <si>
     <t>Veio de #desambiguadorContrataçãoPacoteDados
@@ -1960,7 +1960,7 @@
 8 - A URA Cognitiva transfere para o desambiguador.</t>
   </si>
   <si>
-    <t>62</t>
+    <t>02.062</t>
   </si>
   <si>
     <t>Veio de #desambiguadorContrataçãoPacoteDados
@@ -1993,7 +1993,7 @@
 8 - A URA Cognitiva agradece e encerra a ligação.</t>
   </si>
   <si>
-    <t>63</t>
+    <t>02.063</t>
   </si>
   <si>
     <t>Veio de #desambiguadorContrataçãoPacoteDados
@@ -2022,7 +2022,7 @@
 7 - A URA Cognitiva transfere para o desambiguador.</t>
   </si>
   <si>
-    <t>64</t>
+    <t>02.064</t>
   </si>
   <si>
     <t>Veio de #desambiguadorContrataçãoPacoteDados
@@ -2051,7 +2051,7 @@
 7 - A URA Cognitiva agradece e encerra a ligação.</t>
   </si>
   <si>
-    <t>65</t>
+    <t>02.065</t>
   </si>
   <si>
     <t>Veio de #desambiguadorContrataçãoPacoteDados
@@ -2071,7 +2071,7 @@
 Quer algo mais.</t>
   </si>
   <si>
-    <t>66</t>
+    <t>02.066</t>
   </si>
   <si>
     <t>Veio de #desambiguadorContrataçãoPacoteDados
@@ -2091,7 +2091,7 @@
 Não quer mais nada.</t>
   </si>
   <si>
-    <t>67</t>
+    <t>02.067</t>
   </si>
   <si>
     <t>Veio de #desambiguadorContrataçãoPacoteDados
@@ -2115,7 +2115,7 @@
 6 - A URA Cognitiva transfere para o desambiguador.</t>
   </si>
   <si>
-    <t>68</t>
+    <t>02.068</t>
   </si>
   <si>
     <t>Veio de #desambiguadorContrataçãoPacoteDados
@@ -2139,7 +2139,7 @@
 6 - A URA Cognitiva agradece e encerra a ligação.</t>
   </si>
   <si>
-    <t>69</t>
+    <t>02.069</t>
   </si>
   <si>
     <t>Veio de #desambiguadorContrataçãoPacoteDados
@@ -2153,7 +2153,7 @@
 Quer algo mais.</t>
   </si>
   <si>
-    <t>70</t>
+    <t>02.070</t>
   </si>
   <si>
     <t>Veio de #desambiguadorContrataçãoPacoteDados
@@ -2167,7 +2167,7 @@
 Não quer mais nada.</t>
   </si>
   <si>
-    <t>71</t>
+    <t>02.071</t>
   </si>
   <si>
     <t>Veio de #desambiguadorContrataçãoPacoteDados
@@ -2184,7 +2184,7 @@
 Quer algo mais.</t>
   </si>
   <si>
-    <t>72</t>
+    <t>02.072</t>
   </si>
   <si>
     <t>Veio de #desambiguadorContrataçãoPacoteDados
@@ -2201,7 +2201,7 @@
 Não quer mais nada.</t>
   </si>
   <si>
-    <t>73</t>
+    <t>02.073</t>
   </si>
   <si>
     <t>Veio de #desambiguadorContrataçãoPacoteDados
@@ -2222,7 +2222,7 @@
 Quer algo mais.</t>
   </si>
   <si>
-    <t>74</t>
+    <t>02.074</t>
   </si>
   <si>
     <t>Veio de #desambiguadorContrataçãoPacoteDados
@@ -2243,7 +2243,7 @@
 Não quer mais nada.</t>
   </si>
   <si>
-    <t>75</t>
+    <t>02.075</t>
   </si>
   <si>
     <t>Veio de #desambiguadorContrataçãoPacoteDados
@@ -2264,7 +2264,7 @@
 Quer algo mais.</t>
   </si>
   <si>
-    <t>76</t>
+    <t>02.076</t>
   </si>
   <si>
     <t>Veio de #desambiguadorContrataçãoPacoteDados
@@ -2285,7 +2285,7 @@
 Não quer mais nada.</t>
   </si>
   <si>
-    <t>77</t>
+    <t>02.077</t>
   </si>
   <si>
     <t>Veio de #desambiguadorContrataçãoPacoteDados
@@ -2307,7 +2307,7 @@
 Quer algo mais.</t>
   </si>
   <si>
-    <t>78</t>
+    <t>02.078</t>
   </si>
   <si>
     <t>Veio de #desambiguadorContrataçãoPacoteDados
@@ -2329,7 +2329,7 @@
 Não quer mais nada.</t>
   </si>
   <si>
-    <t>79</t>
+    <t>02.079</t>
   </si>
   <si>
     <t>Veio de #desambiguadorContrataçãoPacoteDados
@@ -2351,7 +2351,7 @@
 Quer algo mais.</t>
   </si>
   <si>
-    <t>80</t>
+    <t>02.080</t>
   </si>
   <si>
     <t>Veio de #desambiguadorContrataçãoPacoteDados
@@ -2373,7 +2373,7 @@
 Não quer mais nada.</t>
   </si>
   <si>
-    <t>81</t>
+    <t>02.081</t>
   </si>
   <si>
     <t>Veio de #desambiguadorContrataçãoPacoteDados
@@ -2394,7 +2394,7 @@
 Quer algo mais.</t>
   </si>
   <si>
-    <t>82</t>
+    <t>02.082</t>
   </si>
   <si>
     <t>Veio de #desambiguadorContrataçãoPacoteDados
@@ -2415,7 +2415,7 @@
 Não quer mais nada.</t>
   </si>
   <si>
-    <t>83</t>
+    <t>02.083</t>
   </si>
   <si>
     <t>Veio de #desambiguadorContrataçãoPacoteDados
@@ -2436,7 +2436,7 @@
 Quer algo mais.</t>
   </si>
   <si>
-    <t>84</t>
+    <t>02.084</t>
   </si>
   <si>
     <t>Veio de #desambiguadorContrataçãoPacoteDados
@@ -2457,7 +2457,7 @@
 Não quer mais nada.</t>
   </si>
   <si>
-    <t>85</t>
+    <t>02.085</t>
   </si>
   <si>
     <t>Veio de #desambiguadorContrataçãoPacoteDados
@@ -2480,7 +2480,7 @@
 Quer algo mais.</t>
   </si>
   <si>
-    <t>86</t>
+    <t>02.086</t>
   </si>
   <si>
     <t>Veio de #desambiguadorContrataçãoPacoteDados
@@ -2503,7 +2503,7 @@
 Não quer mais nada.</t>
   </si>
   <si>
-    <t>87</t>
+    <t>02.087</t>
   </si>
   <si>
     <t>Veio de #desambiguadorContrataçãoPacoteDados
@@ -2526,7 +2526,7 @@
 Quer algo mais.</t>
   </si>
   <si>
-    <t>88</t>
+    <t>02.088</t>
   </si>
   <si>
     <t>Veio de #desambiguadorContrataçãoPacoteDados
@@ -2549,7 +2549,7 @@
 Não quer mais nada.</t>
   </si>
   <si>
-    <t>89</t>
+    <t>02.089</t>
   </si>
   <si>
     <t>Veio de #desambiguadorContrataçãoPacoteDados
@@ -2573,7 +2573,7 @@
 Quer algo mais.</t>
   </si>
   <si>
-    <t>90</t>
+    <t>02.090</t>
   </si>
   <si>
     <t>Veio de #desambiguadorContrataçãoPacoteDados
@@ -2597,7 +2597,7 @@
 Não quer mais nada.</t>
   </si>
   <si>
-    <t>91</t>
+    <t>02.091</t>
   </si>
   <si>
     <t>Veio de #desambiguadorContrataçãoPacoteDados
@@ -2621,7 +2621,7 @@
 Quer algo mais.</t>
   </si>
   <si>
-    <t>92</t>
+    <t>02.092</t>
   </si>
   <si>
     <t>Veio de #desambiguadorContrataçãoPacoteDados
@@ -2645,7 +2645,7 @@
 Não quer mais nada.</t>
   </si>
   <si>
-    <t>93</t>
+    <t>02.093</t>
   </si>
   <si>
     <t>Veio de #desambiguadorContrataçãoPacoteDados
@@ -2668,7 +2668,7 @@
 Quer algo mais.</t>
   </si>
   <si>
-    <t>94</t>
+    <t>02.094</t>
   </si>
   <si>
     <t>Veio de #desambiguadorContrataçãoPacoteDados
@@ -2691,7 +2691,7 @@
 Não quer mais nada.</t>
   </si>
   <si>
-    <t>95</t>
+    <t>02.095</t>
   </si>
   <si>
     <t>Veio de #desambiguadorContrataçãoPacoteDados
@@ -2714,7 +2714,7 @@
 Quer algo mais.</t>
   </si>
   <si>
-    <t>96</t>
+    <t>02.096</t>
   </si>
   <si>
     <t>Veio de #desambiguadorContrataçãoPacoteDados
@@ -2737,7 +2737,7 @@
 Não quer mais nada.</t>
   </si>
   <si>
-    <t>97</t>
+    <t>02.097</t>
   </si>
   <si>
     <t>Veio de #desambiguadorContrataçãoPacoteDados
@@ -2757,7 +2757,7 @@
 Quer algo mais.</t>
   </si>
   <si>
-    <t>98</t>
+    <t>02.098</t>
   </si>
   <si>
     <t>Veio de #desambiguadorContrataçãoPacoteDados
@@ -2777,7 +2777,7 @@
 Não quer mais nada.</t>
   </si>
   <si>
-    <t>99</t>
+    <t>02.099</t>
   </si>
   <si>
     <t>Veio de #desambiguadorContrataçãoPacoteDados
@@ -2797,7 +2797,7 @@
 Quer algo mais.</t>
   </si>
   <si>
-    <t>100</t>
+    <t>02.100</t>
   </si>
   <si>
     <t>Veio de #desambiguadorContrataçãoPacoteDados
@@ -2817,7 +2817,7 @@
 Não quer mais nada.</t>
   </si>
   <si>
-    <t>101</t>
+    <t>02.101</t>
   </si>
   <si>
     <t>Veio de #desambiguadorContrataçãoPacoteDados
@@ -2834,7 +2834,7 @@
 Quer algo mais.</t>
   </si>
   <si>
-    <t>102</t>
+    <t>02.102</t>
   </si>
   <si>
     <t>Veio de #desambiguadorContrataçãoPacoteDados
@@ -2851,7 +2851,7 @@
 Não quer mais nada.</t>
   </si>
   <si>
-    <t>103</t>
+    <t>02.103</t>
   </si>
   <si>
     <t>Veio de #desambiguadorContrataçãoPacoteDados
@@ -2872,7 +2872,7 @@
 Quer algo mais.</t>
   </si>
   <si>
-    <t>104</t>
+    <t>02.104</t>
   </si>
   <si>
     <t>Veio de #desambiguadorContrataçãoPacoteDados
@@ -2893,7 +2893,7 @@
 Não quer mais nada.</t>
   </si>
   <si>
-    <t>105</t>
+    <t>02.105</t>
   </si>
   <si>
     <t>Veio de #desambiguadorContrataçãoPacoteDados
@@ -2914,7 +2914,7 @@
 Quer algo mais.</t>
   </si>
   <si>
-    <t>106</t>
+    <t>02.106</t>
   </si>
   <si>
     <t>Veio de #desambiguadorContrataçãoPacoteDados
@@ -2935,7 +2935,7 @@
 Não quer mais nada.</t>
   </si>
   <si>
-    <t>107</t>
+    <t>02.107</t>
   </si>
   <si>
     <t>Veio de #desambiguadorContrataçãoPacoteDados
@@ -2957,7 +2957,7 @@
 Quer algo mais.</t>
   </si>
   <si>
-    <t>108</t>
+    <t>02.108</t>
   </si>
   <si>
     <t>Veio de #desambiguadorContrataçãoPacoteDados
@@ -2979,7 +2979,7 @@
 Não quer mais nada.</t>
   </si>
   <si>
-    <t>109</t>
+    <t>02.109</t>
   </si>
   <si>
     <t>Veio de #desambiguadorContrataçãoPacoteDados
@@ -3001,7 +3001,7 @@
 Quer algo mais.</t>
   </si>
   <si>
-    <t>110</t>
+    <t>02.110</t>
   </si>
   <si>
     <t>Veio de #desambiguadorContrataçãoPacoteDados
@@ -3023,7 +3023,7 @@
 Não quer mais nada.</t>
   </si>
   <si>
-    <t>111</t>
+    <t>02.111</t>
   </si>
   <si>
     <t>Veio de #desambiguadorContrataçãoPacoteDados
@@ -3044,7 +3044,7 @@
 Quer algo mais.</t>
   </si>
   <si>
-    <t>112</t>
+    <t>02.112</t>
   </si>
   <si>
     <t>Veio de #desambiguadorContrataçãoPacoteDados
@@ -3065,7 +3065,7 @@
 Não quer mais nada.</t>
   </si>
   <si>
-    <t>113</t>
+    <t>02.113</t>
   </si>
   <si>
     <t>Veio de #desambiguadorContrataçãoPacoteDados
@@ -3086,7 +3086,7 @@
 Quer algo mais.</t>
   </si>
   <si>
-    <t>114</t>
+    <t>02.114</t>
   </si>
   <si>
     <t>Veio de #desambiguadorContrataçãoPacoteDados
@@ -3107,7 +3107,7 @@
 Não quer mais nada.</t>
   </si>
   <si>
-    <t>115</t>
+    <t>02.115</t>
   </si>
   <si>
     <t>Veio de #desambiguadorContrataçãoPacoteDados
@@ -3130,7 +3130,7 @@
 Quer algo mais.</t>
   </si>
   <si>
-    <t>116</t>
+    <t>02.116</t>
   </si>
   <si>
     <t>Veio de #desambiguadorContrataçãoPacoteDados
@@ -3153,7 +3153,7 @@
 Não quer mais nada.</t>
   </si>
   <si>
-    <t>117</t>
+    <t>02.117</t>
   </si>
   <si>
     <t>Veio de #desambiguadorContrataçãoPacoteDados
@@ -3176,7 +3176,7 @@
 Quer algo mais.</t>
   </si>
   <si>
-    <t>118</t>
+    <t>02.118</t>
   </si>
   <si>
     <t>Veio de #desambiguadorContrataçãoPacoteDados
@@ -3199,7 +3199,7 @@
 Não quer mais nada.</t>
   </si>
   <si>
-    <t>119</t>
+    <t>02.119</t>
   </si>
   <si>
     <t>Veio de #desambiguadorContrataçãoPacoteDados
@@ -3223,7 +3223,7 @@
 Quer algo mais.</t>
   </si>
   <si>
-    <t>120</t>
+    <t>02.120</t>
   </si>
   <si>
     <t>Veio de #desambiguadorContrataçãoPacoteDados
@@ -3247,7 +3247,7 @@
 Não quer mais nada.</t>
   </si>
   <si>
-    <t>121</t>
+    <t>02.121</t>
   </si>
   <si>
     <t>Veio de #desambiguadorContrataçãoPacoteDados
@@ -3271,7 +3271,7 @@
 Quer algo mais.</t>
   </si>
   <si>
-    <t>122</t>
+    <t>02.122</t>
   </si>
   <si>
     <t>Veio de #desambiguadorContrataçãoPacoteDados
@@ -3295,7 +3295,7 @@
 Não quer mais nada.</t>
   </si>
   <si>
-    <t>123</t>
+    <t>02.123</t>
   </si>
   <si>
     <t>Veio de #desambiguadorContrataçãoPacoteDados
@@ -3318,7 +3318,7 @@
 Quer algo mais.</t>
   </si>
   <si>
-    <t>124</t>
+    <t>02.124</t>
   </si>
   <si>
     <t>Veio de #desambiguadorContrataçãoPacoteDados
@@ -3341,7 +3341,7 @@
 Não quer mais nada.</t>
   </si>
   <si>
-    <t>125</t>
+    <t>02.125</t>
   </si>
   <si>
     <t>Veio de #desambiguadorContrataçãoPacoteDados
@@ -3364,7 +3364,7 @@
 Quer algo mais.</t>
   </si>
   <si>
-    <t>126</t>
+    <t>02.126</t>
   </si>
   <si>
     <t>Veio de #desambiguadorContrataçãoPacoteDados
@@ -3387,7 +3387,7 @@
 Não quer mais nada.</t>
   </si>
   <si>
-    <t>127</t>
+    <t>02.127</t>
   </si>
   <si>
     <t>Veio de #desambiguadorContrataçãoPacoteDados
@@ -3407,7 +3407,7 @@
 Quer algo mais.</t>
   </si>
   <si>
-    <t>128</t>
+    <t>02.128</t>
   </si>
   <si>
     <t>Veio de #desambiguadorContrataçãoPacoteDados
@@ -3427,7 +3427,7 @@
 Não quer mais nada.</t>
   </si>
   <si>
-    <t>129</t>
+    <t>02.129</t>
   </si>
   <si>
     <t>Veio de #desambiguadorContrataçãoPacoteDados
@@ -3447,7 +3447,7 @@
 Quer algo mais.</t>
   </si>
   <si>
-    <t>130</t>
+    <t>02.130</t>
   </si>
   <si>
     <t>Veio de #desambiguadorContrataçãoPacoteDados
@@ -3467,7 +3467,7 @@
 Não quer mais nada.</t>
   </si>
   <si>
-    <t>131</t>
+    <t>02.131</t>
   </si>
   <si>
     <t>Veio de #desambiguadorContrataçãoPacoteDados
@@ -3482,7 +3482,7 @@
 Quer algo mais.</t>
   </si>
   <si>
-    <t>132</t>
+    <t>02.132</t>
   </si>
   <si>
     <t>Veio de #desambiguadorContrataçãoPacoteDados
@@ -3497,7 +3497,7 @@
 Não quer mais nada.</t>
   </si>
   <si>
-    <t>133</t>
+    <t>02.133</t>
   </si>
   <si>
     <t>Veio de #desambiguadorContrataçãoPacoteDados
@@ -3523,7 +3523,7 @@
 8 - A URA Cognitiva transfere para o desambiguador.</t>
   </si>
   <si>
-    <t>134</t>
+    <t>02.134</t>
   </si>
   <si>
     <t>Veio de #desambiguadorContrataçãoPacoteDados
@@ -3549,7 +3549,7 @@
 8 - A URA Cognitiva agradece e encerra a ligação.</t>
   </si>
   <si>
-    <t>135</t>
+    <t>02.135</t>
   </si>
   <si>
     <t>Veio de #desambiguadorContrataçãoPacoteDados
@@ -3580,7 +3580,7 @@
 9 - A URA Cognitiva transfere para o desambiguador.</t>
   </si>
   <si>
-    <t>136</t>
+    <t>02.136</t>
   </si>
   <si>
     <t>Veio de #desambiguadorContrataçãoPacoteDados
@@ -3611,7 +3611,7 @@
 9 - A URA Cognitiva agradece e encerra a ligação.</t>
   </si>
   <si>
-    <t>137</t>
+    <t>02.137</t>
   </si>
   <si>
     <t>Veio de #desambiguadorContrataçãoPacoteDados
@@ -3642,7 +3642,7 @@
 9 - A URA Cognitiva transfere para o desambiguador.</t>
   </si>
   <si>
-    <t>138</t>
+    <t>02.138</t>
   </si>
   <si>
     <t>Veio de #desambiguadorContrataçãoPacoteDados
@@ -3673,7 +3673,7 @@
 9 - A URA Cognitiva agradece e encerra a ligação.</t>
   </si>
   <si>
-    <t>139</t>
+    <t>02.139</t>
   </si>
   <si>
     <t>Veio de #desambiguadorContrataçãoPacoteDados
@@ -3706,7 +3706,7 @@
 10 - A URA Cognitiva transfere para o desambiguador.</t>
   </si>
   <si>
-    <t>140</t>
+    <t>02.140</t>
   </si>
   <si>
     <t>Veio de #desambiguadorContrataçãoPacoteDados
@@ -3739,7 +3739,7 @@
 10 - A URA Cognitiva agradece e encerra a ligação.</t>
   </si>
   <si>
-    <t>141</t>
+    <t>02.141</t>
   </si>
   <si>
     <t>Veio de #desambiguadorContrataçãoPacoteDados
@@ -3772,7 +3772,7 @@
 10 - A URA Cognitiva transfere para o desambiguador.</t>
   </si>
   <si>
-    <t>142</t>
+    <t>02.142</t>
   </si>
   <si>
     <t>Veio de #desambiguadorContrataçãoPacoteDados
@@ -3805,7 +3805,7 @@
 10 - A URA Cognitiva agradece e encerra a ligação.</t>
   </si>
   <si>
-    <t>143</t>
+    <t>02.143</t>
   </si>
   <si>
     <t>Veio de #desambiguadorContrataçãoPacoteDados
@@ -3837,7 +3837,7 @@
 10 - A URA Cognitiva transfere para o desambiguador.</t>
   </si>
   <si>
-    <t>144</t>
+    <t>02.144</t>
   </si>
   <si>
     <t>Veio de #desambiguadorContrataçãoPacoteDados
@@ -3869,7 +3869,7 @@
 10 - A URA Cognitiva agradece e encerra a ligação.</t>
   </si>
   <si>
-    <t>145</t>
+    <t>02.145</t>
   </si>
   <si>
     <t>Veio de #desambiguadorContrataçãoPacoteDados
@@ -3900,7 +3900,7 @@
 9 - A URA Cognitiva transfere para o desambiguador.</t>
   </si>
   <si>
-    <t>146</t>
+    <t>02.146</t>
   </si>
   <si>
     <t>Veio de #desambiguadorContrataçãoPacoteDados
@@ -3931,7 +3931,7 @@
 9 - A URA Cognitiva agradece e encerra a ligação.</t>
   </si>
   <si>
-    <t>147</t>
+    <t>02.147</t>
   </si>
   <si>
     <t>Veio de #desambiguadorContrataçãoPacoteDados
@@ -3965,7 +3965,7 @@
 10 - A URA Cognitiva transfere para o desambiguador.</t>
   </si>
   <si>
-    <t>148</t>
+    <t>02.148</t>
   </si>
   <si>
     <t>Veio de #desambiguadorContrataçãoPacoteDados
@@ -3999,7 +3999,7 @@
 10 - A URA Cognitiva agradece e encerra a ligação.</t>
   </si>
   <si>
-    <t>149</t>
+    <t>02.149</t>
   </si>
   <si>
     <t>Veio de #desambiguadorContrataçãoPacoteDados
@@ -4033,7 +4033,7 @@
 10 - A URA Cognitiva transfere para o desambiguador.</t>
   </si>
   <si>
-    <t>150</t>
+    <t>02.150</t>
   </si>
   <si>
     <t>Veio de #desambiguadorContrataçãoPacoteDados
@@ -4067,7 +4067,7 @@
 10 - A URA Cognitiva agradece e encerra a ligação.</t>
   </si>
   <si>
-    <t>151</t>
+    <t>02.151</t>
   </si>
   <si>
     <t>Veio de #desambiguadorContrataçãoPacoteDados
@@ -4103,7 +4103,7 @@
 11 - A URA Cognitiva transfere para o desambiguador.</t>
   </si>
   <si>
-    <t>152</t>
+    <t>02.152</t>
   </si>
   <si>
     <t>Veio de #desambiguadorContrataçãoPacoteDados
@@ -4139,7 +4139,7 @@
 11 - A URA Cognitiva agradece e encerra a ligação.</t>
   </si>
   <si>
-    <t>153</t>
+    <t>02.153</t>
   </si>
   <si>
     <t>Veio de #desambiguadorContrataçãoPacoteDados
@@ -4175,7 +4175,7 @@
 11 - A URA Cognitiva transfere para o desambiguador.</t>
   </si>
   <si>
-    <t>154</t>
+    <t>02.154</t>
   </si>
   <si>
     <t>Veio de #desambiguadorContrataçãoPacoteDados
@@ -4211,7 +4211,7 @@
 11 - A URA Cognitiva agradece e encerra a ligação.</t>
   </si>
   <si>
-    <t>155</t>
+    <t>02.155</t>
   </si>
   <si>
     <t>Veio de #desambiguadorContrataçãoPacoteDados
@@ -4246,7 +4246,7 @@
 11 - A URA Cognitiva transfere para o desambiguador.</t>
   </si>
   <si>
-    <t>156</t>
+    <t>02.156</t>
   </si>
   <si>
     <t>Veio de #desambiguadorContrataçãoPacoteDados
@@ -4281,7 +4281,7 @@
 11 - A URA Cognitiva agradece e encerra a ligação.</t>
   </si>
   <si>
-    <t>157</t>
+    <t>02.157</t>
   </si>
   <si>
     <t>Veio de #desambiguadorContrataçãoPacoteDados
@@ -4315,7 +4315,7 @@
 10 - A URA Cognitiva transfere para o desambiguador.</t>
   </si>
   <si>
-    <t>158</t>
+    <t>02.158</t>
   </si>
   <si>
     <t>Veio de #desambiguadorContrataçãoPacoteDados
@@ -4349,7 +4349,7 @@
 10 - A URA Cognitiva agradece e encerra a ligação.</t>
   </si>
   <si>
-    <t>159</t>
+    <t>02.159</t>
   </si>
   <si>
     <t>Veio de #desambiguadorContrataçãoPacoteDados
@@ -4379,7 +4379,7 @@
 9 - A URA Cognitiva transfere para o desambiguador.</t>
   </si>
   <si>
-    <t>160</t>
+    <t>02.160</t>
   </si>
   <si>
     <t>Veio de #desambiguadorContrataçãoPacoteDados
@@ -4409,7 +4409,7 @@
 9 - A URA Cognitiva agradece e encerra a ligação.</t>
   </si>
   <si>
-    <t>161</t>
+    <t>02.161</t>
   </si>
   <si>
     <t>Veio de #desambiguadorContrataçãoPacoteDados
@@ -4426,7 +4426,7 @@
 Quer algo mais.</t>
   </si>
   <si>
-    <t>162</t>
+    <t>02.162</t>
   </si>
   <si>
     <t>Veio de #desambiguadorContrataçãoPacoteDados
@@ -4443,7 +4443,7 @@
 Não quer mais nada.</t>
   </si>
   <si>
-    <t>163</t>
+    <t>02.163</t>
   </si>
   <si>
     <t>Veio de #desambiguadorContrataçãoPacoteDados
@@ -4467,7 +4467,7 @@
 7 - A URA Cognitiva transfere para o desambiguador.</t>
   </si>
   <si>
-    <t>164</t>
+    <t>02.164</t>
   </si>
   <si>
     <t>Veio de #desambiguadorContrataçãoPacoteDados
@@ -4491,7 +4491,7 @@
 7 - A URA Cognitiva agradece e encerra a ligação.</t>
   </si>
   <si>
-    <t>165</t>
+    <t>02.165</t>
   </si>
   <si>
     <t>Veio de #desambiguadorContrataçãoPacoteDados
@@ -4520,7 +4520,7 @@
 8 - A URA Cognitiva transfere para o desambiguador.</t>
   </si>
   <si>
-    <t>166</t>
+    <t>02.166</t>
   </si>
   <si>
     <t>Veio de #desambiguadorContrataçãoPacoteDados
@@ -4549,7 +4549,7 @@
 8 - A URA Cognitiva agradece e encerra a ligação.</t>
   </si>
   <si>
-    <t>167</t>
+    <t>02.167</t>
   </si>
   <si>
     <t>Veio de #desambiguadorContrataçãoPacoteDados
@@ -4578,7 +4578,7 @@
 8 - A URA Cognitiva transfere para o desambiguador.</t>
   </si>
   <si>
-    <t>168</t>
+    <t>02.168</t>
   </si>
   <si>
     <t>Veio de #desambiguadorContrataçãoPacoteDados
@@ -4607,7 +4607,7 @@
 8 - A URA Cognitiva agradece e encerra a ligação.</t>
   </si>
   <si>
-    <t>169</t>
+    <t>02.169</t>
   </si>
   <si>
     <t>Veio de #desambiguadorContrataçãoPacoteDados
@@ -4638,7 +4638,7 @@
 9 - A URA Cognitiva transfere para o desambiguador.</t>
   </si>
   <si>
-    <t>170</t>
+    <t>02.170</t>
   </si>
   <si>
     <t>Veio de #desambiguadorContrataçãoPacoteDados
@@ -4669,7 +4669,7 @@
 9 - A URA Cognitiva agradece e encerra a ligação.</t>
   </si>
   <si>
-    <t>171</t>
+    <t>02.171</t>
   </si>
   <si>
     <t>Veio de #desambiguadorContrataçãoPacoteDados
@@ -4700,7 +4700,7 @@
 9 - A URA Cognitiva transfere para o desambiguador.</t>
   </si>
   <si>
-    <t>172</t>
+    <t>02.172</t>
   </si>
   <si>
     <t>Veio de #desambiguadorContrataçãoPacoteDados
@@ -4731,7 +4731,7 @@
 9 - A URA Cognitiva agradece e encerra a ligação.</t>
   </si>
   <si>
-    <t>173</t>
+    <t>02.173</t>
   </si>
   <si>
     <t>Veio de #desambiguadorContrataçãoPacoteDados
@@ -4761,7 +4761,7 @@
 9 - A URA Cognitiva transfere para o desambiguador.</t>
   </si>
   <si>
-    <t>174</t>
+    <t>02.174</t>
   </si>
   <si>
     <t>Veio de #desambiguadorContrataçãoPacoteDados
@@ -4791,7 +4791,7 @@
 9 - A URA Cognitiva agradece e encerra a ligação.</t>
   </si>
   <si>
-    <t>175</t>
+    <t>02.175</t>
   </si>
   <si>
     <t>Veio de #desambiguadorContrataçãoPacoteDados
@@ -4820,7 +4820,7 @@
 8 - A URA Cognitiva transfere para o desambiguador.</t>
   </si>
   <si>
-    <t>176</t>
+    <t>02.176</t>
   </si>
   <si>
     <t>Veio de #desambiguadorContrataçãoPacoteDados
@@ -4849,7 +4849,7 @@
 8 - A URA Cognitiva agradece e encerra a ligação.</t>
   </si>
   <si>
-    <t>177</t>
+    <t>02.177</t>
   </si>
   <si>
     <t>Veio de #desambiguadorContrataçãoPacoteDados
@@ -4881,7 +4881,7 @@
 9 - A URA Cognitiva transfere para o desambiguador.</t>
   </si>
   <si>
-    <t>178</t>
+    <t>02.178</t>
   </si>
   <si>
     <t>Veio de #desambiguadorContrataçãoPacoteDados
@@ -4913,7 +4913,7 @@
 9 - A URA Cognitiva agradece e encerra a ligação.</t>
   </si>
   <si>
-    <t>179</t>
+    <t>02.179</t>
   </si>
   <si>
     <t>Veio de #desambiguadorContrataçãoPacoteDados
@@ -4945,7 +4945,7 @@
 9 - A URA Cognitiva transfere para o desambiguador.</t>
   </si>
   <si>
-    <t>180</t>
+    <t>02.180</t>
   </si>
   <si>
     <t>Veio de #desambiguadorContrataçãoPacoteDados
@@ -4977,7 +4977,7 @@
 9 - A URA Cognitiva agradece e encerra a ligação.</t>
   </si>
   <si>
-    <t>181</t>
+    <t>02.181</t>
   </si>
   <si>
     <t>Veio de #desambiguadorContrataçãoPacoteDados
@@ -5011,7 +5011,7 @@
 10 - A URA Cognitiva transfere para o desambiguador.</t>
   </si>
   <si>
-    <t>182</t>
+    <t>02.182</t>
   </si>
   <si>
     <t>Veio de #desambiguadorContrataçãoPacoteDados
@@ -5045,7 +5045,7 @@
 10 - A URA Cognitiva agradece e encerra a ligação.</t>
   </si>
   <si>
-    <t>183</t>
+    <t>02.183</t>
   </si>
   <si>
     <t>Veio de #desambiguadorContrataçãoPacoteDados
@@ -5079,7 +5079,7 @@
 10 - A URA Cognitiva transfere para o desambiguador.</t>
   </si>
   <si>
-    <t>184</t>
+    <t>02.184</t>
   </si>
   <si>
     <t>Veio de #desambiguadorContrataçãoPacoteDados
@@ -5113,7 +5113,7 @@
 10 - A URA Cognitiva agradece e encerra a ligação.</t>
   </si>
   <si>
-    <t>185</t>
+    <t>02.185</t>
   </si>
   <si>
     <t>Veio de #desambiguadorContrataçãoPacoteDados
@@ -5146,7 +5146,7 @@
 10 - A URA Cognitiva transfere para o desambiguador.</t>
   </si>
   <si>
-    <t>186</t>
+    <t>02.186</t>
   </si>
   <si>
     <t>Veio de #desambiguadorContrataçãoPacoteDados
@@ -5179,7 +5179,7 @@
 10 - A URA Cognitiva agradece e encerra a ligação.</t>
   </si>
   <si>
-    <t>187</t>
+    <t>02.187</t>
   </si>
   <si>
     <t>Veio de #desambiguadorContrataçãoPacoteDados
@@ -5211,7 +5211,7 @@
 9 - A URA Cognitiva transfere para o desambiguador.</t>
   </si>
   <si>
-    <t>188</t>
+    <t>02.188</t>
   </si>
   <si>
     <t>Veio de #desambiguadorContrataçãoPacoteDados
@@ -5243,7 +5243,7 @@
 9 - A URA Cognitiva agradece e encerra a ligação.</t>
   </si>
   <si>
-    <t>189</t>
+    <t>02.189</t>
   </si>
   <si>
     <t>Veio de #desambiguadorContrataçãoPacoteDados
@@ -5271,7 +5271,7 @@
 8 - A URA Cognitiva transfere para o desambiguador.</t>
   </si>
   <si>
-    <t>190</t>
+    <t>02.190</t>
   </si>
   <si>
     <t>Veio de #desambiguadorContrataçãoPacoteDados
@@ -5299,7 +5299,7 @@
 8 - A URA Cognitiva agradece e encerra a ligação.</t>
   </si>
   <si>
-    <t>191</t>
+    <t>02.191</t>
   </si>
   <si>
     <t>Veio de #desambiguadorContrataçãoPacoteDados
@@ -5316,7 +5316,7 @@
 Quer algo mais.</t>
   </si>
   <si>
-    <t>192</t>
+    <t>02.192</t>
   </si>
   <si>
     <t>Veio de #desambiguadorContrataçãoPacoteDados

</xml_diff>